<commit_message>
fixing div/0 issue for motorbikes
</commit_message>
<xml_diff>
--- a/InputData/trans/TTS/Transportation Technology Shareweights.xlsx
+++ b/InputData/trans/TTS/Transportation Technology Shareweights.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mary Francis Swint\Vensim\eps-eu\InputData\trans\TTS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rachel Goldstein\Dropbox (Energy Innovation)\Desktop\Vensim files from GitHub\EPS EU\InputData\trans\TTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{827F4EE3-3B24-454E-B705-B052185DC0B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B8DA58C-1CDC-499B-871C-AD50829BA5E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-37890" yWindow="-2190" windowWidth="19275" windowHeight="15570" firstSheet="7" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="12645" firstSheet="6" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -24519,8 +24519,8 @@
   </sheetPr>
   <dimension ref="A1:AE8"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="AF1" sqref="AF1:AF1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24657,125 +24657,125 @@
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="e">
+      <c r="B2">
         <f>Data!I80</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C2" t="e">
+        <v>0</v>
+      </c>
+      <c r="C2">
         <f>Data!J80</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D2" t="e">
+        <v>7.2426485361517731E-2</v>
+      </c>
+      <c r="D2">
         <f>Data!K80</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E2" t="e">
+        <v>9.534946489910949E-2</v>
+      </c>
+      <c r="E2">
         <f>Data!L80</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F2" t="e">
+        <v>0.12455335818741645</v>
+      </c>
+      <c r="F2">
         <f>Data!M80</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G2" t="e">
+        <v>0.16110894957658525</v>
+      </c>
+      <c r="G2">
         <f>Data!N80</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H2" t="e">
+        <v>0.20587037180094736</v>
+      </c>
+      <c r="H2">
         <f>Data!O80</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I2" t="e">
+        <v>0.259225100817846</v>
+      </c>
+      <c r="I2">
         <f>Data!P80</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J2" t="e">
+        <v>0.32082130082460703</v>
+      </c>
+      <c r="J2">
         <f>Data!Q80</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K2" t="e">
+        <v>0.38936076605077802</v>
+      </c>
+      <c r="K2">
         <f>Data!R80</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L2" t="e">
+        <v>0.46257015465625045</v>
+      </c>
+      <c r="L2">
         <f>Data!S80</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M2" t="e">
+        <v>0.5374298453437496</v>
+      </c>
+      <c r="M2">
         <f>Data!T80</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N2" t="e">
+        <v>0.61063923394922204</v>
+      </c>
+      <c r="N2">
         <f>Data!U80</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O2" t="e">
+        <v>0.67917869917539297</v>
+      </c>
+      <c r="O2">
         <f>Data!V80</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P2" t="e">
+        <v>0.740774899182154</v>
+      </c>
+      <c r="P2">
         <f>Data!W80</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q2" t="e">
+        <v>0.79412962819905253</v>
+      </c>
+      <c r="Q2">
         <f>Data!X80</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R2" t="e">
+        <v>0.83889105042341472</v>
+      </c>
+      <c r="R2">
         <f>Data!Y80</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S2" t="e">
+        <v>0.87544664181258358</v>
+      </c>
+      <c r="S2">
         <f>Data!Z80</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T2" t="e">
+        <v>0.90465053510089055</v>
+      </c>
+      <c r="T2">
         <f>Data!AA80</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U2" t="e">
+        <v>0.92757351463848225</v>
+      </c>
+      <c r="U2">
         <f>Data!AB80</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="V2" t="e">
+        <v>0.94531868278405917</v>
+      </c>
+      <c r="V2">
         <f>Data!AC80</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="W2" t="e">
+        <v>0.95890872179953501</v>
+      </c>
+      <c r="W2">
         <f>Data!AD80</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="X2" t="e">
+        <v>0.96923114064285198</v>
+      </c>
+      <c r="X2">
         <f>Data!AE80</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Y2" t="e">
+        <v>0.97702263008997436</v>
+      </c>
+      <c r="Y2">
         <f>Data!AF80</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Z2" t="e">
+        <v>0.98287596668427235</v>
+      </c>
+      <c r="Z2">
         <f>Data!AG80</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AA2" t="e">
+        <v>0.98725765053588843</v>
+      </c>
+      <c r="AA2">
         <f>Data!AH80</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AB2" t="e">
+        <v>0.99052895641805383</v>
+      </c>
+      <c r="AB2">
         <f>Data!AI80</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AC2" t="e">
+        <v>0.99296641284500486</v>
+      </c>
+      <c r="AC2">
         <f>Data!AJ80</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AD2" t="e">
+        <v>0.99477987430644166</v>
+      </c>
+      <c r="AD2">
         <f>Data!AK80</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AE2" t="e">
+        <v>0.99612759655932892</v>
+      </c>
+      <c r="AE2">
         <f>Data!AL80</f>
-        <v>#DIV/0!</v>
+        <v>0.99712837084429951</v>
       </c>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.25">
@@ -25540,7 +25540,7 @@
   </sheetPr>
   <dimension ref="A1:AE8"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AF1" sqref="AF1:AF1048576"/>
     </sheetView>
   </sheetViews>
@@ -56118,7 +56118,7 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H7"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -63345,8 +63345,8 @@
   </sheetPr>
   <dimension ref="A1:AL93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="N80" sqref="N80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -73227,136 +73227,136 @@
       <c r="C80" t="s">
         <v>1</v>
       </c>
-      <c r="E80" s="22" t="e">
-        <f>'SYVbT-passenger'!C6/SUM('SYVbT-passenger'!6:6)</f>
-        <v>#DIV/0!</v>
+      <c r="E80" s="22">
+        <f>'SYVbT-passenger'!C7/SUM('SYVbT-passenger'!7:7)</f>
+        <v>0</v>
       </c>
       <c r="F80">
         <v>1</v>
       </c>
-      <c r="G80" s="7" t="e">
+      <c r="G80" s="7" t="str">
         <f>IF(E80=F80,"n/a",IF(OR(C80="battery electric vehicle",C80="natural gas vehicle",C80="plugin hybrid vehicle"),"s-curve","linear"))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I80" s="22" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J80" t="e">
+        <v>s-curve</v>
+      </c>
+      <c r="I80" s="22">
+        <f>E80</f>
+        <v>0</v>
+      </c>
+      <c r="J80">
         <f>IF($G80="s-curve",$E80+($F80-$E80)*$O$2/(1+EXP($O$3*(COUNT($I$9:J$9)+$O$4))),TREND($E80:$F80,$E$9:$F$9,J$9))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K80" t="e">
+        <v>7.2426485361517731E-2</v>
+      </c>
+      <c r="K80">
         <f>IF($G80="s-curve",$E80+($F80-$E80)*$O$2/(1+EXP($O$3*(COUNT($I$9:K$9)+$O$4))),TREND($E80:$F80,$E$9:$F$9,K$9))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L80" t="e">
+        <v>9.534946489910949E-2</v>
+      </c>
+      <c r="L80">
         <f>IF($G80="s-curve",$E80+($F80-$E80)*$O$2/(1+EXP($O$3*(COUNT($I$9:L$9)+$O$4))),TREND($E80:$F80,$E$9:$F$9,L$9))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M80" t="e">
+        <v>0.12455335818741645</v>
+      </c>
+      <c r="M80">
         <f>IF($G80="s-curve",$E80+($F80-$E80)*$O$2/(1+EXP($O$3*(COUNT($I$9:M$9)+$O$4))),TREND($E80:$F80,$E$9:$F$9,M$9))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N80" t="e">
+        <v>0.16110894957658525</v>
+      </c>
+      <c r="N80">
         <f>IF($G80="s-curve",$E80+($F80-$E80)*$O$2/(1+EXP($O$3*(COUNT($I$9:N$9)+$O$4))),TREND($E80:$F80,$E$9:$F$9,N$9))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O80" t="e">
+        <v>0.20587037180094736</v>
+      </c>
+      <c r="O80">
         <f>IF($G80="s-curve",$E80+($F80-$E80)*$O$2/(1+EXP($O$3*(COUNT($I$9:O$9)+$O$4))),TREND($E80:$F80,$E$9:$F$9,O$9))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P80" t="e">
+        <v>0.259225100817846</v>
+      </c>
+      <c r="P80">
         <f>IF($G80="s-curve",$E80+($F80-$E80)*$O$2/(1+EXP($O$3*(COUNT($I$9:P$9)+$O$4))),TREND($E80:$F80,$E$9:$F$9,P$9))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q80" t="e">
+        <v>0.32082130082460703</v>
+      </c>
+      <c r="Q80">
         <f>IF($G80="s-curve",$E80+($F80-$E80)*$O$2/(1+EXP($O$3*(COUNT($I$9:Q$9)+$O$4))),TREND($E80:$F80,$E$9:$F$9,Q$9))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R80" t="e">
+        <v>0.38936076605077802</v>
+      </c>
+      <c r="R80">
         <f>IF($G80="s-curve",$E80+($F80-$E80)*$O$2/(1+EXP($O$3*(COUNT($I$9:R$9)+$O$4))),TREND($E80:$F80,$E$9:$F$9,R$9))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S80" t="e">
+        <v>0.46257015465625045</v>
+      </c>
+      <c r="S80">
         <f>IF($G80="s-curve",$E80+($F80-$E80)*$O$2/(1+EXP($O$3*(COUNT($I$9:S$9)+$O$4))),TREND($E80:$F80,$E$9:$F$9,S$9))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T80" t="e">
+        <v>0.5374298453437496</v>
+      </c>
+      <c r="T80">
         <f>IF($G80="s-curve",$E80+($F80-$E80)*$O$2/(1+EXP($O$3*(COUNT($I$9:T$9)+$O$4))),TREND($E80:$F80,$E$9:$F$9,T$9))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U80" t="e">
+        <v>0.61063923394922204</v>
+      </c>
+      <c r="U80">
         <f>IF($G80="s-curve",$E80+($F80-$E80)*$O$2/(1+EXP($O$3*(COUNT($I$9:U$9)+$O$4))),TREND($E80:$F80,$E$9:$F$9,U$9))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="V80" t="e">
+        <v>0.67917869917539297</v>
+      </c>
+      <c r="V80">
         <f>IF($G80="s-curve",$E80+($F80-$E80)*$O$2/(1+EXP($O$3*(COUNT($I$9:V$9)+$O$4))),TREND($E80:$F80,$E$9:$F$9,V$9))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="W80" t="e">
+        <v>0.740774899182154</v>
+      </c>
+      <c r="W80">
         <f>IF($G80="s-curve",$E80+($F80-$E80)*$O$2/(1+EXP($O$3*(COUNT($I$9:W$9)+$O$4))),TREND($E80:$F80,$E$9:$F$9,W$9))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="X80" t="e">
+        <v>0.79412962819905253</v>
+      </c>
+      <c r="X80">
         <f>IF($G80="s-curve",$E80+($F80-$E80)*$O$2/(1+EXP($O$3*(COUNT($I$9:X$9)+$O$4))),TREND($E80:$F80,$E$9:$F$9,X$9))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Y80" t="e">
+        <v>0.83889105042341472</v>
+      </c>
+      <c r="Y80">
         <f>IF($G80="s-curve",$E80+($F80-$E80)*$O$2/(1+EXP($O$3*(COUNT($I$9:Y$9)+$O$4))),TREND($E80:$F80,$E$9:$F$9,Y$9))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Z80" t="e">
+        <v>0.87544664181258358</v>
+      </c>
+      <c r="Z80">
         <f>IF($G80="s-curve",$E80+($F80-$E80)*$O$2/(1+EXP($O$3*(COUNT($I$9:Z$9)+$O$4))),TREND($E80:$F80,$E$9:$F$9,Z$9))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AA80" t="e">
+        <v>0.90465053510089055</v>
+      </c>
+      <c r="AA80">
         <f>IF($G80="s-curve",$E80+($F80-$E80)*$O$2/(1+EXP($O$3*(COUNT($I$9:AA$9)+$O$4))),TREND($E80:$F80,$E$9:$F$9,AA$9))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AB80" t="e">
+        <v>0.92757351463848225</v>
+      </c>
+      <c r="AB80">
         <f>IF($G80="s-curve",$E80+($F80-$E80)*$O$2/(1+EXP($O$3*(COUNT($I$9:AB$9)+$O$4))),TREND($E80:$F80,$E$9:$F$9,AB$9))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AC80" t="e">
+        <v>0.94531868278405917</v>
+      </c>
+      <c r="AC80">
         <f>IF($G80="s-curve",$E80+($F80-$E80)*$O$2/(1+EXP($O$3*(COUNT($I$9:AC$9)+$O$4))),TREND($E80:$F80,$E$9:$F$9,AC$9))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AD80" t="e">
+        <v>0.95890872179953501</v>
+      </c>
+      <c r="AD80">
         <f>IF($G80="s-curve",$E80+($F80-$E80)*$O$2/(1+EXP($O$3*(COUNT($I$9:AD$9)+$O$4))),TREND($E80:$F80,$E$9:$F$9,AD$9))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AE80" t="e">
+        <v>0.96923114064285198</v>
+      </c>
+      <c r="AE80">
         <f>IF($G80="s-curve",$E80+($F80-$E80)*$O$2/(1+EXP($O$3*(COUNT($I$9:AE$9)+$O$4))),TREND($E80:$F80,$E$9:$F$9,AE$9))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AF80" t="e">
+        <v>0.97702263008997436</v>
+      </c>
+      <c r="AF80">
         <f>IF($G80="s-curve",$E80+($F80-$E80)*$O$2/(1+EXP($O$3*(COUNT($I$9:AF$9)+$O$4))),TREND($E80:$F80,$E$9:$F$9,AF$9))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AG80" t="e">
+        <v>0.98287596668427235</v>
+      </c>
+      <c r="AG80">
         <f>IF($G80="s-curve",$E80+($F80-$E80)*$O$2/(1+EXP($O$3*(COUNT($I$9:AG$9)+$O$4))),TREND($E80:$F80,$E$9:$F$9,AG$9))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AH80" t="e">
+        <v>0.98725765053588843</v>
+      </c>
+      <c r="AH80">
         <f>IF($G80="s-curve",$E80+($F80-$E80)*$O$2/(1+EXP($O$3*(COUNT($I$9:AH$9)+$O$4))),TREND($E80:$F80,$E$9:$F$9,AH$9))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AI80" t="e">
+        <v>0.99052895641805383</v>
+      </c>
+      <c r="AI80">
         <f>IF($G80="s-curve",$E80+($F80-$E80)*$O$2/(1+EXP($O$3*(COUNT($I$9:AI$9)+$O$4))),TREND($E80:$F80,$E$9:$F$9,AI$9))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AJ80" t="e">
+        <v>0.99296641284500486</v>
+      </c>
+      <c r="AJ80">
         <f>IF($G80="s-curve",$E80+($F80-$E80)*$O$2/(1+EXP($O$3*(COUNT($I$9:AJ$9)+$O$4))),TREND($E80:$F80,$E$9:$F$9,AJ$9))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AK80" t="e">
+        <v>0.99477987430644166</v>
+      </c>
+      <c r="AK80">
         <f>IF($G80="s-curve",$E80+($F80-$E80)*$O$2/(1+EXP($O$3*(COUNT($I$9:AK$9)+$O$4))),TREND($E80:$F80,$E$9:$F$9,AK$9))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AL80" t="e">
+        <v>0.99612759655932892</v>
+      </c>
+      <c r="AL80">
         <f>IF($G80="s-curve",$E80+($F80-$E80)*$O$2/(1+EXP($O$3*(COUNT($I$9:AL$9)+$O$4))),TREND($E80:$F80,$E$9:$F$9,AL$9))</f>
-        <v>#DIV/0!</v>
+        <v>0.99712837084429951</v>
       </c>
     </row>
     <row r="81" spans="1:38" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updates to BRZSPbS and TTS to smooth sales shares
</commit_message>
<xml_diff>
--- a/InputData/trans/TTS/Transportation Technology Shareweights.xlsx
+++ b/InputData/trans/TTS/Transportation Technology Shareweights.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mary Francis Swint\Vensim\eps-eu\InputData\trans\TTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F794058-BCE9-4C15-AE16-1BC82961E46E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E803E369-3891-4FC1-9D03-55B00C5B5522}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="90" yWindow="1300" windowWidth="19110" windowHeight="10000" firstSheet="7" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" firstSheet="7" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -10144,123 +10144,123 @@
       </c>
       <c r="B2">
         <f>Data!I24</f>
-        <v>0.8</v>
+        <v>0.6</v>
       </c>
       <c r="C2">
         <f>Data!J24</f>
-        <v>0.92312502511458017</v>
+        <v>0.6289705941446071</v>
       </c>
       <c r="D2">
         <f>Data!K24</f>
-        <v>0.96209409032848614</v>
+        <v>0.63813978595964382</v>
       </c>
       <c r="E2">
         <f>Data!L24</f>
-        <v>1.0117407089186079</v>
+        <v>0.64982134327496655</v>
       </c>
       <c r="F2">
         <f>Data!M24</f>
-        <v>1.0738852142801949</v>
+        <v>0.66444357983063407</v>
       </c>
       <c r="G2">
         <f>Data!N24</f>
-        <v>1.1499796320616105</v>
+        <v>0.68234814872037897</v>
       </c>
       <c r="H2">
         <f>Data!O24</f>
-        <v>1.2406826713903383</v>
+        <v>0.70369004032713844</v>
       </c>
       <c r="I2">
         <f>Data!P24</f>
-        <v>1.3453962114018321</v>
+        <v>0.72832852032984285</v>
       </c>
       <c r="J2">
         <f>Data!Q24</f>
-        <v>1.4619133022863227</v>
+        <v>0.75574430642031121</v>
       </c>
       <c r="K2">
         <f>Data!R24</f>
-        <v>1.5863692629156259</v>
+        <v>0.78502806186250018</v>
       </c>
       <c r="L2">
         <f>Data!S24</f>
-        <v>1.7136307370843742</v>
+        <v>0.8149719381374998</v>
       </c>
       <c r="M2">
         <f>Data!T24</f>
-        <v>1.8380866977136774</v>
+        <v>0.84425569357968877</v>
       </c>
       <c r="N2">
         <f>Data!U24</f>
-        <v>1.954603788598168</v>
+        <v>0.87167147967015723</v>
       </c>
       <c r="O2">
         <f>Data!V24</f>
-        <v>2.0593173286096618</v>
+        <v>0.89630995967286164</v>
       </c>
       <c r="P2">
         <f>Data!W24</f>
-        <v>2.1500203679383896</v>
+        <v>0.91765185127962101</v>
       </c>
       <c r="Q2">
         <f>Data!X24</f>
-        <v>2.2261147857198051</v>
+        <v>0.93555642016936591</v>
       </c>
       <c r="R2">
         <f>Data!Y24</f>
-        <v>2.2882592910813919</v>
+        <v>0.95017865672503343</v>
       </c>
       <c r="S2">
         <f>Data!Z24</f>
-        <v>2.3379059096715142</v>
+        <v>0.96186021404035627</v>
       </c>
       <c r="T2">
         <f>Data!AA24</f>
-        <v>2.3768749748854199</v>
+        <v>0.97102940585539288</v>
       </c>
       <c r="U2">
         <f>Data!AB24</f>
-        <v>2.4070417607329007</v>
+        <v>0.97812747311362369</v>
       </c>
       <c r="V2">
         <f>Data!AC24</f>
-        <v>2.4301448270592099</v>
+        <v>0.98356348871981403</v>
       </c>
       <c r="W2">
         <f>Data!AD24</f>
-        <v>2.4476929390928484</v>
+        <v>0.98769245625714075</v>
       </c>
       <c r="X2">
         <f>Data!AE24</f>
-        <v>2.4609384711529563</v>
+        <v>0.99080905203598979</v>
       </c>
       <c r="Y2">
         <f>Data!AF24</f>
-        <v>2.4708891433632632</v>
+        <v>0.99315038667370892</v>
       </c>
       <c r="Z2">
         <f>Data!AG24</f>
-        <v>2.4783380059110103</v>
+        <v>0.99490306021435537</v>
       </c>
       <c r="AA2">
         <f>Data!AH24</f>
-        <v>2.4838992259106916</v>
+        <v>0.99621158256722153</v>
       </c>
       <c r="AB2">
         <f>Data!AI24</f>
-        <v>2.4880429018365082</v>
+        <v>0.99718656513800186</v>
       </c>
       <c r="AC2">
         <f>Data!AJ24</f>
-        <v>2.4911257863209508</v>
+        <v>0.99791194972257657</v>
       </c>
       <c r="AD2">
         <f>Data!AK24</f>
-        <v>2.4934169141508589</v>
+        <v>0.99845103862373152</v>
       </c>
       <c r="AE2">
         <f>Data!AL24</f>
-        <v>2.4951182304353092</v>
+        <v>0.99885134833771982</v>
       </c>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.25">
@@ -10269,123 +10269,123 @@
       </c>
       <c r="B3">
         <f>Data!I25</f>
-        <v>2.4652000233370237E-2</v>
+        <v>0.29802375741500553</v>
       </c>
       <c r="C3">
         <f>Data!J25</f>
-        <v>2.8190631841939744E-2</v>
+        <v>0.29596244960239987</v>
       </c>
       <c r="D3">
         <f>Data!K25</f>
-        <v>2.9404090553188392E-2</v>
+        <v>0.29525559107671612</v>
       </c>
       <c r="E3">
         <f>Data!L25</f>
-        <v>3.1022432090970165E-2</v>
+        <v>0.29431288202296346</v>
       </c>
       <c r="F3">
         <f>Data!M25</f>
-        <v>3.3171904436085045E-2</v>
+        <v>0.2930607810336332</v>
       </c>
       <c r="G3">
         <f>Data!N25</f>
-        <v>3.6011302648198545E-2</v>
+        <v>0.29140678752282123</v>
       </c>
       <c r="H3">
         <f>Data!O25</f>
-        <v>3.9735188957166843E-2</v>
+        <v>0.28923756597307232</v>
       </c>
       <c r="I3">
         <f>Data!P25</f>
-        <v>4.4573274188492537E-2</v>
+        <v>0.28641930626464923</v>
       </c>
       <c r="J3">
         <f>Data!Q25</f>
-        <v>5.0782542518116404E-2</v>
+        <v>0.28280231112804816</v>
       </c>
       <c r="K3">
         <f>Data!R25</f>
-        <v>5.8627740396068245E-2</v>
+        <v>0.27823236164867954</v>
       </c>
       <c r="L3">
         <f>Data!S25</f>
-        <v>6.834601268394247E-2</v>
+        <v>0.2725713172654462</v>
       </c>
       <c r="M3">
         <f>Data!T25</f>
-        <v>8.0094247462594942E-2</v>
+        <v>0.26572778823718668</v>
       </c>
       <c r="N3">
         <f>Data!U25</f>
-        <v>9.3884505464127355E-2</v>
+        <v>0.25769474900033379</v>
       </c>
       <c r="O3">
         <f>Data!V25</f>
-        <v>0.10952333536510674</v>
+        <v>0.24858488795211589</v>
       </c>
       <c r="P3">
         <f>Data!W25</f>
-        <v>0.12658024788693495</v>
+        <v>0.23864897177620478</v>
       </c>
       <c r="Q3">
         <f>Data!X25</f>
-        <v>0.14441049547812879</v>
+        <v>0.22826257592436899</v>
       </c>
       <c r="R3">
         <f>Data!Y25</f>
-        <v>0.16224074306932265</v>
+        <v>0.21787618007253318</v>
       </c>
       <c r="S3">
         <f>Data!Z25</f>
-        <v>0.17929765559115082</v>
+        <v>0.20794026389662207</v>
       </c>
       <c r="T3">
         <f>Data!AA25</f>
-        <v>0.19493648549213022</v>
+        <v>0.19883040284840414</v>
       </c>
       <c r="U3">
         <f>Data!AB25</f>
-        <v>0.20872674349366263</v>
+        <v>0.19079736361155128</v>
       </c>
       <c r="V3">
         <f>Data!AC25</f>
-        <v>0.2204749782723151</v>
+        <v>0.18395383458329176</v>
       </c>
       <c r="W3">
         <f>Data!AD25</f>
-        <v>0.23019325056018936</v>
+        <v>0.17829279020005839</v>
       </c>
       <c r="X3">
         <f>Data!AE25</f>
-        <v>0.2380384484381412</v>
+        <v>0.17372284072068978</v>
       </c>
       <c r="Y3">
         <f>Data!AF25</f>
-        <v>0.24424771676776508</v>
+        <v>0.17010584558408873</v>
       </c>
       <c r="Z3">
         <f>Data!AG25</f>
-        <v>0.24908580199909075</v>
+        <v>0.16728758587566564</v>
       </c>
       <c r="AA3">
         <f>Data!AH25</f>
-        <v>0.25280968830805906</v>
+        <v>0.1651183643259167</v>
       </c>
       <c r="AB3">
         <f>Data!AI25</f>
-        <v>0.25564908652017254</v>
+        <v>0.16346437081510473</v>
       </c>
       <c r="AC3">
         <f>Data!AJ25</f>
-        <v>0.25779855886528741</v>
+        <v>0.1622122698257745</v>
       </c>
       <c r="AD3">
         <f>Data!AK25</f>
-        <v>0.25941690040306919</v>
+        <v>0.16126956077202181</v>
       </c>
       <c r="AE3">
         <f>Data!AL25</f>
-        <v>0.26063035911431781</v>
+        <v>0.16056270224633809</v>
       </c>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.25">
@@ -10394,123 +10394,123 @@
       </c>
       <c r="B4">
         <f>Data!I26</f>
-        <v>2.1762390509853201E-3</v>
+        <v>0.29802375741500553</v>
       </c>
       <c r="C4">
         <f>Data!J26</f>
-        <v>2.1762390509853201E-3</v>
+        <v>0.29802375741500553</v>
       </c>
       <c r="D4">
         <f>Data!K26</f>
-        <v>2.1762390509853201E-3</v>
+        <v>0.29802375741500553</v>
       </c>
       <c r="E4">
         <f>Data!L26</f>
-        <v>2.1762390509853201E-3</v>
+        <v>0.29802375741500553</v>
       </c>
       <c r="F4">
         <f>Data!M26</f>
-        <v>2.1762390509853201E-3</v>
+        <v>0.29802375741500553</v>
       </c>
       <c r="G4">
         <f>Data!N26</f>
-        <v>2.1762390509853201E-3</v>
+        <v>0.29802375741500553</v>
       </c>
       <c r="H4">
         <f>Data!O26</f>
-        <v>2.1762390509853201E-3</v>
+        <v>0.29802375741500553</v>
       </c>
       <c r="I4">
         <f>Data!P26</f>
-        <v>2.1762390509853201E-3</v>
+        <v>0.29802375741500553</v>
       </c>
       <c r="J4">
         <f>Data!Q26</f>
-        <v>2.1762390509853201E-3</v>
+        <v>0.29802375741500553</v>
       </c>
       <c r="K4">
         <f>Data!R26</f>
-        <v>2.1762390509853201E-3</v>
+        <v>0.29802375741500553</v>
       </c>
       <c r="L4">
         <f>Data!S26</f>
-        <v>2.1762390509853201E-3</v>
+        <v>0.29802375741500553</v>
       </c>
       <c r="M4">
         <f>Data!T26</f>
-        <v>2.1762390509853201E-3</v>
+        <v>0.29802375741500553</v>
       </c>
       <c r="N4">
         <f>Data!U26</f>
-        <v>2.1762390509853201E-3</v>
+        <v>0.29802375741500553</v>
       </c>
       <c r="O4">
         <f>Data!V26</f>
-        <v>2.1762390509853201E-3</v>
+        <v>0.29802375741500553</v>
       </c>
       <c r="P4">
         <f>Data!W26</f>
-        <v>2.1762390509853201E-3</v>
+        <v>0.29802375741500553</v>
       </c>
       <c r="Q4">
         <f>Data!X26</f>
-        <v>2.1762390509853201E-3</v>
+        <v>0.29802375741500553</v>
       </c>
       <c r="R4">
         <f>Data!Y26</f>
-        <v>2.1762390509853201E-3</v>
+        <v>0.29802375741500553</v>
       </c>
       <c r="S4">
         <f>Data!Z26</f>
-        <v>2.1762390509853201E-3</v>
+        <v>0.29802375741500553</v>
       </c>
       <c r="T4">
         <f>Data!AA26</f>
-        <v>2.1762390509853201E-3</v>
+        <v>0.29802375741500553</v>
       </c>
       <c r="U4">
         <f>Data!AB26</f>
-        <v>2.1762390509853201E-3</v>
+        <v>0.29802375741500553</v>
       </c>
       <c r="V4">
         <f>Data!AC26</f>
-        <v>2.1762390509853201E-3</v>
+        <v>0.29802375741500553</v>
       </c>
       <c r="W4">
         <f>Data!AD26</f>
-        <v>2.1762390509853201E-3</v>
+        <v>0.29802375741500553</v>
       </c>
       <c r="X4">
         <f>Data!AE26</f>
-        <v>2.1762390509853201E-3</v>
+        <v>0.29802375741500553</v>
       </c>
       <c r="Y4">
         <f>Data!AF26</f>
-        <v>2.1762390509853201E-3</v>
+        <v>0.29802375741500553</v>
       </c>
       <c r="Z4">
         <f>Data!AG26</f>
-        <v>2.1762390509853201E-3</v>
+        <v>0.29802375741500553</v>
       </c>
       <c r="AA4">
         <f>Data!AH26</f>
-        <v>2.1762390509853201E-3</v>
+        <v>0.29802375741500553</v>
       </c>
       <c r="AB4">
         <f>Data!AI26</f>
-        <v>2.1762390509853201E-3</v>
+        <v>0.29802375741500553</v>
       </c>
       <c r="AC4">
         <f>Data!AJ26</f>
-        <v>2.1762390509853201E-3</v>
+        <v>0.29802375741500553</v>
       </c>
       <c r="AD4">
         <f>Data!AK26</f>
-        <v>2.1762390509853201E-3</v>
+        <v>0.29802375741500553</v>
       </c>
       <c r="AE4">
         <f>Data!AL26</f>
-        <v>2.1762390509853201E-3</v>
+        <v>0.29802375741500553</v>
       </c>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.25">
@@ -10519,123 +10519,123 @@
       </c>
       <c r="B5">
         <f>Data!I27</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="C5">
         <f>Data!J27</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D5">
         <f>Data!K27</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E5">
         <f>Data!L27</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="F5">
         <f>Data!M27</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="G5">
         <f>Data!N27</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="H5">
         <f>Data!O27</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="I5">
         <f>Data!P27</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J5">
         <f>Data!Q27</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="K5">
         <f>Data!R27</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="L5">
         <f>Data!S27</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="M5">
         <f>Data!T27</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="N5">
         <f>Data!U27</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="O5">
         <f>Data!V27</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="P5">
         <f>Data!W27</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="Q5">
         <f>Data!X27</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="R5">
         <f>Data!Y27</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="S5">
         <f>Data!Z27</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="T5">
         <f>Data!AA27</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="U5">
         <f>Data!AB27</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="V5">
         <f>Data!AC27</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="W5">
         <f>Data!AD27</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="X5">
         <f>Data!AE27</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="Y5">
         <f>Data!AF27</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="Z5">
         <f>Data!AG27</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="AA5">
         <f>Data!AH27</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="AB5">
         <f>Data!AI27</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="AC5">
         <f>Data!AJ27</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="AD5">
         <f>Data!AK27</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="AE5">
         <f>Data!AL27</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.25">
@@ -10644,123 +10644,123 @@
       </c>
       <c r="B6">
         <f>Data!I28</f>
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="C6">
         <f>Data!J28</f>
-        <v>1.985225968306727E-2</v>
+        <v>8.8644190159638335E-5</v>
       </c>
       <c r="D6">
         <f>Data!K28</f>
-        <v>1.9801596942659226E-2</v>
+        <v>1.1904183440446507E-4</v>
       </c>
       <c r="E6">
         <f>Data!L28</f>
-        <v>1.9734030064231342E-2</v>
+        <v>1.5958196146119519E-4</v>
       </c>
       <c r="F6">
         <f>Data!M28</f>
-        <v>1.9644288107273637E-2</v>
+        <v>2.1342713563581709E-4</v>
       </c>
       <c r="G6">
         <f>Data!N28</f>
-        <v>1.9525741268224331E-2</v>
+        <v>2.845552390654007E-4</v>
       </c>
       <c r="H6">
         <f>Data!O28</f>
-        <v>1.9370266439430035E-2</v>
+        <v>3.7784013634197905E-4</v>
       </c>
       <c r="I6">
         <f>Data!P28</f>
-        <v>1.9168273035060777E-2</v>
+        <v>4.9903617896353422E-4</v>
       </c>
       <c r="J6">
         <f>Data!Q28</f>
-        <v>1.8909031788043873E-2</v>
+        <v>6.5458092717367755E-4</v>
       </c>
       <c r="K6">
         <f>Data!R28</f>
-        <v>1.8581489350995122E-2</v>
+        <v>8.5110638940292692E-4</v>
       </c>
       <c r="L6">
         <f>Data!S28</f>
-        <v>1.8175744761936438E-2</v>
+        <v>1.0945531428381381E-3</v>
       </c>
       <c r="M6">
         <f>Data!T28</f>
-        <v>1.7685247834990175E-2</v>
+        <v>1.3888512990058942E-3</v>
       </c>
       <c r="N6">
         <f>Data!U28</f>
-        <v>1.7109495026250039E-2</v>
+        <v>1.7343029842499763E-3</v>
       </c>
       <c r="O6">
         <f>Data!V28</f>
-        <v>1.6456563062257956E-2</v>
+        <v>2.1260621626452273E-3</v>
       </c>
       <c r="P6">
         <f>Data!W28</f>
-        <v>1.5744425168116589E-2</v>
+        <v>2.553344899130046E-3</v>
       </c>
       <c r="Q6">
         <f>Data!X28</f>
-        <v>1.4999999999999999E-2</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="R6">
         <f>Data!Y28</f>
-        <v>1.4255574831883409E-2</v>
+        <v>3.4466551008699542E-3</v>
       </c>
       <c r="S6">
         <f>Data!Z28</f>
-        <v>1.3543436937742046E-2</v>
+        <v>3.8739378373547728E-3</v>
       </c>
       <c r="T6">
         <f>Data!AA28</f>
-        <v>1.2890504973749961E-2</v>
+        <v>4.2656970157500234E-3</v>
       </c>
       <c r="U6">
         <f>Data!AB28</f>
-        <v>1.2314752165009824E-2</v>
+        <v>4.6111487009941055E-3</v>
       </c>
       <c r="V6">
         <f>Data!AC28</f>
-        <v>1.1824255238063564E-2</v>
+        <v>4.9054468571618614E-3</v>
       </c>
       <c r="W6">
         <f>Data!AD28</f>
-        <v>1.1418510649004877E-2</v>
+        <v>5.1488936105970736E-3</v>
       </c>
       <c r="X6">
         <f>Data!AE28</f>
-        <v>1.1090968211956129E-2</v>
+        <v>5.3454190728263228E-3</v>
       </c>
       <c r="Y6">
         <f>Data!AF28</f>
-        <v>1.0831726964939224E-2</v>
+        <v>5.5009638210364665E-3</v>
       </c>
       <c r="Z6">
         <f>Data!AG28</f>
-        <v>1.0629733560569964E-2</v>
+        <v>5.6221598636580217E-3</v>
       </c>
       <c r="AA6">
         <f>Data!AH28</f>
-        <v>1.0474258731775666E-2</v>
+        <v>5.7154447609346001E-3</v>
       </c>
       <c r="AB6">
         <f>Data!AI28</f>
-        <v>1.0355711892726362E-2</v>
+        <v>5.7865728643641829E-3</v>
       </c>
       <c r="AC6">
         <f>Data!AJ28</f>
-        <v>1.026596993576866E-2</v>
+        <v>5.840418038538805E-3</v>
       </c>
       <c r="AD6">
         <f>Data!AK28</f>
-        <v>1.0198403057340774E-2</v>
+        <v>5.880958165595535E-3</v>
       </c>
       <c r="AE6">
         <f>Data!AL28</f>
-        <v>1.0147740316932731E-2</v>
+        <v>5.9113558098403615E-3</v>
       </c>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.25">
@@ -10769,123 +10769,123 @@
       </c>
       <c r="B7">
         <f>Data!I29</f>
-        <v>1.1960398418308864E-2</v>
+        <v>2.1496445375763083E-2</v>
       </c>
       <c r="C7">
         <f>B7</f>
-        <v>1.1960398418308864E-2</v>
+        <v>2.1496445375763083E-2</v>
       </c>
       <c r="D7">
         <f t="shared" ref="D7:AE7" si="0">C7</f>
-        <v>1.1960398418308864E-2</v>
+        <v>2.1496445375763083E-2</v>
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
-        <v>1.1960398418308864E-2</v>
+        <v>2.1496445375763083E-2</v>
       </c>
       <c r="F7">
         <f t="shared" si="0"/>
-        <v>1.1960398418308864E-2</v>
+        <v>2.1496445375763083E-2</v>
       </c>
       <c r="G7">
         <f t="shared" si="0"/>
-        <v>1.1960398418308864E-2</v>
+        <v>2.1496445375763083E-2</v>
       </c>
       <c r="H7">
         <f t="shared" si="0"/>
-        <v>1.1960398418308864E-2</v>
+        <v>2.1496445375763083E-2</v>
       </c>
       <c r="I7">
         <f t="shared" si="0"/>
-        <v>1.1960398418308864E-2</v>
+        <v>2.1496445375763083E-2</v>
       </c>
       <c r="J7">
         <f t="shared" si="0"/>
-        <v>1.1960398418308864E-2</v>
+        <v>2.1496445375763083E-2</v>
       </c>
       <c r="K7">
         <f t="shared" si="0"/>
-        <v>1.1960398418308864E-2</v>
+        <v>2.1496445375763083E-2</v>
       </c>
       <c r="L7">
         <f t="shared" si="0"/>
-        <v>1.1960398418308864E-2</v>
+        <v>2.1496445375763083E-2</v>
       </c>
       <c r="M7">
         <f t="shared" si="0"/>
-        <v>1.1960398418308864E-2</v>
+        <v>2.1496445375763083E-2</v>
       </c>
       <c r="N7">
         <f t="shared" si="0"/>
-        <v>1.1960398418308864E-2</v>
+        <v>2.1496445375763083E-2</v>
       </c>
       <c r="O7">
         <f t="shared" si="0"/>
-        <v>1.1960398418308864E-2</v>
+        <v>2.1496445375763083E-2</v>
       </c>
       <c r="P7">
         <f t="shared" si="0"/>
-        <v>1.1960398418308864E-2</v>
+        <v>2.1496445375763083E-2</v>
       </c>
       <c r="Q7">
         <f t="shared" si="0"/>
-        <v>1.1960398418308864E-2</v>
+        <v>2.1496445375763083E-2</v>
       </c>
       <c r="R7">
         <f t="shared" si="0"/>
-        <v>1.1960398418308864E-2</v>
+        <v>2.1496445375763083E-2</v>
       </c>
       <c r="S7">
         <f t="shared" si="0"/>
-        <v>1.1960398418308864E-2</v>
+        <v>2.1496445375763083E-2</v>
       </c>
       <c r="T7">
         <f t="shared" si="0"/>
-        <v>1.1960398418308864E-2</v>
+        <v>2.1496445375763083E-2</v>
       </c>
       <c r="U7">
         <f t="shared" si="0"/>
-        <v>1.1960398418308864E-2</v>
+        <v>2.1496445375763083E-2</v>
       </c>
       <c r="V7">
         <f t="shared" si="0"/>
-        <v>1.1960398418308864E-2</v>
+        <v>2.1496445375763083E-2</v>
       </c>
       <c r="W7">
         <f t="shared" si="0"/>
-        <v>1.1960398418308864E-2</v>
+        <v>2.1496445375763083E-2</v>
       </c>
       <c r="X7">
         <f t="shared" si="0"/>
-        <v>1.1960398418308864E-2</v>
+        <v>2.1496445375763083E-2</v>
       </c>
       <c r="Y7">
         <f t="shared" si="0"/>
-        <v>1.1960398418308864E-2</v>
+        <v>2.1496445375763083E-2</v>
       </c>
       <c r="Z7">
         <f t="shared" si="0"/>
-        <v>1.1960398418308864E-2</v>
+        <v>2.1496445375763083E-2</v>
       </c>
       <c r="AA7">
         <f t="shared" si="0"/>
-        <v>1.1960398418308864E-2</v>
+        <v>2.1496445375763083E-2</v>
       </c>
       <c r="AB7">
         <f t="shared" si="0"/>
-        <v>1.1960398418308864E-2</v>
+        <v>2.1496445375763083E-2</v>
       </c>
       <c r="AC7">
         <f t="shared" si="0"/>
-        <v>1.1960398418308864E-2</v>
+        <v>2.1496445375763083E-2</v>
       </c>
       <c r="AD7">
         <f t="shared" si="0"/>
-        <v>1.1960398418308864E-2</v>
+        <v>2.1496445375763083E-2</v>
       </c>
       <c r="AE7">
         <f t="shared" si="0"/>
-        <v>1.1960398418308864E-2</v>
+        <v>2.1496445375763083E-2</v>
       </c>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.25">
@@ -10894,123 +10894,123 @@
       </c>
       <c r="B8">
         <f>Data!I30</f>
-        <v>2.0195858052701565E-3</v>
+        <v>8.470448323552864E-5</v>
       </c>
       <c r="C8">
         <f>Data!J30</f>
-        <v>2.7284499652394639E-3</v>
+        <v>8.2215464117929744E-4</v>
       </c>
       <c r="D8">
         <f>Data!K30</f>
-        <v>2.9715318921412692E-3</v>
+        <v>1.0750392070949643E-3</v>
       </c>
       <c r="E8">
         <f>Data!L30</f>
-        <v>3.2957205734227501E-3</v>
+        <v>1.4123012774822749E-3</v>
       </c>
       <c r="F8">
         <f>Data!M30</f>
-        <v>3.7263061999703714E-3</v>
+        <v>1.860250907661926E-3</v>
       </c>
       <c r="G8">
         <f>Data!N30</f>
-        <v>4.2950988438765388E-3</v>
+        <v>2.4519809580343683E-3</v>
       </c>
       <c r="H8">
         <f>Data!O30</f>
-        <v>5.0410735121170485E-3</v>
+        <v>3.2280381605029394E-3</v>
       </c>
       <c r="I8">
         <f>Data!P30</f>
-        <v>6.010246232741108E-3</v>
+        <v>4.2362942076558247E-3</v>
       </c>
       <c r="J8">
         <f>Data!Q30</f>
-        <v>7.2540964735640472E-3</v>
+        <v>5.530304553154162E-3</v>
       </c>
       <c r="K8">
         <f>Data!R30</f>
-        <v>8.8256586531590669E-3</v>
+        <v>7.1652423071111148E-3</v>
       </c>
       <c r="L8">
         <f>Data!S30</f>
-        <v>1.0772437997189686E-2</v>
+        <v>9.1905284138303605E-3</v>
       </c>
       <c r="M8">
         <f>Data!T30</f>
-        <v>1.3125862568802056E-2</v>
+        <v>1.1638858319689102E-2</v>
       </c>
       <c r="N8">
         <f>Data!U30</f>
-        <v>1.5888348392515139E-2</v>
+        <v>1.4512745478976212E-2</v>
       </c>
       <c r="O8">
         <f>Data!V30</f>
-        <v>1.9021142999847009E-2</v>
+        <v>1.7771874672476845E-2</v>
       </c>
       <c r="P8">
         <f>Data!W30</f>
-        <v>2.2438010112313542E-2</v>
+        <v>2.1326532015952099E-2</v>
       </c>
       <c r="Q8">
         <f>Data!X30</f>
-        <v>2.6009792902635082E-2</v>
+        <v>2.5042352241617768E-2</v>
       </c>
       <c r="R8">
         <f>Data!Y30</f>
-        <v>2.9581575692956621E-2</v>
+        <v>2.8758172467283436E-2</v>
       </c>
       <c r="S8">
         <f>Data!Z30</f>
-        <v>3.2998442805423155E-2</v>
+        <v>3.2312829810758684E-2</v>
       </c>
       <c r="T8">
         <f>Data!AA30</f>
-        <v>3.6131237412755014E-2</v>
+        <v>3.5571959004259315E-2</v>
       </c>
       <c r="U8">
         <f>Data!AB30</f>
-        <v>3.88937232364681E-2</v>
+        <v>3.8445846163546425E-2</v>
       </c>
       <c r="V8">
         <f>Data!AC30</f>
-        <v>4.1247147808080475E-2</v>
+        <v>4.0894176069405173E-2</v>
       </c>
       <c r="W8">
         <f>Data!AD30</f>
-        <v>4.3193927152111095E-2</v>
+        <v>4.2919462176124419E-2</v>
       </c>
       <c r="X8">
         <f>Data!AE30</f>
-        <v>4.4765489331706113E-2</v>
+        <v>4.4554399930081368E-2</v>
       </c>
       <c r="Y8">
         <f>Data!AF30</f>
-        <v>4.6009339572529055E-2</v>
+        <v>4.5848410275579711E-2</v>
       </c>
       <c r="Z8">
         <f>Data!AG30</f>
-        <v>4.6978512293153113E-2</v>
+        <v>4.6856666322732596E-2</v>
       </c>
       <c r="AA8">
         <f>Data!AH30</f>
-        <v>4.7724486961393628E-2</v>
+        <v>4.7632723525201169E-2</v>
       </c>
       <c r="AB8">
         <f>Data!AI30</f>
-        <v>4.8293279605299791E-2</v>
+        <v>4.822445357557361E-2</v>
       </c>
       <c r="AC8">
         <f>Data!AJ30</f>
-        <v>4.8723865231847407E-2</v>
+        <v>4.8672403205753251E-2</v>
       </c>
       <c r="AD8">
         <f>Data!AK30</f>
-        <v>4.9048053913128893E-2</v>
+        <v>4.900966527614057E-2</v>
       </c>
       <c r="AE8">
         <f>Data!AL30</f>
-        <v>4.9291135840030698E-2</v>
+        <v>4.9262549842056233E-2</v>
       </c>
     </row>
   </sheetData>
@@ -63348,8 +63348,8 @@
   </sheetPr>
   <dimension ref="A1:AL95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -65586,13 +65586,13 @@
         <v>1</v>
       </c>
       <c r="D24">
-        <v>0.9</v>
+        <v>0.6</v>
       </c>
       <c r="E24" s="22">
-        <v>0.8</v>
+        <v>0.6</v>
       </c>
       <c r="F24" s="29">
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="G24" s="7" t="str">
         <f>IF(E24=F24,"n/a",IF(OR(C24="battery electric vehicle",C24="natural gas vehicle",C24="plugin hybrid vehicle"),"s-curve","linear"))</f>
@@ -65600,123 +65600,123 @@
       </c>
       <c r="I24" s="22">
         <f t="shared" ref="I24" si="3">E24</f>
-        <v>0.8</v>
+        <v>0.6</v>
       </c>
       <c r="J24">
         <f>IF($G24="s-curve",$E24+($F24-$E24)*$O$2/(1+EXP($O$3*(COUNT($I$9:J$9)+$O$4))),TREND($E24:$F24,$E$9:$F$9,J$9))</f>
-        <v>0.92312502511458017</v>
+        <v>0.6289705941446071</v>
       </c>
       <c r="K24">
         <f>IF($G24="s-curve",$E24+($F24-$E24)*$O$2/(1+EXP($O$3*(COUNT($I$9:K$9)+$O$4))),TREND($E24:$F24,$E$9:$F$9,K$9))</f>
-        <v>0.96209409032848614</v>
+        <v>0.63813978595964382</v>
       </c>
       <c r="L24">
         <f>IF($G24="s-curve",$E24+($F24-$E24)*$O$2/(1+EXP($O$3*(COUNT($I$9:L$9)+$O$4))),TREND($E24:$F24,$E$9:$F$9,L$9))</f>
-        <v>1.0117407089186079</v>
+        <v>0.64982134327496655</v>
       </c>
       <c r="M24">
         <f>IF($G24="s-curve",$E24+($F24-$E24)*$O$2/(1+EXP($O$3*(COUNT($I$9:M$9)+$O$4))),TREND($E24:$F24,$E$9:$F$9,M$9))</f>
-        <v>1.0738852142801949</v>
+        <v>0.66444357983063407</v>
       </c>
       <c r="N24">
         <f>IF($G24="s-curve",$E24+($F24-$E24)*$O$2/(1+EXP($O$3*(COUNT($I$9:N$9)+$O$4))),TREND($E24:$F24,$E$9:$F$9,N$9))</f>
-        <v>1.1499796320616105</v>
+        <v>0.68234814872037897</v>
       </c>
       <c r="O24">
         <f>IF($G24="s-curve",$E24+($F24-$E24)*$O$2/(1+EXP($O$3*(COUNT($I$9:O$9)+$O$4))),TREND($E24:$F24,$E$9:$F$9,O$9))</f>
-        <v>1.2406826713903383</v>
+        <v>0.70369004032713844</v>
       </c>
       <c r="P24">
         <f>IF($G24="s-curve",$E24+($F24-$E24)*$O$2/(1+EXP($O$3*(COUNT($I$9:P$9)+$O$4))),TREND($E24:$F24,$E$9:$F$9,P$9))</f>
-        <v>1.3453962114018321</v>
+        <v>0.72832852032984285</v>
       </c>
       <c r="Q24">
         <f>IF($G24="s-curve",$E24+($F24-$E24)*$O$2/(1+EXP($O$3*(COUNT($I$9:Q$9)+$O$4))),TREND($E24:$F24,$E$9:$F$9,Q$9))</f>
-        <v>1.4619133022863227</v>
+        <v>0.75574430642031121</v>
       </c>
       <c r="R24">
         <f>IF($G24="s-curve",$E24+($F24-$E24)*$O$2/(1+EXP($O$3*(COUNT($I$9:R$9)+$O$4))),TREND($E24:$F24,$E$9:$F$9,R$9))</f>
-        <v>1.5863692629156259</v>
+        <v>0.78502806186250018</v>
       </c>
       <c r="S24">
         <f>IF($G24="s-curve",$E24+($F24-$E24)*$O$2/(1+EXP($O$3*(COUNT($I$9:S$9)+$O$4))),TREND($E24:$F24,$E$9:$F$9,S$9))</f>
-        <v>1.7136307370843742</v>
+        <v>0.8149719381374998</v>
       </c>
       <c r="T24">
         <f>IF($G24="s-curve",$E24+($F24-$E24)*$O$2/(1+EXP($O$3*(COUNT($I$9:T$9)+$O$4))),TREND($E24:$F24,$E$9:$F$9,T$9))</f>
-        <v>1.8380866977136774</v>
+        <v>0.84425569357968877</v>
       </c>
       <c r="U24">
         <f>IF($G24="s-curve",$E24+($F24-$E24)*$O$2/(1+EXP($O$3*(COUNT($I$9:U$9)+$O$4))),TREND($E24:$F24,$E$9:$F$9,U$9))</f>
-        <v>1.954603788598168</v>
+        <v>0.87167147967015723</v>
       </c>
       <c r="V24">
         <f>IF($G24="s-curve",$E24+($F24-$E24)*$O$2/(1+EXP($O$3*(COUNT($I$9:V$9)+$O$4))),TREND($E24:$F24,$E$9:$F$9,V$9))</f>
-        <v>2.0593173286096618</v>
+        <v>0.89630995967286164</v>
       </c>
       <c r="W24">
         <f>IF($G24="s-curve",$E24+($F24-$E24)*$O$2/(1+EXP($O$3*(COUNT($I$9:W$9)+$O$4))),TREND($E24:$F24,$E$9:$F$9,W$9))</f>
-        <v>2.1500203679383896</v>
+        <v>0.91765185127962101</v>
       </c>
       <c r="X24">
         <f>IF($G24="s-curve",$E24+($F24-$E24)*$O$2/(1+EXP($O$3*(COUNT($I$9:X$9)+$O$4))),TREND($E24:$F24,$E$9:$F$9,X$9))</f>
-        <v>2.2261147857198051</v>
+        <v>0.93555642016936591</v>
       </c>
       <c r="Y24">
         <f>IF($G24="s-curve",$E24+($F24-$E24)*$O$2/(1+EXP($O$3*(COUNT($I$9:Y$9)+$O$4))),TREND($E24:$F24,$E$9:$F$9,Y$9))</f>
-        <v>2.2882592910813919</v>
+        <v>0.95017865672503343</v>
       </c>
       <c r="Z24">
         <f>IF($G24="s-curve",$E24+($F24-$E24)*$O$2/(1+EXP($O$3*(COUNT($I$9:Z$9)+$O$4))),TREND($E24:$F24,$E$9:$F$9,Z$9))</f>
-        <v>2.3379059096715142</v>
+        <v>0.96186021404035627</v>
       </c>
       <c r="AA24">
         <f>IF($G24="s-curve",$E24+($F24-$E24)*$O$2/(1+EXP($O$3*(COUNT($I$9:AA$9)+$O$4))),TREND($E24:$F24,$E$9:$F$9,AA$9))</f>
-        <v>2.3768749748854199</v>
+        <v>0.97102940585539288</v>
       </c>
       <c r="AB24">
         <f>IF($G24="s-curve",$E24+($F24-$E24)*$O$2/(1+EXP($O$3*(COUNT($I$9:AB$9)+$O$4))),TREND($E24:$F24,$E$9:$F$9,AB$9))</f>
-        <v>2.4070417607329007</v>
+        <v>0.97812747311362369</v>
       </c>
       <c r="AC24">
         <f>IF($G24="s-curve",$E24+($F24-$E24)*$O$2/(1+EXP($O$3*(COUNT($I$9:AC$9)+$O$4))),TREND($E24:$F24,$E$9:$F$9,AC$9))</f>
-        <v>2.4301448270592099</v>
+        <v>0.98356348871981403</v>
       </c>
       <c r="AD24">
         <f>IF($G24="s-curve",$E24+($F24-$E24)*$O$2/(1+EXP($O$3*(COUNT($I$9:AD$9)+$O$4))),TREND($E24:$F24,$E$9:$F$9,AD$9))</f>
-        <v>2.4476929390928484</v>
+        <v>0.98769245625714075</v>
       </c>
       <c r="AE24">
         <f>IF($G24="s-curve",$E24+($F24-$E24)*$O$2/(1+EXP($O$3*(COUNT($I$9:AE$9)+$O$4))),TREND($E24:$F24,$E$9:$F$9,AE$9))</f>
-        <v>2.4609384711529563</v>
+        <v>0.99080905203598979</v>
       </c>
       <c r="AF24">
         <f>IF($G24="s-curve",$E24+($F24-$E24)*$O$2/(1+EXP($O$3*(COUNT($I$9:AF$9)+$O$4))),TREND($E24:$F24,$E$9:$F$9,AF$9))</f>
-        <v>2.4708891433632632</v>
+        <v>0.99315038667370892</v>
       </c>
       <c r="AG24">
         <f>IF($G24="s-curve",$E24+($F24-$E24)*$O$2/(1+EXP($O$3*(COUNT($I$9:AG$9)+$O$4))),TREND($E24:$F24,$E$9:$F$9,AG$9))</f>
-        <v>2.4783380059110103</v>
+        <v>0.99490306021435537</v>
       </c>
       <c r="AH24">
         <f>IF($G24="s-curve",$E24+($F24-$E24)*$O$2/(1+EXP($O$3*(COUNT($I$9:AH$9)+$O$4))),TREND($E24:$F24,$E$9:$F$9,AH$9))</f>
-        <v>2.4838992259106916</v>
+        <v>0.99621158256722153</v>
       </c>
       <c r="AI24">
         <f>IF($G24="s-curve",$E24+($F24-$E24)*$O$2/(1+EXP($O$3*(COUNT($I$9:AI$9)+$O$4))),TREND($E24:$F24,$E$9:$F$9,AI$9))</f>
-        <v>2.4880429018365082</v>
+        <v>0.99718656513800186</v>
       </c>
       <c r="AJ24">
         <f>IF($G24="s-curve",$E24+($F24-$E24)*$O$2/(1+EXP($O$3*(COUNT($I$9:AJ$9)+$O$4))),TREND($E24:$F24,$E$9:$F$9,AJ$9))</f>
-        <v>2.4911257863209508</v>
+        <v>0.99791194972257657</v>
       </c>
       <c r="AK24">
         <f>IF($G24="s-curve",$E24+($F24-$E24)*$O$2/(1+EXP($O$3*(COUNT($I$9:AK$9)+$O$4))),TREND($E24:$F24,$E$9:$F$9,AK$9))</f>
-        <v>2.4934169141508589</v>
+        <v>0.99845103862373152</v>
       </c>
       <c r="AL24">
         <f>IF($G24="s-curve",$E24+($F24-$E24)*$O$2/(1+EXP($O$3*(COUNT($I$9:AL$9)+$O$4))),TREND($E24:$F24,$E$9:$F$9,AL$9))</f>
-        <v>2.4951182304353092</v>
+        <v>0.99885134833771982</v>
       </c>
     </row>
     <row r="25" spans="1:38" x14ac:dyDescent="0.25">
@@ -65724,12 +65724,10 @@
         <v>2</v>
       </c>
       <c r="E25" s="22">
-        <f>'SYVbT-passenger'!D3/SUM('SYVbT-passenger'!3:3)*5</f>
-        <v>2.4652000233370237E-2</v>
+        <v>0.29802375741500553</v>
       </c>
       <c r="F25" s="22">
-        <f>F32*5</f>
-        <v>0.26416899072288735</v>
+        <v>0.15850139443373243</v>
       </c>
       <c r="G25" s="7" t="str">
         <f>IF(E25=F25,"n/a",IF(OR(C25="battery electric vehicle",C25="natural gas vehicle",C25="plugin hybrid vehicle"),"s-curve","linear"))</f>
@@ -65737,123 +65735,123 @@
       </c>
       <c r="I25" s="22">
         <f t="shared" si="1"/>
-        <v>2.4652000233370237E-2</v>
+        <v>0.29802375741500553</v>
       </c>
       <c r="J25">
         <f>IF($G25="s-curve",$E25+($F25-$E25)*$I$2/(1+EXP($I$3*(COUNT($I$9:J$9)+$I$4))),TREND($E25:$F25,$E$9:$F$9,J$9))</f>
-        <v>2.8190631841939744E-2</v>
+        <v>0.29596244960239987</v>
       </c>
       <c r="K25">
         <f>IF($G25="s-curve",$E25+($F25-$E25)*$I$2/(1+EXP($I$3*(COUNT($I$9:K$9)+$I$4))),TREND($E25:$F25,$E$9:$F$9,K$9))</f>
-        <v>2.9404090553188392E-2</v>
+        <v>0.29525559107671612</v>
       </c>
       <c r="L25">
         <f>IF($G25="s-curve",$E25+($F25-$E25)*$I$2/(1+EXP($I$3*(COUNT($I$9:L$9)+$I$4))),TREND($E25:$F25,$E$9:$F$9,L$9))</f>
-        <v>3.1022432090970165E-2</v>
+        <v>0.29431288202296346</v>
       </c>
       <c r="M25">
         <f>IF($G25="s-curve",$E25+($F25-$E25)*$I$2/(1+EXP($I$3*(COUNT($I$9:M$9)+$I$4))),TREND($E25:$F25,$E$9:$F$9,M$9))</f>
-        <v>3.3171904436085045E-2</v>
+        <v>0.2930607810336332</v>
       </c>
       <c r="N25">
         <f>IF($G25="s-curve",$E25+($F25-$E25)*$I$2/(1+EXP($I$3*(COUNT($I$9:N$9)+$I$4))),TREND($E25:$F25,$E$9:$F$9,N$9))</f>
-        <v>3.6011302648198545E-2</v>
+        <v>0.29140678752282123</v>
       </c>
       <c r="O25">
         <f>IF($G25="s-curve",$E25+($F25-$E25)*$I$2/(1+EXP($I$3*(COUNT($I$9:O$9)+$I$4))),TREND($E25:$F25,$E$9:$F$9,O$9))</f>
-        <v>3.9735188957166843E-2</v>
+        <v>0.28923756597307232</v>
       </c>
       <c r="P25">
         <f>IF($G25="s-curve",$E25+($F25-$E25)*$I$2/(1+EXP($I$3*(COUNT($I$9:P$9)+$I$4))),TREND($E25:$F25,$E$9:$F$9,P$9))</f>
-        <v>4.4573274188492537E-2</v>
+        <v>0.28641930626464923</v>
       </c>
       <c r="Q25">
         <f>IF($G25="s-curve",$E25+($F25-$E25)*$I$2/(1+EXP($I$3*(COUNT($I$9:Q$9)+$I$4))),TREND($E25:$F25,$E$9:$F$9,Q$9))</f>
-        <v>5.0782542518116404E-2</v>
+        <v>0.28280231112804816</v>
       </c>
       <c r="R25">
         <f>IF($G25="s-curve",$E25+($F25-$E25)*$I$2/(1+EXP($I$3*(COUNT($I$9:R$9)+$I$4))),TREND($E25:$F25,$E$9:$F$9,R$9))</f>
-        <v>5.8627740396068245E-2</v>
+        <v>0.27823236164867954</v>
       </c>
       <c r="S25">
         <f>IF($G25="s-curve",$E25+($F25-$E25)*$I$2/(1+EXP($I$3*(COUNT($I$9:S$9)+$I$4))),TREND($E25:$F25,$E$9:$F$9,S$9))</f>
-        <v>6.834601268394247E-2</v>
+        <v>0.2725713172654462</v>
       </c>
       <c r="T25">
         <f>IF($G25="s-curve",$E25+($F25-$E25)*$I$2/(1+EXP($I$3*(COUNT($I$9:T$9)+$I$4))),TREND($E25:$F25,$E$9:$F$9,T$9))</f>
-        <v>8.0094247462594942E-2</v>
+        <v>0.26572778823718668</v>
       </c>
       <c r="U25">
         <f>IF($G25="s-curve",$E25+($F25-$E25)*$I$2/(1+EXP($I$3*(COUNT($I$9:U$9)+$I$4))),TREND($E25:$F25,$E$9:$F$9,U$9))</f>
-        <v>9.3884505464127355E-2</v>
+        <v>0.25769474900033379</v>
       </c>
       <c r="V25">
         <f>IF($G25="s-curve",$E25+($F25-$E25)*$I$2/(1+EXP($I$3*(COUNT($I$9:V$9)+$I$4))),TREND($E25:$F25,$E$9:$F$9,V$9))</f>
-        <v>0.10952333536510674</v>
+        <v>0.24858488795211589</v>
       </c>
       <c r="W25">
         <f>IF($G25="s-curve",$E25+($F25-$E25)*$I$2/(1+EXP($I$3*(COUNT($I$9:W$9)+$I$4))),TREND($E25:$F25,$E$9:$F$9,W$9))</f>
-        <v>0.12658024788693495</v>
+        <v>0.23864897177620478</v>
       </c>
       <c r="X25">
         <f>IF($G25="s-curve",$E25+($F25-$E25)*$I$2/(1+EXP($I$3*(COUNT($I$9:X$9)+$I$4))),TREND($E25:$F25,$E$9:$F$9,X$9))</f>
-        <v>0.14441049547812879</v>
+        <v>0.22826257592436899</v>
       </c>
       <c r="Y25">
         <f>IF($G25="s-curve",$E25+($F25-$E25)*$I$2/(1+EXP($I$3*(COUNT($I$9:Y$9)+$I$4))),TREND($E25:$F25,$E$9:$F$9,Y$9))</f>
-        <v>0.16224074306932265</v>
+        <v>0.21787618007253318</v>
       </c>
       <c r="Z25">
         <f>IF($G25="s-curve",$E25+($F25-$E25)*$I$2/(1+EXP($I$3*(COUNT($I$9:Z$9)+$I$4))),TREND($E25:$F25,$E$9:$F$9,Z$9))</f>
-        <v>0.17929765559115082</v>
+        <v>0.20794026389662207</v>
       </c>
       <c r="AA25">
         <f>IF($G25="s-curve",$E25+($F25-$E25)*$I$2/(1+EXP($I$3*(COUNT($I$9:AA$9)+$I$4))),TREND($E25:$F25,$E$9:$F$9,AA$9))</f>
-        <v>0.19493648549213022</v>
+        <v>0.19883040284840414</v>
       </c>
       <c r="AB25">
         <f>IF($G25="s-curve",$E25+($F25-$E25)*$I$2/(1+EXP($I$3*(COUNT($I$9:AB$9)+$I$4))),TREND($E25:$F25,$E$9:$F$9,AB$9))</f>
-        <v>0.20872674349366263</v>
+        <v>0.19079736361155128</v>
       </c>
       <c r="AC25">
         <f>IF($G25="s-curve",$E25+($F25-$E25)*$I$2/(1+EXP($I$3*(COUNT($I$9:AC$9)+$I$4))),TREND($E25:$F25,$E$9:$F$9,AC$9))</f>
-        <v>0.2204749782723151</v>
+        <v>0.18395383458329176</v>
       </c>
       <c r="AD25">
         <f>IF($G25="s-curve",$E25+($F25-$E25)*$I$2/(1+EXP($I$3*(COUNT($I$9:AD$9)+$I$4))),TREND($E25:$F25,$E$9:$F$9,AD$9))</f>
-        <v>0.23019325056018936</v>
+        <v>0.17829279020005839</v>
       </c>
       <c r="AE25">
         <f>IF($G25="s-curve",$E25+($F25-$E25)*$I$2/(1+EXP($I$3*(COUNT($I$9:AE$9)+$I$4))),TREND($E25:$F25,$E$9:$F$9,AE$9))</f>
-        <v>0.2380384484381412</v>
+        <v>0.17372284072068978</v>
       </c>
       <c r="AF25">
         <f>IF($G25="s-curve",$E25+($F25-$E25)*$I$2/(1+EXP($I$3*(COUNT($I$9:AF$9)+$I$4))),TREND($E25:$F25,$E$9:$F$9,AF$9))</f>
-        <v>0.24424771676776508</v>
+        <v>0.17010584558408873</v>
       </c>
       <c r="AG25">
         <f>IF($G25="s-curve",$E25+($F25-$E25)*$I$2/(1+EXP($I$3*(COUNT($I$9:AG$9)+$I$4))),TREND($E25:$F25,$E$9:$F$9,AG$9))</f>
-        <v>0.24908580199909075</v>
+        <v>0.16728758587566564</v>
       </c>
       <c r="AH25">
         <f>IF($G25="s-curve",$E25+($F25-$E25)*$I$2/(1+EXP($I$3*(COUNT($I$9:AH$9)+$I$4))),TREND($E25:$F25,$E$9:$F$9,AH$9))</f>
-        <v>0.25280968830805906</v>
+        <v>0.1651183643259167</v>
       </c>
       <c r="AI25">
         <f>IF($G25="s-curve",$E25+($F25-$E25)*$I$2/(1+EXP($I$3*(COUNT($I$9:AI$9)+$I$4))),TREND($E25:$F25,$E$9:$F$9,AI$9))</f>
-        <v>0.25564908652017254</v>
+        <v>0.16346437081510473</v>
       </c>
       <c r="AJ25">
         <f>IF($G25="s-curve",$E25+($F25-$E25)*$I$2/(1+EXP($I$3*(COUNT($I$9:AJ$9)+$I$4))),TREND($E25:$F25,$E$9:$F$9,AJ$9))</f>
-        <v>0.25779855886528741</v>
+        <v>0.1622122698257745</v>
       </c>
       <c r="AK25">
         <f>IF($G25="s-curve",$E25+($F25-$E25)*$I$2/(1+EXP($I$3*(COUNT($I$9:AK$9)+$I$4))),TREND($E25:$F25,$E$9:$F$9,AK$9))</f>
-        <v>0.25941690040306919</v>
+        <v>0.16126956077202181</v>
       </c>
       <c r="AL25">
         <f>IF($G25="s-curve",$E25+($F25-$E25)*$I$2/(1+EXP($I$3*(COUNT($I$9:AL$9)+$I$4))),TREND($E25:$F25,$E$9:$F$9,AL$9))</f>
-        <v>0.26063035911431781</v>
+        <v>0.16056270224633809</v>
       </c>
     </row>
     <row r="26" spans="1:38" x14ac:dyDescent="0.25">
@@ -65861,11 +65859,10 @@
         <v>3</v>
       </c>
       <c r="E26" s="22">
-        <v>2.1762390509853201E-3</v>
+        <v>0.29802375741500553</v>
       </c>
       <c r="F26" s="22">
-        <f>E26</f>
-        <v>2.1762390509853201E-3</v>
+        <v>0.29802375741500553</v>
       </c>
       <c r="G26" s="7" t="str">
         <f>IF(E26=F26,"n/a",IF(OR(C26="battery electric vehicle",C26="natural gas vehicle",C26="plugin hybrid vehicle"),"s-curve","linear"))</f>
@@ -65873,123 +65870,123 @@
       </c>
       <c r="I26" s="22">
         <f t="shared" si="1"/>
-        <v>2.1762390509853201E-3</v>
+        <v>0.29802375741500553</v>
       </c>
       <c r="J26">
         <f>IF($G26="s-curve",$E26+($F26-$E26)*$I$2/(1+EXP($I$3*(COUNT($I$9:J$9)+$I$4))),TREND($E26:$F26,$E$9:$F$9,J$9))</f>
-        <v>2.1762390509853201E-3</v>
+        <v>0.29802375741500553</v>
       </c>
       <c r="K26">
         <f>IF($G26="s-curve",$E26+($F26-$E26)*$I$2/(1+EXP($I$3*(COUNT($I$9:K$9)+$I$4))),TREND($E26:$F26,$E$9:$F$9,K$9))</f>
-        <v>2.1762390509853201E-3</v>
+        <v>0.29802375741500553</v>
       </c>
       <c r="L26">
         <f>IF($G26="s-curve",$E26+($F26-$E26)*$I$2/(1+EXP($I$3*(COUNT($I$9:L$9)+$I$4))),TREND($E26:$F26,$E$9:$F$9,L$9))</f>
-        <v>2.1762390509853201E-3</v>
+        <v>0.29802375741500553</v>
       </c>
       <c r="M26">
         <f>IF($G26="s-curve",$E26+($F26-$E26)*$I$2/(1+EXP($I$3*(COUNT($I$9:M$9)+$I$4))),TREND($E26:$F26,$E$9:$F$9,M$9))</f>
-        <v>2.1762390509853201E-3</v>
+        <v>0.29802375741500553</v>
       </c>
       <c r="N26">
         <f>IF($G26="s-curve",$E26+($F26-$E26)*$I$2/(1+EXP($I$3*(COUNT($I$9:N$9)+$I$4))),TREND($E26:$F26,$E$9:$F$9,N$9))</f>
-        <v>2.1762390509853201E-3</v>
+        <v>0.29802375741500553</v>
       </c>
       <c r="O26">
         <f>IF($G26="s-curve",$E26+($F26-$E26)*$I$2/(1+EXP($I$3*(COUNT($I$9:O$9)+$I$4))),TREND($E26:$F26,$E$9:$F$9,O$9))</f>
-        <v>2.1762390509853201E-3</v>
+        <v>0.29802375741500553</v>
       </c>
       <c r="P26">
         <f>IF($G26="s-curve",$E26+($F26-$E26)*$I$2/(1+EXP($I$3*(COUNT($I$9:P$9)+$I$4))),TREND($E26:$F26,$E$9:$F$9,P$9))</f>
-        <v>2.1762390509853201E-3</v>
+        <v>0.29802375741500553</v>
       </c>
       <c r="Q26">
         <f>IF($G26="s-curve",$E26+($F26-$E26)*$I$2/(1+EXP($I$3*(COUNT($I$9:Q$9)+$I$4))),TREND($E26:$F26,$E$9:$F$9,Q$9))</f>
-        <v>2.1762390509853201E-3</v>
+        <v>0.29802375741500553</v>
       </c>
       <c r="R26">
         <f>IF($G26="s-curve",$E26+($F26-$E26)*$I$2/(1+EXP($I$3*(COUNT($I$9:R$9)+$I$4))),TREND($E26:$F26,$E$9:$F$9,R$9))</f>
-        <v>2.1762390509853201E-3</v>
+        <v>0.29802375741500553</v>
       </c>
       <c r="S26">
         <f>IF($G26="s-curve",$E26+($F26-$E26)*$I$2/(1+EXP($I$3*(COUNT($I$9:S$9)+$I$4))),TREND($E26:$F26,$E$9:$F$9,S$9))</f>
-        <v>2.1762390509853201E-3</v>
+        <v>0.29802375741500553</v>
       </c>
       <c r="T26">
         <f>IF($G26="s-curve",$E26+($F26-$E26)*$I$2/(1+EXP($I$3*(COUNT($I$9:T$9)+$I$4))),TREND($E26:$F26,$E$9:$F$9,T$9))</f>
-        <v>2.1762390509853201E-3</v>
+        <v>0.29802375741500553</v>
       </c>
       <c r="U26">
         <f>IF($G26="s-curve",$E26+($F26-$E26)*$I$2/(1+EXP($I$3*(COUNT($I$9:U$9)+$I$4))),TREND($E26:$F26,$E$9:$F$9,U$9))</f>
-        <v>2.1762390509853201E-3</v>
+        <v>0.29802375741500553</v>
       </c>
       <c r="V26">
         <f>IF($G26="s-curve",$E26+($F26-$E26)*$I$2/(1+EXP($I$3*(COUNT($I$9:V$9)+$I$4))),TREND($E26:$F26,$E$9:$F$9,V$9))</f>
-        <v>2.1762390509853201E-3</v>
+        <v>0.29802375741500553</v>
       </c>
       <c r="W26">
         <f>IF($G26="s-curve",$E26+($F26-$E26)*$I$2/(1+EXP($I$3*(COUNT($I$9:W$9)+$I$4))),TREND($E26:$F26,$E$9:$F$9,W$9))</f>
-        <v>2.1762390509853201E-3</v>
+        <v>0.29802375741500553</v>
       </c>
       <c r="X26">
         <f>IF($G26="s-curve",$E26+($F26-$E26)*$I$2/(1+EXP($I$3*(COUNT($I$9:X$9)+$I$4))),TREND($E26:$F26,$E$9:$F$9,X$9))</f>
-        <v>2.1762390509853201E-3</v>
+        <v>0.29802375741500553</v>
       </c>
       <c r="Y26">
         <f>IF($G26="s-curve",$E26+($F26-$E26)*$I$2/(1+EXP($I$3*(COUNT($I$9:Y$9)+$I$4))),TREND($E26:$F26,$E$9:$F$9,Y$9))</f>
-        <v>2.1762390509853201E-3</v>
+        <v>0.29802375741500553</v>
       </c>
       <c r="Z26">
         <f>IF($G26="s-curve",$E26+($F26-$E26)*$I$2/(1+EXP($I$3*(COUNT($I$9:Z$9)+$I$4))),TREND($E26:$F26,$E$9:$F$9,Z$9))</f>
-        <v>2.1762390509853201E-3</v>
+        <v>0.29802375741500553</v>
       </c>
       <c r="AA26">
         <f>IF($G26="s-curve",$E26+($F26-$E26)*$I$2/(1+EXP($I$3*(COUNT($I$9:AA$9)+$I$4))),TREND($E26:$F26,$E$9:$F$9,AA$9))</f>
-        <v>2.1762390509853201E-3</v>
+        <v>0.29802375741500553</v>
       </c>
       <c r="AB26">
         <f>IF($G26="s-curve",$E26+($F26-$E26)*$I$2/(1+EXP($I$3*(COUNT($I$9:AB$9)+$I$4))),TREND($E26:$F26,$E$9:$F$9,AB$9))</f>
-        <v>2.1762390509853201E-3</v>
+        <v>0.29802375741500553</v>
       </c>
       <c r="AC26">
         <f>IF($G26="s-curve",$E26+($F26-$E26)*$I$2/(1+EXP($I$3*(COUNT($I$9:AC$9)+$I$4))),TREND($E26:$F26,$E$9:$F$9,AC$9))</f>
-        <v>2.1762390509853201E-3</v>
+        <v>0.29802375741500553</v>
       </c>
       <c r="AD26">
         <f>IF($G26="s-curve",$E26+($F26-$E26)*$I$2/(1+EXP($I$3*(COUNT($I$9:AD$9)+$I$4))),TREND($E26:$F26,$E$9:$F$9,AD$9))</f>
-        <v>2.1762390509853201E-3</v>
+        <v>0.29802375741500553</v>
       </c>
       <c r="AE26">
         <f>IF($G26="s-curve",$E26+($F26-$E26)*$I$2/(1+EXP($I$3*(COUNT($I$9:AE$9)+$I$4))),TREND($E26:$F26,$E$9:$F$9,AE$9))</f>
-        <v>2.1762390509853201E-3</v>
+        <v>0.29802375741500553</v>
       </c>
       <c r="AF26">
         <f>IF($G26="s-curve",$E26+($F26-$E26)*$I$2/(1+EXP($I$3*(COUNT($I$9:AF$9)+$I$4))),TREND($E26:$F26,$E$9:$F$9,AF$9))</f>
-        <v>2.1762390509853201E-3</v>
+        <v>0.29802375741500553</v>
       </c>
       <c r="AG26">
         <f>IF($G26="s-curve",$E26+($F26-$E26)*$I$2/(1+EXP($I$3*(COUNT($I$9:AG$9)+$I$4))),TREND($E26:$F26,$E$9:$F$9,AG$9))</f>
-        <v>2.1762390509853201E-3</v>
+        <v>0.29802375741500553</v>
       </c>
       <c r="AH26">
         <f>IF($G26="s-curve",$E26+($F26-$E26)*$I$2/(1+EXP($I$3*(COUNT($I$9:AH$9)+$I$4))),TREND($E26:$F26,$E$9:$F$9,AH$9))</f>
-        <v>2.1762390509853201E-3</v>
+        <v>0.29802375741500553</v>
       </c>
       <c r="AI26">
         <f>IF($G26="s-curve",$E26+($F26-$E26)*$I$2/(1+EXP($I$3*(COUNT($I$9:AI$9)+$I$4))),TREND($E26:$F26,$E$9:$F$9,AI$9))</f>
-        <v>2.1762390509853201E-3</v>
+        <v>0.29802375741500553</v>
       </c>
       <c r="AJ26">
         <f>IF($G26="s-curve",$E26+($F26-$E26)*$I$2/(1+EXP($I$3*(COUNT($I$9:AJ$9)+$I$4))),TREND($E26:$F26,$E$9:$F$9,AJ$9))</f>
-        <v>2.1762390509853201E-3</v>
+        <v>0.29802375741500553</v>
       </c>
       <c r="AK26">
         <f>IF($G26="s-curve",$E26+($F26-$E26)*$I$2/(1+EXP($I$3*(COUNT($I$9:AK$9)+$I$4))),TREND($E26:$F26,$E$9:$F$9,AK$9))</f>
-        <v>2.1762390509853201E-3</v>
+        <v>0.29802375741500553</v>
       </c>
       <c r="AL26">
         <f>IF($G26="s-curve",$E26+($F26-$E26)*$I$2/(1+EXP($I$3*(COUNT($I$9:AL$9)+$I$4))),TREND($E26:$F26,$E$9:$F$9,AL$9))</f>
-        <v>2.1762390509853201E-3</v>
+        <v>0.29802375741500553</v>
       </c>
     </row>
     <row r="27" spans="1:38" x14ac:dyDescent="0.25">
@@ -65997,10 +65994,10 @@
         <v>4</v>
       </c>
       <c r="E27">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="F27">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="G27" s="7" t="str">
         <f>IF(E27=F27,"n/a",IF(OR(C27="battery electric vehicle",C27="natural gas vehicle",C27="plugin hybrid vehicle"),"s-curve","linear"))</f>
@@ -66008,123 +66005,123 @@
       </c>
       <c r="I27" s="22">
         <f t="shared" si="1"/>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J27">
         <f>IF($G27="s-curve",$E27+($F27-$E27)*$I$2/(1+EXP($I$3*(COUNT($I$9:J$9)+$I$4))),TREND($E27:$F27,$E$9:$F$9,J$9))</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="K27">
         <f>IF($G27="s-curve",$E27+($F27-$E27)*$I$2/(1+EXP($I$3*(COUNT($I$9:K$9)+$I$4))),TREND($E27:$F27,$E$9:$F$9,K$9))</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="L27">
         <f>IF($G27="s-curve",$E27+($F27-$E27)*$I$2/(1+EXP($I$3*(COUNT($I$9:L$9)+$I$4))),TREND($E27:$F27,$E$9:$F$9,L$9))</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="M27">
         <f>IF($G27="s-curve",$E27+($F27-$E27)*$I$2/(1+EXP($I$3*(COUNT($I$9:M$9)+$I$4))),TREND($E27:$F27,$E$9:$F$9,M$9))</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="N27">
         <f>IF($G27="s-curve",$E27+($F27-$E27)*$I$2/(1+EXP($I$3*(COUNT($I$9:N$9)+$I$4))),TREND($E27:$F27,$E$9:$F$9,N$9))</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="O27">
         <f>IF($G27="s-curve",$E27+($F27-$E27)*$I$2/(1+EXP($I$3*(COUNT($I$9:O$9)+$I$4))),TREND($E27:$F27,$E$9:$F$9,O$9))</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="P27">
         <f>IF($G27="s-curve",$E27+($F27-$E27)*$I$2/(1+EXP($I$3*(COUNT($I$9:P$9)+$I$4))),TREND($E27:$F27,$E$9:$F$9,P$9))</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="Q27">
         <f>IF($G27="s-curve",$E27+($F27-$E27)*$I$2/(1+EXP($I$3*(COUNT($I$9:Q$9)+$I$4))),TREND($E27:$F27,$E$9:$F$9,Q$9))</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="R27">
         <f>IF($G27="s-curve",$E27+($F27-$E27)*$I$2/(1+EXP($I$3*(COUNT($I$9:R$9)+$I$4))),TREND($E27:$F27,$E$9:$F$9,R$9))</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="S27">
         <f>IF($G27="s-curve",$E27+($F27-$E27)*$I$2/(1+EXP($I$3*(COUNT($I$9:S$9)+$I$4))),TREND($E27:$F27,$E$9:$F$9,S$9))</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="T27">
         <f>IF($G27="s-curve",$E27+($F27-$E27)*$I$2/(1+EXP($I$3*(COUNT($I$9:T$9)+$I$4))),TREND($E27:$F27,$E$9:$F$9,T$9))</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="U27">
         <f>IF($G27="s-curve",$E27+($F27-$E27)*$I$2/(1+EXP($I$3*(COUNT($I$9:U$9)+$I$4))),TREND($E27:$F27,$E$9:$F$9,U$9))</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="V27">
         <f>IF($G27="s-curve",$E27+($F27-$E27)*$I$2/(1+EXP($I$3*(COUNT($I$9:V$9)+$I$4))),TREND($E27:$F27,$E$9:$F$9,V$9))</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="W27">
         <f>IF($G27="s-curve",$E27+($F27-$E27)*$I$2/(1+EXP($I$3*(COUNT($I$9:W$9)+$I$4))),TREND($E27:$F27,$E$9:$F$9,W$9))</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="X27">
         <f>IF($G27="s-curve",$E27+($F27-$E27)*$I$2/(1+EXP($I$3*(COUNT($I$9:X$9)+$I$4))),TREND($E27:$F27,$E$9:$F$9,X$9))</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="Y27">
         <f>IF($G27="s-curve",$E27+($F27-$E27)*$I$2/(1+EXP($I$3*(COUNT($I$9:Y$9)+$I$4))),TREND($E27:$F27,$E$9:$F$9,Y$9))</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="Z27">
         <f>IF($G27="s-curve",$E27+($F27-$E27)*$I$2/(1+EXP($I$3*(COUNT($I$9:Z$9)+$I$4))),TREND($E27:$F27,$E$9:$F$9,Z$9))</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="AA27">
         <f>IF($G27="s-curve",$E27+($F27-$E27)*$I$2/(1+EXP($I$3*(COUNT($I$9:AA$9)+$I$4))),TREND($E27:$F27,$E$9:$F$9,AA$9))</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="AB27">
         <f>IF($G27="s-curve",$E27+($F27-$E27)*$I$2/(1+EXP($I$3*(COUNT($I$9:AB$9)+$I$4))),TREND($E27:$F27,$E$9:$F$9,AB$9))</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="AC27">
         <f>IF($G27="s-curve",$E27+($F27-$E27)*$I$2/(1+EXP($I$3*(COUNT($I$9:AC$9)+$I$4))),TREND($E27:$F27,$E$9:$F$9,AC$9))</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="AD27">
         <f>IF($G27="s-curve",$E27+($F27-$E27)*$I$2/(1+EXP($I$3*(COUNT($I$9:AD$9)+$I$4))),TREND($E27:$F27,$E$9:$F$9,AD$9))</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="AE27">
         <f>IF($G27="s-curve",$E27+($F27-$E27)*$I$2/(1+EXP($I$3*(COUNT($I$9:AE$9)+$I$4))),TREND($E27:$F27,$E$9:$F$9,AE$9))</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="AF27">
         <f>IF($G27="s-curve",$E27+($F27-$E27)*$I$2/(1+EXP($I$3*(COUNT($I$9:AF$9)+$I$4))),TREND($E27:$F27,$E$9:$F$9,AF$9))</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="AG27">
         <f>IF($G27="s-curve",$E27+($F27-$E27)*$I$2/(1+EXP($I$3*(COUNT($I$9:AG$9)+$I$4))),TREND($E27:$F27,$E$9:$F$9,AG$9))</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="AH27">
         <f>IF($G27="s-curve",$E27+($F27-$E27)*$I$2/(1+EXP($I$3*(COUNT($I$9:AH$9)+$I$4))),TREND($E27:$F27,$E$9:$F$9,AH$9))</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="AI27">
         <f>IF($G27="s-curve",$E27+($F27-$E27)*$I$2/(1+EXP($I$3*(COUNT($I$9:AI$9)+$I$4))),TREND($E27:$F27,$E$9:$F$9,AI$9))</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="AJ27">
         <f>IF($G27="s-curve",$E27+($F27-$E27)*$I$2/(1+EXP($I$3*(COUNT($I$9:AJ$9)+$I$4))),TREND($E27:$F27,$E$9:$F$9,AJ$9))</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="AK27">
         <f>IF($G27="s-curve",$E27+($F27-$E27)*$I$2/(1+EXP($I$3*(COUNT($I$9:AK$9)+$I$4))),TREND($E27:$F27,$E$9:$F$9,AK$9))</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="AL27">
         <f>IF($G27="s-curve",$E27+($F27-$E27)*$I$2/(1+EXP($I$3*(COUNT($I$9:AL$9)+$I$4))),TREND($E27:$F27,$E$9:$F$9,AL$9))</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:38" x14ac:dyDescent="0.25">
@@ -66132,10 +66129,10 @@
         <v>5</v>
       </c>
       <c r="E28" s="22">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="F28" s="22">
-        <v>0.01</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="G28" s="7" t="str">
         <f>IF(E28=F28,"n/a",IF(OR(C28="battery electric vehicle",C28="natural gas vehicle",C28="plugin hybrid vehicle"),"s-curve","linear"))</f>
@@ -66143,123 +66140,123 @@
       </c>
       <c r="I28" s="22">
         <f t="shared" si="1"/>
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="J28">
         <f>IF($G28="s-curve",$E28+($F28-$E28)*$I$2/(1+EXP($I$3*(COUNT($I$9:J$9)+$I$4))),TREND($E28:$F28,$E$9:$F$9,J$9))</f>
-        <v>1.985225968306727E-2</v>
+        <v>8.8644190159638335E-5</v>
       </c>
       <c r="K28">
         <f>IF($G28="s-curve",$E28+($F28-$E28)*$I$2/(1+EXP($I$3*(COUNT($I$9:K$9)+$I$4))),TREND($E28:$F28,$E$9:$F$9,K$9))</f>
-        <v>1.9801596942659226E-2</v>
+        <v>1.1904183440446507E-4</v>
       </c>
       <c r="L28">
         <f>IF($G28="s-curve",$E28+($F28-$E28)*$I$2/(1+EXP($I$3*(COUNT($I$9:L$9)+$I$4))),TREND($E28:$F28,$E$9:$F$9,L$9))</f>
-        <v>1.9734030064231342E-2</v>
+        <v>1.5958196146119519E-4</v>
       </c>
       <c r="M28">
         <f>IF($G28="s-curve",$E28+($F28-$E28)*$I$2/(1+EXP($I$3*(COUNT($I$9:M$9)+$I$4))),TREND($E28:$F28,$E$9:$F$9,M$9))</f>
-        <v>1.9644288107273637E-2</v>
+        <v>2.1342713563581709E-4</v>
       </c>
       <c r="N28">
         <f>IF($G28="s-curve",$E28+($F28-$E28)*$I$2/(1+EXP($I$3*(COUNT($I$9:N$9)+$I$4))),TREND($E28:$F28,$E$9:$F$9,N$9))</f>
-        <v>1.9525741268224331E-2</v>
+        <v>2.845552390654007E-4</v>
       </c>
       <c r="O28">
         <f>IF($G28="s-curve",$E28+($F28-$E28)*$I$2/(1+EXP($I$3*(COUNT($I$9:O$9)+$I$4))),TREND($E28:$F28,$E$9:$F$9,O$9))</f>
-        <v>1.9370266439430035E-2</v>
+        <v>3.7784013634197905E-4</v>
       </c>
       <c r="P28">
         <f>IF($G28="s-curve",$E28+($F28-$E28)*$I$2/(1+EXP($I$3*(COUNT($I$9:P$9)+$I$4))),TREND($E28:$F28,$E$9:$F$9,P$9))</f>
-        <v>1.9168273035060777E-2</v>
+        <v>4.9903617896353422E-4</v>
       </c>
       <c r="Q28">
         <f>IF($G28="s-curve",$E28+($F28-$E28)*$I$2/(1+EXP($I$3*(COUNT($I$9:Q$9)+$I$4))),TREND($E28:$F28,$E$9:$F$9,Q$9))</f>
-        <v>1.8909031788043873E-2</v>
+        <v>6.5458092717367755E-4</v>
       </c>
       <c r="R28">
         <f>IF($G28="s-curve",$E28+($F28-$E28)*$I$2/(1+EXP($I$3*(COUNT($I$9:R$9)+$I$4))),TREND($E28:$F28,$E$9:$F$9,R$9))</f>
-        <v>1.8581489350995122E-2</v>
+        <v>8.5110638940292692E-4</v>
       </c>
       <c r="S28">
         <f>IF($G28="s-curve",$E28+($F28-$E28)*$I$2/(1+EXP($I$3*(COUNT($I$9:S$9)+$I$4))),TREND($E28:$F28,$E$9:$F$9,S$9))</f>
-        <v>1.8175744761936438E-2</v>
+        <v>1.0945531428381381E-3</v>
       </c>
       <c r="T28">
         <f>IF($G28="s-curve",$E28+($F28-$E28)*$I$2/(1+EXP($I$3*(COUNT($I$9:T$9)+$I$4))),TREND($E28:$F28,$E$9:$F$9,T$9))</f>
-        <v>1.7685247834990175E-2</v>
+        <v>1.3888512990058942E-3</v>
       </c>
       <c r="U28">
         <f>IF($G28="s-curve",$E28+($F28-$E28)*$I$2/(1+EXP($I$3*(COUNT($I$9:U$9)+$I$4))),TREND($E28:$F28,$E$9:$F$9,U$9))</f>
-        <v>1.7109495026250039E-2</v>
+        <v>1.7343029842499763E-3</v>
       </c>
       <c r="V28">
         <f>IF($G28="s-curve",$E28+($F28-$E28)*$I$2/(1+EXP($I$3*(COUNT($I$9:V$9)+$I$4))),TREND($E28:$F28,$E$9:$F$9,V$9))</f>
-        <v>1.6456563062257956E-2</v>
+        <v>2.1260621626452273E-3</v>
       </c>
       <c r="W28">
         <f>IF($G28="s-curve",$E28+($F28-$E28)*$I$2/(1+EXP($I$3*(COUNT($I$9:W$9)+$I$4))),TREND($E28:$F28,$E$9:$F$9,W$9))</f>
-        <v>1.5744425168116589E-2</v>
+        <v>2.553344899130046E-3</v>
       </c>
       <c r="X28">
         <f>IF($G28="s-curve",$E28+($F28-$E28)*$I$2/(1+EXP($I$3*(COUNT($I$9:X$9)+$I$4))),TREND($E28:$F28,$E$9:$F$9,X$9))</f>
-        <v>1.4999999999999999E-2</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="Y28">
         <f>IF($G28="s-curve",$E28+($F28-$E28)*$I$2/(1+EXP($I$3*(COUNT($I$9:Y$9)+$I$4))),TREND($E28:$F28,$E$9:$F$9,Y$9))</f>
-        <v>1.4255574831883409E-2</v>
+        <v>3.4466551008699542E-3</v>
       </c>
       <c r="Z28">
         <f>IF($G28="s-curve",$E28+($F28-$E28)*$I$2/(1+EXP($I$3*(COUNT($I$9:Z$9)+$I$4))),TREND($E28:$F28,$E$9:$F$9,Z$9))</f>
-        <v>1.3543436937742046E-2</v>
+        <v>3.8739378373547728E-3</v>
       </c>
       <c r="AA28">
         <f>IF($G28="s-curve",$E28+($F28-$E28)*$I$2/(1+EXP($I$3*(COUNT($I$9:AA$9)+$I$4))),TREND($E28:$F28,$E$9:$F$9,AA$9))</f>
-        <v>1.2890504973749961E-2</v>
+        <v>4.2656970157500234E-3</v>
       </c>
       <c r="AB28">
         <f>IF($G28="s-curve",$E28+($F28-$E28)*$I$2/(1+EXP($I$3*(COUNT($I$9:AB$9)+$I$4))),TREND($E28:$F28,$E$9:$F$9,AB$9))</f>
-        <v>1.2314752165009824E-2</v>
+        <v>4.6111487009941055E-3</v>
       </c>
       <c r="AC28">
         <f>IF($G28="s-curve",$E28+($F28-$E28)*$I$2/(1+EXP($I$3*(COUNT($I$9:AC$9)+$I$4))),TREND($E28:$F28,$E$9:$F$9,AC$9))</f>
-        <v>1.1824255238063564E-2</v>
+        <v>4.9054468571618614E-3</v>
       </c>
       <c r="AD28">
         <f>IF($G28="s-curve",$E28+($F28-$E28)*$I$2/(1+EXP($I$3*(COUNT($I$9:AD$9)+$I$4))),TREND($E28:$F28,$E$9:$F$9,AD$9))</f>
-        <v>1.1418510649004877E-2</v>
+        <v>5.1488936105970736E-3</v>
       </c>
       <c r="AE28">
         <f>IF($G28="s-curve",$E28+($F28-$E28)*$I$2/(1+EXP($I$3*(COUNT($I$9:AE$9)+$I$4))),TREND($E28:$F28,$E$9:$F$9,AE$9))</f>
-        <v>1.1090968211956129E-2</v>
+        <v>5.3454190728263228E-3</v>
       </c>
       <c r="AF28">
         <f>IF($G28="s-curve",$E28+($F28-$E28)*$I$2/(1+EXP($I$3*(COUNT($I$9:AF$9)+$I$4))),TREND($E28:$F28,$E$9:$F$9,AF$9))</f>
-        <v>1.0831726964939224E-2</v>
+        <v>5.5009638210364665E-3</v>
       </c>
       <c r="AG28">
         <f>IF($G28="s-curve",$E28+($F28-$E28)*$I$2/(1+EXP($I$3*(COUNT($I$9:AG$9)+$I$4))),TREND($E28:$F28,$E$9:$F$9,AG$9))</f>
-        <v>1.0629733560569964E-2</v>
+        <v>5.6221598636580217E-3</v>
       </c>
       <c r="AH28">
         <f>IF($G28="s-curve",$E28+($F28-$E28)*$I$2/(1+EXP($I$3*(COUNT($I$9:AH$9)+$I$4))),TREND($E28:$F28,$E$9:$F$9,AH$9))</f>
-        <v>1.0474258731775666E-2</v>
+        <v>5.7154447609346001E-3</v>
       </c>
       <c r="AI28">
         <f>IF($G28="s-curve",$E28+($F28-$E28)*$I$2/(1+EXP($I$3*(COUNT($I$9:AI$9)+$I$4))),TREND($E28:$F28,$E$9:$F$9,AI$9))</f>
-        <v>1.0355711892726362E-2</v>
+        <v>5.7865728643641829E-3</v>
       </c>
       <c r="AJ28">
         <f>IF($G28="s-curve",$E28+($F28-$E28)*$I$2/(1+EXP($I$3*(COUNT($I$9:AJ$9)+$I$4))),TREND($E28:$F28,$E$9:$F$9,AJ$9))</f>
-        <v>1.026596993576866E-2</v>
+        <v>5.840418038538805E-3</v>
       </c>
       <c r="AK28">
         <f>IF($G28="s-curve",$E28+($F28-$E28)*$I$2/(1+EXP($I$3*(COUNT($I$9:AK$9)+$I$4))),TREND($E28:$F28,$E$9:$F$9,AK$9))</f>
-        <v>1.0198403057340774E-2</v>
+        <v>5.880958165595535E-3</v>
       </c>
       <c r="AL28">
         <f>IF($G28="s-curve",$E28+($F28-$E28)*$I$2/(1+EXP($I$3*(COUNT($I$9:AL$9)+$I$4))),TREND($E28:$F28,$E$9:$F$9,AL$9))</f>
-        <v>1.0147740316932731E-2</v>
+        <v>5.9113558098403615E-3</v>
       </c>
     </row>
     <row r="29" spans="1:38" x14ac:dyDescent="0.25">
@@ -66267,11 +66264,10 @@
         <v>124</v>
       </c>
       <c r="E29" s="22">
-        <f>'SYVbT-passenger'!G3/SUM('SYVbT-passenger'!3:3)*5</f>
-        <v>1.1960398418308864E-2</v>
+        <v>2.1496445375763083E-2</v>
       </c>
       <c r="F29" s="22">
-        <v>1.4999999999999999E-2</v>
+        <v>0.53425472287359943</v>
       </c>
       <c r="G29" s="7" t="str">
         <f>IF(E29=F29,"n/a",IF(OR(C29="battery electric vehicle",C29="natural gas vehicle",C29="plugin hybrid vehicle",C29="hydrogen vehicle"),"s-curve","linear"))</f>
@@ -66279,123 +66275,123 @@
       </c>
       <c r="I29" s="22">
         <f t="shared" si="1"/>
-        <v>1.1960398418308864E-2</v>
+        <v>2.1496445375763083E-2</v>
       </c>
       <c r="J29">
         <f>IF($G29="s-curve",$E29+($F29-$E29)*$I$2/(1+EXP($I$3*(COUNT($I$9:J$9)+$I$4))),TREND($E29:$F29,$E$9:$F$9,J$9))</f>
-        <v>1.1960398418308871E-2</v>
+        <v>2.1496445375760231E-2</v>
       </c>
       <c r="K29">
         <f>IF($G29="s-curve",$E29+($F29-$E29)*$I$2/(1+EXP($I$3*(COUNT($I$9:K$9)+$I$4))),TREND($E29:$F29,$E$9:$F$9,K$9))</f>
-        <v>1.2068955617654975E-2</v>
+        <v>3.9809241000682505E-2</v>
       </c>
       <c r="L29">
         <f>IF($G29="s-curve",$E29+($F29-$E29)*$I$2/(1+EXP($I$3*(COUNT($I$9:L$9)+$I$4))),TREND($E29:$F29,$E$9:$F$9,L$9))</f>
-        <v>1.2177512817001079E-2</v>
+        <v>5.8122036625604778E-2</v>
       </c>
       <c r="M29">
         <f>IF($G29="s-curve",$E29+($F29-$E29)*$I$2/(1+EXP($I$3*(COUNT($I$9:M$9)+$I$4))),TREND($E29:$F29,$E$9:$F$9,M$9))</f>
-        <v>1.2286070016347211E-2</v>
+        <v>7.6434832250534157E-2</v>
       </c>
       <c r="N29">
         <f>IF($G29="s-curve",$E29+($F29-$E29)*$I$2/(1+EXP($I$3*(COUNT($I$9:N$9)+$I$4))),TREND($E29:$F29,$E$9:$F$9,N$9))</f>
-        <v>1.2394627215693316E-2</v>
+        <v>9.4747627875456431E-2</v>
       </c>
       <c r="O29">
         <f>IF($G29="s-curve",$E29+($F29-$E29)*$I$2/(1+EXP($I$3*(COUNT($I$9:O$9)+$I$4))),TREND($E29:$F29,$E$9:$F$9,O$9))</f>
-        <v>1.250318441503942E-2</v>
+        <v>0.1130604235003787</v>
       </c>
       <c r="P29">
         <f>IF($G29="s-curve",$E29+($F29-$E29)*$I$2/(1+EXP($I$3*(COUNT($I$9:P$9)+$I$4))),TREND($E29:$F29,$E$9:$F$9,P$9))</f>
-        <v>1.2611741614385524E-2</v>
+        <v>0.13137321912530098</v>
       </c>
       <c r="Q29">
         <f>IF($G29="s-curve",$E29+($F29-$E29)*$I$2/(1+EXP($I$3*(COUNT($I$9:Q$9)+$I$4))),TREND($E29:$F29,$E$9:$F$9,Q$9))</f>
-        <v>1.2720298813731656E-2</v>
+        <v>0.14968601475022325</v>
       </c>
       <c r="R29">
         <f>IF($G29="s-curve",$E29+($F29-$E29)*$I$2/(1+EXP($I$3*(COUNT($I$9:R$9)+$I$4))),TREND($E29:$F29,$E$9:$F$9,R$9))</f>
-        <v>1.2828856013077761E-2</v>
+        <v>0.16799881037514552</v>
       </c>
       <c r="S29">
         <f>IF($G29="s-curve",$E29+($F29-$E29)*$I$2/(1+EXP($I$3*(COUNT($I$9:S$9)+$I$4))),TREND($E29:$F29,$E$9:$F$9,S$9))</f>
-        <v>1.2937413212423865E-2</v>
+        <v>0.1863116060000678</v>
       </c>
       <c r="T29">
         <f>IF($G29="s-curve",$E29+($F29-$E29)*$I$2/(1+EXP($I$3*(COUNT($I$9:T$9)+$I$4))),TREND($E29:$F29,$E$9:$F$9,T$9))</f>
-        <v>1.3045970411769997E-2</v>
+        <v>0.20462440162499007</v>
       </c>
       <c r="U29">
         <f>IF($G29="s-curve",$E29+($F29-$E29)*$I$2/(1+EXP($I$3*(COUNT($I$9:U$9)+$I$4))),TREND($E29:$F29,$E$9:$F$9,U$9))</f>
-        <v>1.3154527611116101E-2</v>
+        <v>0.22293719724991234</v>
       </c>
       <c r="V29">
         <f>IF($G29="s-curve",$E29+($F29-$E29)*$I$2/(1+EXP($I$3*(COUNT($I$9:V$9)+$I$4))),TREND($E29:$F29,$E$9:$F$9,V$9))</f>
-        <v>1.3263084810462206E-2</v>
+        <v>0.24124999287483462</v>
       </c>
       <c r="W29">
         <f>IF($G29="s-curve",$E29+($F29-$E29)*$I$2/(1+EXP($I$3*(COUNT($I$9:W$9)+$I$4))),TREND($E29:$F29,$E$9:$F$9,W$9))</f>
-        <v>1.337164200980831E-2</v>
+        <v>0.25956278849975689</v>
       </c>
       <c r="X29">
         <f>IF($G29="s-curve",$E29+($F29-$E29)*$I$2/(1+EXP($I$3*(COUNT($I$9:X$9)+$I$4))),TREND($E29:$F29,$E$9:$F$9,X$9))</f>
-        <v>1.3480199209154442E-2</v>
+        <v>0.27787558412467916</v>
       </c>
       <c r="Y29">
         <f>IF($G29="s-curve",$E29+($F29-$E29)*$I$2/(1+EXP($I$3*(COUNT($I$9:Y$9)+$I$4))),TREND($E29:$F29,$E$9:$F$9,Y$9))</f>
-        <v>1.3588756408500546E-2</v>
+        <v>0.29618837974960144</v>
       </c>
       <c r="Z29">
         <f>IF($G29="s-curve",$E29+($F29-$E29)*$I$2/(1+EXP($I$3*(COUNT($I$9:Z$9)+$I$4))),TREND($E29:$F29,$E$9:$F$9,Z$9))</f>
-        <v>1.3697313607846651E-2</v>
+        <v>0.31450117537452371</v>
       </c>
       <c r="AA29">
         <f>IF($G29="s-curve",$E29+($F29-$E29)*$I$2/(1+EXP($I$3*(COUNT($I$9:AA$9)+$I$4))),TREND($E29:$F29,$E$9:$F$9,AA$9))</f>
-        <v>1.3805870807192783E-2</v>
+        <v>0.33281397099944598</v>
       </c>
       <c r="AB29">
         <f>IF($G29="s-curve",$E29+($F29-$E29)*$I$2/(1+EXP($I$3*(COUNT($I$9:AB$9)+$I$4))),TREND($E29:$F29,$E$9:$F$9,AB$9))</f>
-        <v>1.3914428006538887E-2</v>
+        <v>0.35112676662436826</v>
       </c>
       <c r="AC29">
         <f>IF($G29="s-curve",$E29+($F29-$E29)*$I$2/(1+EXP($I$3*(COUNT($I$9:AC$9)+$I$4))),TREND($E29:$F29,$E$9:$F$9,AC$9))</f>
-        <v>1.4022985205884991E-2</v>
+        <v>0.36943956224929764</v>
       </c>
       <c r="AD29">
         <f>IF($G29="s-curve",$E29+($F29-$E29)*$I$2/(1+EXP($I$3*(COUNT($I$9:AD$9)+$I$4))),TREND($E29:$F29,$E$9:$F$9,AD$9))</f>
-        <v>1.4131542405231096E-2</v>
+        <v>0.38775235787421991</v>
       </c>
       <c r="AE29">
         <f>IF($G29="s-curve",$E29+($F29-$E29)*$I$2/(1+EXP($I$3*(COUNT($I$9:AE$9)+$I$4))),TREND($E29:$F29,$E$9:$F$9,AE$9))</f>
-        <v>1.4240099604577228E-2</v>
+        <v>0.40606515349914218</v>
       </c>
       <c r="AF29">
         <f>IF($G29="s-curve",$E29+($F29-$E29)*$I$2/(1+EXP($I$3*(COUNT($I$9:AF$9)+$I$4))),TREND($E29:$F29,$E$9:$F$9,AF$9))</f>
-        <v>1.4348656803923332E-2</v>
+        <v>0.42437794912406446</v>
       </c>
       <c r="AG29">
         <f>IF($G29="s-curve",$E29+($F29-$E29)*$I$2/(1+EXP($I$3*(COUNT($I$9:AG$9)+$I$4))),TREND($E29:$F29,$E$9:$F$9,AG$9))</f>
-        <v>1.4457214003269436E-2</v>
+        <v>0.44269074474898673</v>
       </c>
       <c r="AH29">
         <f>IF($G29="s-curve",$E29+($F29-$E29)*$I$2/(1+EXP($I$3*(COUNT($I$9:AH$9)+$I$4))),TREND($E29:$F29,$E$9:$F$9,AH$9))</f>
-        <v>1.4565771202615541E-2</v>
+        <v>0.461003540373909</v>
       </c>
       <c r="AI29">
         <f>IF($G29="s-curve",$E29+($F29-$E29)*$I$2/(1+EXP($I$3*(COUNT($I$9:AI$9)+$I$4))),TREND($E29:$F29,$E$9:$F$9,AI$9))</f>
-        <v>1.4674328401961673E-2</v>
+        <v>0.47931633599883128</v>
       </c>
       <c r="AJ29">
         <f>IF($G29="s-curve",$E29+($F29-$E29)*$I$2/(1+EXP($I$3*(COUNT($I$9:AJ$9)+$I$4))),TREND($E29:$F29,$E$9:$F$9,AJ$9))</f>
-        <v>1.4782885601307777E-2</v>
+        <v>0.49762913162375355</v>
       </c>
       <c r="AK29">
         <f>IF($G29="s-curve",$E29+($F29-$E29)*$I$2/(1+EXP($I$3*(COUNT($I$9:AK$9)+$I$4))),TREND($E29:$F29,$E$9:$F$9,AK$9))</f>
-        <v>1.4891442800653881E-2</v>
+        <v>0.51594192724867582</v>
       </c>
       <c r="AL29">
         <f>IF($G29="s-curve",$E29+($F29-$E29)*$I$2/(1+EXP($I$3*(COUNT($I$9:AL$9)+$I$4))),TREND($E29:$F29,$E$9:$F$9,AL$9))</f>
-        <v>1.5000000000000013E-2</v>
+        <v>0.5342547228735981</v>
       </c>
     </row>
     <row r="30" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -66406,8 +66402,7 @@
       </c>
       <c r="D30" s="23"/>
       <c r="E30" s="26">
-        <f>'SYVbT-passenger'!H3/SUM('SYVbT-passenger'!3:3)+0.002</f>
-        <v>2.0195858052701565E-3</v>
+        <v>8.470448323552864E-5</v>
       </c>
       <c r="F30" s="26">
         <v>0.05</v>
@@ -66418,123 +66413,123 @@
       </c>
       <c r="I30" s="22">
         <f t="shared" si="1"/>
-        <v>2.0195858052701565E-3</v>
+        <v>8.470448323552864E-5</v>
       </c>
       <c r="J30">
         <f>IF($G30="s-curve",$E30+($F30-$E30)*$I$2/(1+EXP($I$3*(COUNT($I$9:J$9)+$I$4))),TREND($E30:$F30,$E$9:$F$9,J$9))</f>
-        <v>2.7284499652394639E-3</v>
+        <v>8.2215464117929744E-4</v>
       </c>
       <c r="K30">
         <f>IF($G30="s-curve",$E30+($F30-$E30)*$I$2/(1+EXP($I$3*(COUNT($I$9:K$9)+$I$4))),TREND($E30:$F30,$E$9:$F$9,K$9))</f>
-        <v>2.9715318921412692E-3</v>
+        <v>1.0750392070949643E-3</v>
       </c>
       <c r="L30">
         <f>IF($G30="s-curve",$E30+($F30-$E30)*$I$2/(1+EXP($I$3*(COUNT($I$9:L$9)+$I$4))),TREND($E30:$F30,$E$9:$F$9,L$9))</f>
-        <v>3.2957205734227501E-3</v>
+        <v>1.4123012774822749E-3</v>
       </c>
       <c r="M30">
         <f>IF($G30="s-curve",$E30+($F30-$E30)*$I$2/(1+EXP($I$3*(COUNT($I$9:M$9)+$I$4))),TREND($E30:$F30,$E$9:$F$9,M$9))</f>
-        <v>3.7263061999703714E-3</v>
+        <v>1.860250907661926E-3</v>
       </c>
       <c r="N30">
         <f>IF($G30="s-curve",$E30+($F30-$E30)*$I$2/(1+EXP($I$3*(COUNT($I$9:N$9)+$I$4))),TREND($E30:$F30,$E$9:$F$9,N$9))</f>
-        <v>4.2950988438765388E-3</v>
+        <v>2.4519809580343683E-3</v>
       </c>
       <c r="O30">
         <f>IF($G30="s-curve",$E30+($F30-$E30)*$I$2/(1+EXP($I$3*(COUNT($I$9:O$9)+$I$4))),TREND($E30:$F30,$E$9:$F$9,O$9))</f>
-        <v>5.0410735121170485E-3</v>
+        <v>3.2280381605029394E-3</v>
       </c>
       <c r="P30">
         <f>IF($G30="s-curve",$E30+($F30-$E30)*$I$2/(1+EXP($I$3*(COUNT($I$9:P$9)+$I$4))),TREND($E30:$F30,$E$9:$F$9,P$9))</f>
-        <v>6.010246232741108E-3</v>
+        <v>4.2362942076558247E-3</v>
       </c>
       <c r="Q30">
         <f>IF($G30="s-curve",$E30+($F30-$E30)*$I$2/(1+EXP($I$3*(COUNT($I$9:Q$9)+$I$4))),TREND($E30:$F30,$E$9:$F$9,Q$9))</f>
-        <v>7.2540964735640472E-3</v>
+        <v>5.530304553154162E-3</v>
       </c>
       <c r="R30">
         <f>IF($G30="s-curve",$E30+($F30-$E30)*$I$2/(1+EXP($I$3*(COUNT($I$9:R$9)+$I$4))),TREND($E30:$F30,$E$9:$F$9,R$9))</f>
-        <v>8.8256586531590669E-3</v>
+        <v>7.1652423071111148E-3</v>
       </c>
       <c r="S30">
         <f>IF($G30="s-curve",$E30+($F30-$E30)*$I$2/(1+EXP($I$3*(COUNT($I$9:S$9)+$I$4))),TREND($E30:$F30,$E$9:$F$9,S$9))</f>
-        <v>1.0772437997189686E-2</v>
+        <v>9.1905284138303605E-3</v>
       </c>
       <c r="T30">
         <f>IF($G30="s-curve",$E30+($F30-$E30)*$I$2/(1+EXP($I$3*(COUNT($I$9:T$9)+$I$4))),TREND($E30:$F30,$E$9:$F$9,T$9))</f>
-        <v>1.3125862568802056E-2</v>
+        <v>1.1638858319689102E-2</v>
       </c>
       <c r="U30">
         <f>IF($G30="s-curve",$E30+($F30-$E30)*$I$2/(1+EXP($I$3*(COUNT($I$9:U$9)+$I$4))),TREND($E30:$F30,$E$9:$F$9,U$9))</f>
-        <v>1.5888348392515139E-2</v>
+        <v>1.4512745478976212E-2</v>
       </c>
       <c r="V30">
         <f>IF($G30="s-curve",$E30+($F30-$E30)*$I$2/(1+EXP($I$3*(COUNT($I$9:V$9)+$I$4))),TREND($E30:$F30,$E$9:$F$9,V$9))</f>
-        <v>1.9021142999847009E-2</v>
+        <v>1.7771874672476845E-2</v>
       </c>
       <c r="W30">
         <f>IF($G30="s-curve",$E30+($F30-$E30)*$I$2/(1+EXP($I$3*(COUNT($I$9:W$9)+$I$4))),TREND($E30:$F30,$E$9:$F$9,W$9))</f>
-        <v>2.2438010112313542E-2</v>
+        <v>2.1326532015952099E-2</v>
       </c>
       <c r="X30">
         <f>IF($G30="s-curve",$E30+($F30-$E30)*$I$2/(1+EXP($I$3*(COUNT($I$9:X$9)+$I$4))),TREND($E30:$F30,$E$9:$F$9,X$9))</f>
-        <v>2.6009792902635082E-2</v>
+        <v>2.5042352241617768E-2</v>
       </c>
       <c r="Y30">
         <f>IF($G30="s-curve",$E30+($F30-$E30)*$I$2/(1+EXP($I$3*(COUNT($I$9:Y$9)+$I$4))),TREND($E30:$F30,$E$9:$F$9,Y$9))</f>
-        <v>2.9581575692956621E-2</v>
+        <v>2.8758172467283436E-2</v>
       </c>
       <c r="Z30">
         <f>IF($G30="s-curve",$E30+($F30-$E30)*$I$2/(1+EXP($I$3*(COUNT($I$9:Z$9)+$I$4))),TREND($E30:$F30,$E$9:$F$9,Z$9))</f>
-        <v>3.2998442805423155E-2</v>
+        <v>3.2312829810758684E-2</v>
       </c>
       <c r="AA30">
         <f>IF($G30="s-curve",$E30+($F30-$E30)*$I$2/(1+EXP($I$3*(COUNT($I$9:AA$9)+$I$4))),TREND($E30:$F30,$E$9:$F$9,AA$9))</f>
-        <v>3.6131237412755014E-2</v>
+        <v>3.5571959004259315E-2</v>
       </c>
       <c r="AB30">
         <f>IF($G30="s-curve",$E30+($F30-$E30)*$I$2/(1+EXP($I$3*(COUNT($I$9:AB$9)+$I$4))),TREND($E30:$F30,$E$9:$F$9,AB$9))</f>
-        <v>3.88937232364681E-2</v>
+        <v>3.8445846163546425E-2</v>
       </c>
       <c r="AC30">
         <f>IF($G30="s-curve",$E30+($F30-$E30)*$I$2/(1+EXP($I$3*(COUNT($I$9:AC$9)+$I$4))),TREND($E30:$F30,$E$9:$F$9,AC$9))</f>
-        <v>4.1247147808080475E-2</v>
+        <v>4.0894176069405173E-2</v>
       </c>
       <c r="AD30">
         <f>IF($G30="s-curve",$E30+($F30-$E30)*$I$2/(1+EXP($I$3*(COUNT($I$9:AD$9)+$I$4))),TREND($E30:$F30,$E$9:$F$9,AD$9))</f>
-        <v>4.3193927152111095E-2</v>
+        <v>4.2919462176124419E-2</v>
       </c>
       <c r="AE30">
         <f>IF($G30="s-curve",$E30+($F30-$E30)*$I$2/(1+EXP($I$3*(COUNT($I$9:AE$9)+$I$4))),TREND($E30:$F30,$E$9:$F$9,AE$9))</f>
-        <v>4.4765489331706113E-2</v>
+        <v>4.4554399930081368E-2</v>
       </c>
       <c r="AF30">
         <f>IF($G30="s-curve",$E30+($F30-$E30)*$I$2/(1+EXP($I$3*(COUNT($I$9:AF$9)+$I$4))),TREND($E30:$F30,$E$9:$F$9,AF$9))</f>
-        <v>4.6009339572529055E-2</v>
+        <v>4.5848410275579711E-2</v>
       </c>
       <c r="AG30">
         <f>IF($G30="s-curve",$E30+($F30-$E30)*$I$2/(1+EXP($I$3*(COUNT($I$9:AG$9)+$I$4))),TREND($E30:$F30,$E$9:$F$9,AG$9))</f>
-        <v>4.6978512293153113E-2</v>
+        <v>4.6856666322732596E-2</v>
       </c>
       <c r="AH30">
         <f>IF($G30="s-curve",$E30+($F30-$E30)*$I$2/(1+EXP($I$3*(COUNT($I$9:AH$9)+$I$4))),TREND($E30:$F30,$E$9:$F$9,AH$9))</f>
-        <v>4.7724486961393628E-2</v>
+        <v>4.7632723525201169E-2</v>
       </c>
       <c r="AI30">
         <f>IF($G30="s-curve",$E30+($F30-$E30)*$I$2/(1+EXP($I$3*(COUNT($I$9:AI$9)+$I$4))),TREND($E30:$F30,$E$9:$F$9,AI$9))</f>
-        <v>4.8293279605299791E-2</v>
+        <v>4.822445357557361E-2</v>
       </c>
       <c r="AJ30">
         <f>IF($G30="s-curve",$E30+($F30-$E30)*$I$2/(1+EXP($I$3*(COUNT($I$9:AJ$9)+$I$4))),TREND($E30:$F30,$E$9:$F$9,AJ$9))</f>
-        <v>4.8723865231847407E-2</v>
+        <v>4.8672403205753251E-2</v>
       </c>
       <c r="AK30">
         <f>IF($G30="s-curve",$E30+($F30-$E30)*$I$2/(1+EXP($I$3*(COUNT($I$9:AK$9)+$I$4))),TREND($E30:$F30,$E$9:$F$9,AK$9))</f>
-        <v>4.9048053913128893E-2</v>
+        <v>4.900966527614057E-2</v>
       </c>
       <c r="AL30">
         <f>IF($G30="s-curve",$E30+($F30-$E30)*$I$2/(1+EXP($I$3*(COUNT($I$9:AL$9)+$I$4))),TREND($E30:$F30,$E$9:$F$9,AL$9))</f>
-        <v>4.9291135840030698E-2</v>
+        <v>4.9262549842056233E-2</v>
       </c>
     </row>
     <row r="31" spans="1:38" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updates TTS to limit PHEV sales through 2035; update VTQaZ to allow hydrogen FCVs to qualify as zero emission
</commit_message>
<xml_diff>
--- a/InputData/trans/TTS/Transportation Technology Shareweights.xlsx
+++ b/InputData/trans/TTS/Transportation Technology Shareweights.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dobrien\Dropbox (Energy Innovation)\Desktop\Models\E.U. Models\eps-eu\InputData\trans\TTS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Modeling\EPS\EU\eps-eu\InputData\trans\TTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{676525AD-CC88-4B9E-AB3D-EFB071118F81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8E0C601-6A9C-43D6-83E1-44E669E6CDB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60765" yWindow="2805" windowWidth="21600" windowHeight="12525" firstSheet="7" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32280" yWindow="210" windowWidth="22995" windowHeight="15075" firstSheet="7" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -7095,16 +7095,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>437356</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>260464</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>145144</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>513557</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>145257</xdr:rowOff>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>336665</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>114869</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8613,119 +8613,119 @@
       </c>
       <c r="C6">
         <f>Data!J14</f>
-        <v>0.17534926987653121</v>
+        <v>0.15724264853615177</v>
       </c>
       <c r="D6">
         <f>Data!K14</f>
-        <v>0.18337231271468832</v>
+        <v>0.15953494648991096</v>
       </c>
       <c r="E6">
         <f>Data!L14</f>
-        <v>0.19359367536559574</v>
+        <v>0.16245533581874164</v>
       </c>
       <c r="F6">
         <f>Data!M14</f>
-        <v>0.20638813235180481</v>
+        <v>0.16611089495765852</v>
       </c>
       <c r="G6">
         <f>Data!N14</f>
-        <v>0.22205463013033155</v>
+        <v>0.17058703718009474</v>
       </c>
       <c r="H6">
         <f>Data!O14</f>
-        <v>0.24072878528624608</v>
+        <v>0.17592251008178461</v>
       </c>
       <c r="I6">
         <f>Data!P14</f>
-        <v>0.26228745528861241</v>
+        <v>0.18208213008246071</v>
       </c>
       <c r="J6">
         <f>Data!Q14</f>
-        <v>0.28627626811777229</v>
+        <v>0.1889360766050778</v>
       </c>
       <c r="K6">
         <f>Data!R14</f>
-        <v>0.31189955412968762</v>
+        <v>0.19625701546562505</v>
       </c>
       <c r="L6">
         <f>Data!S14</f>
-        <v>0.33810044587031229</v>
+        <v>0.20374298453437495</v>
       </c>
       <c r="M6">
         <f>Data!T14</f>
-        <v>0.36372373188222767</v>
+        <v>0.21106392339492219</v>
       </c>
       <c r="N6">
         <f>Data!U14</f>
-        <v>0.3877125447113875</v>
+        <v>0.21791786991753931</v>
       </c>
       <c r="O6">
         <f>Data!V14</f>
-        <v>0.40927121471375394</v>
+        <v>0.22407748991821541</v>
       </c>
       <c r="P6">
         <f>Data!W14</f>
-        <v>0.42794536986966836</v>
+        <v>0.22941296281990525</v>
       </c>
       <c r="Q6">
         <f>Data!X14</f>
-        <v>0.44361186764819516</v>
+        <v>0.23388910504234148</v>
       </c>
       <c r="R6">
         <f>Data!Y14</f>
-        <v>0.45640632463440423</v>
+        <v>0.23754466418125836</v>
       </c>
       <c r="S6">
         <f>Data!Z14</f>
-        <v>0.46662768728531168</v>
+        <v>0.24046505351008907</v>
       </c>
       <c r="T6">
         <f>Data!AA14</f>
-        <v>0.47465073012346881</v>
+        <v>0.24275735146384822</v>
       </c>
       <c r="U6">
         <f>Data!AB14</f>
-        <v>0.48086153897442074</v>
+        <v>0.24453186827840592</v>
       </c>
       <c r="V6">
         <f>Data!AC14</f>
-        <v>0.48561805262983726</v>
+        <v>0.24589087217995351</v>
       </c>
       <c r="W6">
         <f>Data!AD14</f>
-        <v>0.48923089922499818</v>
+        <v>0.24692311406428519</v>
       </c>
       <c r="X6">
         <f>Data!AE14</f>
-        <v>0.49195792053149101</v>
+        <v>0.24770226300899745</v>
       </c>
       <c r="Y6">
         <f>Data!AF14</f>
-        <v>0.49400658833949529</v>
+        <v>0.24828759666842723</v>
       </c>
       <c r="Z6">
         <f>Data!AG14</f>
-        <v>0.49554017768756087</v>
+        <v>0.24872576505358884</v>
       </c>
       <c r="AA6">
         <f>Data!AH14</f>
-        <v>0.49668513474631881</v>
+        <v>0.24905289564180538</v>
       </c>
       <c r="AB6">
         <f>Data!AI14</f>
-        <v>0.49753824449575168</v>
+        <v>0.24929664128450046</v>
       </c>
       <c r="AC6">
         <f>Data!AJ14</f>
-        <v>0.49817295600725453</v>
+        <v>0.24947798743064414</v>
       </c>
       <c r="AD6">
         <f>Data!AK14</f>
-        <v>0.49864465879576514</v>
+        <v>0.24961275965593288</v>
       </c>
       <c r="AE6">
         <f>Data!AL14</f>
-        <v>0.49899492979550486</v>
+        <v>0.24971283708442996</v>
       </c>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.35">
@@ -9634,119 +9634,119 @@
       </c>
       <c r="C6">
         <f>Data!J21</f>
-        <v>1.5833609527091983E-2</v>
+        <v>1.2140101603773719E-2</v>
       </c>
       <c r="D6">
         <f>Data!K21</f>
-        <v>1.8323312087103298E-2</v>
+        <v>1.3363235653583922E-2</v>
       </c>
       <c r="E6">
         <f>Data!L21</f>
-        <v>2.164372919914653E-2</v>
+        <v>1.4994480804930065E-2</v>
       </c>
       <c r="F6">
         <f>Data!M21</f>
-        <v>2.605388897689399E-2</v>
+        <v>1.7161091658734945E-2</v>
       </c>
       <c r="G6">
         <f>Data!N21</f>
-        <v>3.1879597698632259E-2</v>
+        <v>2.0023129404240558E-2</v>
       </c>
       <c r="H6">
         <f>Data!O21</f>
-        <v>3.9520046599517591E-2</v>
+        <v>2.3776707585268467E-2</v>
       </c>
       <c r="I6">
         <f>Data!P21</f>
-        <v>4.9446542717040881E-2</v>
+        <v>2.8653368593560293E-2</v>
       </c>
       <c r="J6">
         <f>Data!Q21</f>
-        <v>6.218635093033742E-2</v>
+        <v>3.4912145631434188E-2</v>
       </c>
       <c r="K6">
         <f>Data!R21</f>
-        <v>7.8282662291795646E-2</v>
+        <v>4.2819896066673677E-2</v>
       </c>
       <c r="L6">
         <f>Data!S21</f>
-        <v>9.8222036552919223E-2</v>
+        <v>5.2615655601330122E-2</v>
       </c>
       <c r="M6">
         <f>Data!T21</f>
-        <v>0.12232636736606015</v>
+        <v>6.4457563240814544E-2</v>
       </c>
       <c r="N6">
         <f>Data!U21</f>
-        <v>0.15062040022549095</v>
+        <v>7.8357775881741934E-2</v>
       </c>
       <c r="O6">
         <f>Data!V21</f>
-        <v>0.18270722318791771</v>
+        <v>9.4121299744366602E-2</v>
       </c>
       <c r="P6">
         <f>Data!W21</f>
-        <v>0.21770358390280897</v>
+        <v>0.11131421310572374</v>
       </c>
       <c r="Q6">
         <f>Data!X21</f>
-        <v>0.25428662761243104</v>
+        <v>0.12928662761243104</v>
       </c>
       <c r="R6">
         <f>Data!Y21</f>
-        <v>0.2908696713220531</v>
+        <v>0.14725904211913834</v>
       </c>
       <c r="S6">
         <f>Data!Z21</f>
-        <v>0.32586603203694436</v>
+        <v>0.16445195548049549</v>
       </c>
       <c r="T6">
         <f>Data!AA21</f>
-        <v>0.35795285499937113</v>
+        <v>0.18021547934312016</v>
       </c>
       <c r="U6">
         <f>Data!AB21</f>
-        <v>0.3862468878588019</v>
+        <v>0.19411569198404752</v>
       </c>
       <c r="V6">
         <f>Data!AC21</f>
-        <v>0.41035121867194285</v>
+        <v>0.20595759962353194</v>
       </c>
       <c r="W6">
         <f>Data!AD21</f>
-        <v>0.43029059293306648</v>
+        <v>0.21575335915818841</v>
       </c>
       <c r="X6">
         <f>Data!AE21</f>
-        <v>0.44638690429452466</v>
+        <v>0.22366110959342791</v>
       </c>
       <c r="Y6">
         <f>Data!AF21</f>
-        <v>0.45912671250782122</v>
+        <v>0.22991988663130181</v>
       </c>
       <c r="Z6">
         <f>Data!AG21</f>
-        <v>0.4690532086253445</v>
+        <v>0.23479654763959362</v>
       </c>
       <c r="AA6">
         <f>Data!AH21</f>
-        <v>0.47669365752622989</v>
+        <v>0.23855012582062154</v>
       </c>
       <c r="AB6">
         <f>Data!AI21</f>
-        <v>0.4825193662479681</v>
+        <v>0.24141216356612716</v>
       </c>
       <c r="AC6">
         <f>Data!AJ21</f>
-        <v>0.48692952602571554</v>
+        <v>0.243578774419932</v>
       </c>
       <c r="AD6">
         <f>Data!AK21</f>
-        <v>0.49024994313775883</v>
+        <v>0.24521001957127816</v>
       </c>
       <c r="AE6">
         <f>Data!AL21</f>
-        <v>0.49273964569777012</v>
+        <v>0.24643315362108836</v>
       </c>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.35">
@@ -63356,8 +63356,8 @@
   </sheetPr>
   <dimension ref="A1:AL95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -64220,7 +64220,7 @@
         <v>0.15</v>
       </c>
       <c r="F14" s="41">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="G14" s="7" t="str">
         <f>IF(E14=F14,"n/a",IF(OR(C14="battery electric vehicle",C14="natural gas vehicle",C14="plugin hybrid vehicle",C14="hydrogen vehicle"),"s-curve","linear"))</f>
@@ -64232,119 +64232,119 @@
       </c>
       <c r="J14">
         <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:J$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,J$9))</f>
-        <v>0.17534926987653121</v>
+        <v>0.15724264853615177</v>
       </c>
       <c r="K14">
         <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:K$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,K$9))</f>
-        <v>0.18337231271468832</v>
+        <v>0.15953494648991096</v>
       </c>
       <c r="L14">
         <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:L$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,L$9))</f>
-        <v>0.19359367536559574</v>
+        <v>0.16245533581874164</v>
       </c>
       <c r="M14">
         <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:M$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,M$9))</f>
-        <v>0.20638813235180481</v>
+        <v>0.16611089495765852</v>
       </c>
       <c r="N14">
         <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:N$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,N$9))</f>
-        <v>0.22205463013033155</v>
+        <v>0.17058703718009474</v>
       </c>
       <c r="O14">
         <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:O$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,O$9))</f>
-        <v>0.24072878528624608</v>
+        <v>0.17592251008178461</v>
       </c>
       <c r="P14">
         <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:P$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,P$9))</f>
-        <v>0.26228745528861241</v>
+        <v>0.18208213008246071</v>
       </c>
       <c r="Q14">
         <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:Q$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,Q$9))</f>
-        <v>0.28627626811777229</v>
+        <v>0.1889360766050778</v>
       </c>
       <c r="R14">
         <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:R$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,R$9))</f>
-        <v>0.31189955412968762</v>
+        <v>0.19625701546562505</v>
       </c>
       <c r="S14">
         <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:S$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,S$9))</f>
-        <v>0.33810044587031229</v>
+        <v>0.20374298453437495</v>
       </c>
       <c r="T14">
         <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:T$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,T$9))</f>
-        <v>0.36372373188222767</v>
+        <v>0.21106392339492219</v>
       </c>
       <c r="U14">
         <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:U$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,U$9))</f>
-        <v>0.3877125447113875</v>
+        <v>0.21791786991753931</v>
       </c>
       <c r="V14">
         <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:V$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,V$9))</f>
-        <v>0.40927121471375394</v>
+        <v>0.22407748991821541</v>
       </c>
       <c r="W14">
         <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:W$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,W$9))</f>
-        <v>0.42794536986966836</v>
+        <v>0.22941296281990525</v>
       </c>
       <c r="X14">
         <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:X$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,X$9))</f>
-        <v>0.44361186764819516</v>
+        <v>0.23388910504234148</v>
       </c>
       <c r="Y14">
         <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:Y$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,Y$9))</f>
-        <v>0.45640632463440423</v>
+        <v>0.23754466418125836</v>
       </c>
       <c r="Z14">
         <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:Z$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,Z$9))</f>
-        <v>0.46662768728531168</v>
+        <v>0.24046505351008907</v>
       </c>
       <c r="AA14">
         <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:AA$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,AA$9))</f>
-        <v>0.47465073012346881</v>
+        <v>0.24275735146384822</v>
       </c>
       <c r="AB14">
         <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:AB$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,AB$9))</f>
-        <v>0.48086153897442074</v>
+        <v>0.24453186827840592</v>
       </c>
       <c r="AC14">
         <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:AC$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,AC$9))</f>
-        <v>0.48561805262983726</v>
+        <v>0.24589087217995351</v>
       </c>
       <c r="AD14">
         <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:AD$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,AD$9))</f>
-        <v>0.48923089922499818</v>
+        <v>0.24692311406428519</v>
       </c>
       <c r="AE14">
         <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:AE$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,AE$9))</f>
-        <v>0.49195792053149101</v>
+        <v>0.24770226300899745</v>
       </c>
       <c r="AF14">
         <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:AF$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,AF$9))</f>
-        <v>0.49400658833949529</v>
+        <v>0.24828759666842723</v>
       </c>
       <c r="AG14">
         <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:AG$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,AG$9))</f>
-        <v>0.49554017768756087</v>
+        <v>0.24872576505358884</v>
       </c>
       <c r="AH14">
         <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:AH$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,AH$9))</f>
-        <v>0.49668513474631881</v>
+        <v>0.24905289564180538</v>
       </c>
       <c r="AI14">
         <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:AI$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,AI$9))</f>
-        <v>0.49753824449575168</v>
+        <v>0.24929664128450046</v>
       </c>
       <c r="AJ14">
         <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:AJ$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,AJ$9))</f>
-        <v>0.49817295600725453</v>
+        <v>0.24947798743064414</v>
       </c>
       <c r="AK14">
         <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:AK$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,AK$9))</f>
-        <v>0.49864465879576514</v>
+        <v>0.24961275965593288</v>
       </c>
       <c r="AL14">
         <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:AL$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,AL$9))</f>
-        <v>0.49899492979550486</v>
+        <v>0.24971283708442996</v>
       </c>
     </row>
     <row r="15" spans="1:38" x14ac:dyDescent="0.35">
@@ -65182,7 +65182,7 @@
       </c>
       <c r="F21" s="22">
         <f>F14</f>
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="G21" s="7" t="str">
         <f>IF(E21=F21,"n/a",IF(OR(C21="battery electric vehicle",C21="natural gas vehicle",C21="plugin hybrid vehicle"),"s-curve","linear"))</f>
@@ -65194,119 +65194,119 @@
       </c>
       <c r="J21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:J$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,J$9))</f>
-        <v>1.5833609527091983E-2</v>
+        <v>1.2140101603773719E-2</v>
       </c>
       <c r="K21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:K$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,K$9))</f>
-        <v>1.8323312087103298E-2</v>
+        <v>1.3363235653583922E-2</v>
       </c>
       <c r="L21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:L$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,L$9))</f>
-        <v>2.164372919914653E-2</v>
+        <v>1.4994480804930065E-2</v>
       </c>
       <c r="M21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:M$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,M$9))</f>
-        <v>2.605388897689399E-2</v>
+        <v>1.7161091658734945E-2</v>
       </c>
       <c r="N21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:N$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,N$9))</f>
-        <v>3.1879597698632259E-2</v>
+        <v>2.0023129404240558E-2</v>
       </c>
       <c r="O21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:O$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,O$9))</f>
-        <v>3.9520046599517591E-2</v>
+        <v>2.3776707585268467E-2</v>
       </c>
       <c r="P21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:P$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,P$9))</f>
-        <v>4.9446542717040881E-2</v>
+        <v>2.8653368593560293E-2</v>
       </c>
       <c r="Q21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:Q$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,Q$9))</f>
-        <v>6.218635093033742E-2</v>
+        <v>3.4912145631434188E-2</v>
       </c>
       <c r="R21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:R$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,R$9))</f>
-        <v>7.8282662291795646E-2</v>
+        <v>4.2819896066673677E-2</v>
       </c>
       <c r="S21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:S$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,S$9))</f>
-        <v>9.8222036552919223E-2</v>
+        <v>5.2615655601330122E-2</v>
       </c>
       <c r="T21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:T$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,T$9))</f>
-        <v>0.12232636736606015</v>
+        <v>6.4457563240814544E-2</v>
       </c>
       <c r="U21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:U$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,U$9))</f>
-        <v>0.15062040022549095</v>
+        <v>7.8357775881741934E-2</v>
       </c>
       <c r="V21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:V$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,V$9))</f>
-        <v>0.18270722318791771</v>
+        <v>9.4121299744366602E-2</v>
       </c>
       <c r="W21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:W$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,W$9))</f>
-        <v>0.21770358390280897</v>
+        <v>0.11131421310572374</v>
       </c>
       <c r="X21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:X$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,X$9))</f>
-        <v>0.25428662761243104</v>
+        <v>0.12928662761243104</v>
       </c>
       <c r="Y21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:Y$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,Y$9))</f>
-        <v>0.2908696713220531</v>
+        <v>0.14725904211913834</v>
       </c>
       <c r="Z21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:Z$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,Z$9))</f>
-        <v>0.32586603203694436</v>
+        <v>0.16445195548049549</v>
       </c>
       <c r="AA21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:AA$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,AA$9))</f>
-        <v>0.35795285499937113</v>
+        <v>0.18021547934312016</v>
       </c>
       <c r="AB21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:AB$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,AB$9))</f>
-        <v>0.3862468878588019</v>
+        <v>0.19411569198404752</v>
       </c>
       <c r="AC21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:AC$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,AC$9))</f>
-        <v>0.41035121867194285</v>
+        <v>0.20595759962353194</v>
       </c>
       <c r="AD21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:AD$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,AD$9))</f>
-        <v>0.43029059293306648</v>
+        <v>0.21575335915818841</v>
       </c>
       <c r="AE21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:AE$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,AE$9))</f>
-        <v>0.44638690429452466</v>
+        <v>0.22366110959342791</v>
       </c>
       <c r="AF21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:AF$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,AF$9))</f>
-        <v>0.45912671250782122</v>
+        <v>0.22991988663130181</v>
       </c>
       <c r="AG21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:AG$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,AG$9))</f>
-        <v>0.4690532086253445</v>
+        <v>0.23479654763959362</v>
       </c>
       <c r="AH21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:AH$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,AH$9))</f>
-        <v>0.47669365752622989</v>
+        <v>0.23855012582062154</v>
       </c>
       <c r="AI21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:AI$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,AI$9))</f>
-        <v>0.4825193662479681</v>
+        <v>0.24141216356612716</v>
       </c>
       <c r="AJ21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:AJ$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,AJ$9))</f>
-        <v>0.48692952602571554</v>
+        <v>0.243578774419932</v>
       </c>
       <c r="AK21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:AK$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,AK$9))</f>
-        <v>0.49024994313775883</v>
+        <v>0.24521001957127816</v>
       </c>
       <c r="AL21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:AL$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,AL$9))</f>
-        <v>0.49273964569777012</v>
+        <v>0.24643315362108836</v>
       </c>
     </row>
     <row r="22" spans="1:38" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Calibrate TTS and policy scenario for frgt-HDVs
</commit_message>
<xml_diff>
--- a/InputData/trans/TTS/Transportation Technology Shareweights.xlsx
+++ b/InputData/trans/TTS/Transportation Technology Shareweights.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Modeling\EPS\EU\eps-eu\InputData\trans\TTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBB696AF-2C83-446D-A3FA-68614E057911}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D77DF435-BE5F-497D-B589-B49F6535A47F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="63885" yWindow="3720" windowWidth="22140" windowHeight="13245" firstSheet="7" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32700" yWindow="2040" windowWidth="22140" windowHeight="13245" firstSheet="7" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -4736,91 +4736,91 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="29"/>
                 <c:pt idx="0" formatCode="0.0000">
-                  <c:v>2.5</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.5</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.5</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.5</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.5</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.5</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.5</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.5</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.5</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.5</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.5</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.5</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.5</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.5</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.5</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.5</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.5</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2.5</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.5</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2.5</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2.5</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2.5</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2.5</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2.5</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2.5</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2.5</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2.5</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2.5</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2.5</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8984,8 +8984,8 @@
   </sheetPr>
   <dimension ref="A1:AD8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O11" sqref="A11:O12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10964,8 +10964,8 @@
   </sheetPr>
   <dimension ref="A1:AD8"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="AE1" sqref="AE1:AE1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -11100,119 +11100,119 @@
       </c>
       <c r="B2">
         <f>Data!I31</f>
-        <v>0.5</v>
+        <v>0.05</v>
       </c>
       <c r="C2">
         <f>Data!J31</f>
-        <v>0.53456921017167336</v>
+        <v>6.3827684068669371E-2</v>
       </c>
       <c r="D2">
         <f>Data!K31</f>
-        <v>0.52866208794943437</v>
+        <v>6.1464835179773747E-2</v>
       </c>
       <c r="E2">
         <f>Data!L31</f>
-        <v>0.53456921017167336</v>
+        <v>6.3827684068669371E-2</v>
       </c>
       <c r="F2">
         <f>Data!M31</f>
-        <v>0.54158634824696117</v>
+        <v>6.6634539298784476E-2</v>
       </c>
       <c r="G2">
         <f>Data!N31</f>
-        <v>0.5498752445598426</v>
+        <v>6.9950097823937032E-2</v>
       </c>
       <c r="H2">
         <f>Data!O31</f>
-        <v>0.55960146101105879</v>
+        <v>7.3840584404423509E-2</v>
       </c>
       <c r="I2">
         <f>Data!P31</f>
-        <v>0.57092553245024391</v>
+        <v>7.8370212980097553E-2</v>
       </c>
       <c r="J2">
         <f>Data!Q31</f>
-        <v>0.58399080743303777</v>
+        <v>8.3596322973215106E-2</v>
       </c>
       <c r="K2">
         <f>Data!R31</f>
-        <v>0.59890805572070915</v>
+        <v>8.9563222288283645E-2</v>
       </c>
       <c r="L2">
         <f>Data!S31</f>
-        <v>0.61573760825049118</v>
+        <v>9.6295043300196476E-2</v>
       </c>
       <c r="M2">
         <f>Data!T31</f>
-        <v>0.63447071068499761</v>
+        <v>0.10378828427399903</v>
       </c>
       <c r="N2">
         <f>Data!U31</f>
-        <v>0.65501275943619375</v>
+        <v>0.1120051037744775</v>
       </c>
       <c r="O2">
         <f>Data!V31</f>
-        <v>0.6771718468871023</v>
+        <v>0.12086873875484092</v>
       </c>
       <c r="P2">
         <f>Data!W31</f>
-        <v>0.700656169943774</v>
+        <v>0.13026246797750962</v>
       </c>
       <c r="Q2">
         <f>Data!X31</f>
-        <v>0.72508300134376102</v>
+        <v>0.14003320053750445</v>
       </c>
       <c r="R2">
         <f>Data!Y31</f>
-        <v>0.75</v>
+        <v>0.15000000000000002</v>
       </c>
       <c r="S2">
         <f>Data!Z31</f>
-        <v>0.77491699865623898</v>
+        <v>0.15996679946249559</v>
       </c>
       <c r="T2">
         <f>Data!AA31</f>
-        <v>0.799343830056226</v>
+        <v>0.16973753202249042</v>
       </c>
       <c r="U2">
         <f>Data!AB31</f>
-        <v>0.8228281531128977</v>
+        <v>0.1791312612451591</v>
       </c>
       <c r="V2">
         <f>Data!AC31</f>
-        <v>0.84498724056380625</v>
+        <v>0.18799489622552251</v>
       </c>
       <c r="W2">
         <f>Data!AD31</f>
-        <v>0.86552928931500239</v>
+        <v>0.19621171572600099</v>
       </c>
       <c r="X2">
         <f>Data!AE31</f>
-        <v>0.88426239174950894</v>
+        <v>0.20370495669980354</v>
       </c>
       <c r="Y2">
         <f>Data!AF31</f>
-        <v>0.90109194427929085</v>
+        <v>0.21043677771171637</v>
       </c>
       <c r="Z2">
         <f>Data!AG31</f>
-        <v>0.91600919256696223</v>
+        <v>0.21640367702678492</v>
       </c>
       <c r="AA2">
         <f>Data!AH31</f>
-        <v>0.9290744675497562</v>
+        <v>0.22162978701990249</v>
       </c>
       <c r="AB2">
         <f>Data!AI31</f>
-        <v>0.9403985389889411</v>
+        <v>0.22615941559557651</v>
       </c>
       <c r="AC2">
         <f>Data!AJ31</f>
-        <v>0.9501247554401574</v>
+        <v>0.23004990217606297</v>
       </c>
       <c r="AD2">
         <f>Data!AK31</f>
-        <v>0.95841365175303883</v>
+        <v>0.23336546070121555</v>
       </c>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.35">
@@ -11463,119 +11463,119 @@
       </c>
       <c r="B5">
         <f>Data!I34</f>
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="C5">
         <f>Data!J34</f>
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="D5">
         <f>Data!K34</f>
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="E5">
         <f>Data!L34</f>
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="F5">
         <f>Data!M34</f>
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="G5">
         <f>Data!N34</f>
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="H5">
         <f>Data!O34</f>
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="I5">
         <f>Data!P34</f>
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="J5">
         <f>Data!Q34</f>
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="K5">
         <f>Data!R34</f>
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="L5">
         <f>Data!S34</f>
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="M5">
         <f>Data!T34</f>
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="N5">
         <f>Data!U34</f>
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="O5">
         <f>Data!V34</f>
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="P5">
         <f>Data!W34</f>
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="Q5">
         <f>Data!X34</f>
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="R5">
         <f>Data!Y34</f>
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="S5">
         <f>Data!Z34</f>
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="T5">
         <f>Data!AA34</f>
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="U5">
         <f>Data!AB34</f>
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="V5">
         <f>Data!AC34</f>
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="W5">
         <f>Data!AD34</f>
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="X5">
         <f>Data!AE34</f>
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="Y5">
         <f>Data!AF34</f>
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="Z5">
         <f>Data!AG34</f>
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="AA5">
         <f>Data!AH34</f>
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="AB5">
         <f>Data!AI34</f>
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="AC5">
         <f>Data!AJ34</f>
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="AD5">
         <f>Data!AK34</f>
-        <v>2.5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.35">
@@ -11826,119 +11826,119 @@
       </c>
       <c r="B8">
         <f>Data!I37</f>
-        <v>7.4999999999999997E-2</v>
+        <v>0.01</v>
       </c>
       <c r="C8">
         <f>Data!J37</f>
-        <v>7.6108052376995472E-2</v>
+        <v>1.0295480633865461E-2</v>
       </c>
       <c r="D8">
         <f>Data!K37</f>
-        <v>7.6488022930055813E-2</v>
+        <v>1.039680611468155E-2</v>
       </c>
       <c r="E8">
         <f>Data!L37</f>
-        <v>7.6994774518264933E-2</v>
+        <v>1.0531939871537317E-2</v>
       </c>
       <c r="F8">
         <f>Data!M37</f>
-        <v>7.7667839195447716E-2</v>
+        <v>1.0711423785452723E-2</v>
       </c>
       <c r="G8">
         <f>Data!N37</f>
-        <v>7.8556940488317503E-2</v>
+        <v>1.0948517463551336E-2</v>
       </c>
       <c r="H8">
         <f>Data!O37</f>
-        <v>7.9723001704274737E-2</v>
+        <v>1.125946712113993E-2</v>
       </c>
       <c r="I8">
         <f>Data!P37</f>
-        <v>8.1237952237044178E-2</v>
+        <v>1.1663453929878448E-2</v>
       </c>
       <c r="J8">
         <f>Data!Q37</f>
-        <v>8.3182261589670958E-2</v>
+        <v>1.2181936423912259E-2</v>
       </c>
       <c r="K8">
         <f>Data!R37</f>
-        <v>8.5638829867536584E-2</v>
+        <v>1.2837021298009756E-2</v>
       </c>
       <c r="L8">
         <f>Data!S37</f>
-        <v>8.8681914285476726E-2</v>
+        <v>1.3648510476127126E-2</v>
       </c>
       <c r="M8">
         <f>Data!T37</f>
-        <v>9.2360641237573676E-2</v>
+        <v>1.4629504330019647E-2</v>
       </c>
       <c r="N8">
         <f>Data!U37</f>
-        <v>9.6678787303124708E-2</v>
+        <v>1.5781009947499921E-2</v>
       </c>
       <c r="O8">
         <f>Data!V37</f>
-        <v>0.10157577703306533</v>
+        <v>1.708687387548409E-2</v>
       </c>
       <c r="P8">
         <f>Data!W37</f>
-        <v>0.10691681123912558</v>
+        <v>1.8511149663766817E-2</v>
       </c>
       <c r="Q8">
         <f>Data!X37</f>
-        <v>0.11249999999999999</v>
+        <v>1.9999999999999997E-2</v>
       </c>
       <c r="R8">
         <f>Data!Y37</f>
-        <v>0.11808318876087442</v>
+        <v>2.1488850336233177E-2</v>
       </c>
       <c r="S8">
         <f>Data!Z37</f>
-        <v>0.12342422296693464</v>
+        <v>2.2913126124515907E-2</v>
       </c>
       <c r="T8">
         <f>Data!AA37</f>
-        <v>0.1283212126968753</v>
+        <v>2.4218990052500076E-2</v>
       </c>
       <c r="U8">
         <f>Data!AB37</f>
-        <v>0.13263935876242633</v>
+        <v>2.5370495669980349E-2</v>
       </c>
       <c r="V8">
         <f>Data!AC37</f>
-        <v>0.13631808571452325</v>
+        <v>2.6351489523872867E-2</v>
       </c>
       <c r="W8">
         <f>Data!AD37</f>
-        <v>0.13936117013246341</v>
+        <v>2.7162978701990241E-2</v>
       </c>
       <c r="X8">
         <f>Data!AE37</f>
-        <v>0.14181773841032902</v>
+        <v>2.7818063576087737E-2</v>
       </c>
       <c r="Y8">
         <f>Data!AF37</f>
-        <v>0.14376204776295581</v>
+        <v>2.8336546070121552E-2</v>
       </c>
       <c r="Z8">
         <f>Data!AG37</f>
-        <v>0.14527699829572527</v>
+        <v>2.8740532878860067E-2</v>
       </c>
       <c r="AA8">
         <f>Data!AH37</f>
-        <v>0.14644305951168249</v>
+        <v>2.9051482536448667E-2</v>
       </c>
       <c r="AB8">
         <f>Data!AI37</f>
-        <v>0.1473321608045523</v>
+        <v>2.9288576214547273E-2</v>
       </c>
       <c r="AC8">
         <f>Data!AJ37</f>
-        <v>0.14800522548173506</v>
+        <v>2.9468060128462675E-2</v>
       </c>
       <c r="AD8">
         <f>Data!AK37</f>
-        <v>0.14851197706994418</v>
+        <v>2.960319388531845E-2</v>
       </c>
     </row>
   </sheetData>
@@ -63006,8 +63006,8 @@
   </sheetPr>
   <dimension ref="A1:AK95"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -66118,10 +66118,10 @@
         <v>1</v>
       </c>
       <c r="E31" s="22">
-        <v>0.5</v>
+        <v>0.05</v>
       </c>
       <c r="F31" s="22">
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="G31" s="7" t="str">
         <f>IF(E31=F31,"n/a",IF(OR(C31="battery electric vehicle",C31="natural gas vehicle",C31="plugin hybrid vehicle"),"s-curve","linear"))</f>
@@ -66129,119 +66129,119 @@
       </c>
       <c r="I31" s="22">
         <f t="shared" si="2"/>
-        <v>0.5</v>
+        <v>0.05</v>
       </c>
       <c r="J31">
         <f>IF($G31="s-curve",$E31+($F31-$E31)*$R$2/(1+EXP($R$3*(COUNT(J$9:$K$9)+$R$4))),TREND($E31:$F31,$E$9:$F$9,J$9))</f>
-        <v>0.53456921017167336</v>
+        <v>6.3827684068669371E-2</v>
       </c>
       <c r="K31">
         <f>IF($G31="s-curve",$E31+($F31-$E31)*$R$2/(1+EXP($R$3*(COUNT($K$9:K$9)+$R$4))),TREND($E31:$F31,$E$9:$F$9,K$9))</f>
-        <v>0.52866208794943437</v>
+        <v>6.1464835179773747E-2</v>
       </c>
       <c r="L31">
         <f>IF($G31="s-curve",$E31+($F31-$E31)*$R$2/(1+EXP($R$3*(COUNT($K$9:L$9)+$R$4))),TREND($E31:$F31,$E$9:$F$9,L$9))</f>
-        <v>0.53456921017167336</v>
+        <v>6.3827684068669371E-2</v>
       </c>
       <c r="M31">
         <f>IF($G31="s-curve",$E31+($F31-$E31)*$R$2/(1+EXP($R$3*(COUNT($K$9:M$9)+$R$4))),TREND($E31:$F31,$E$9:$F$9,M$9))</f>
-        <v>0.54158634824696117</v>
+        <v>6.6634539298784476E-2</v>
       </c>
       <c r="N31">
         <f>IF($G31="s-curve",$E31+($F31-$E31)*$R$2/(1+EXP($R$3*(COUNT($K$9:N$9)+$R$4))),TREND($E31:$F31,$E$9:$F$9,N$9))</f>
-        <v>0.5498752445598426</v>
+        <v>6.9950097823937032E-2</v>
       </c>
       <c r="O31">
         <f>IF($G31="s-curve",$E31+($F31-$E31)*$R$2/(1+EXP($R$3*(COUNT($K$9:O$9)+$R$4))),TREND($E31:$F31,$E$9:$F$9,O$9))</f>
-        <v>0.55960146101105879</v>
+        <v>7.3840584404423509E-2</v>
       </c>
       <c r="P31">
         <f>IF($G31="s-curve",$E31+($F31-$E31)*$R$2/(1+EXP($R$3*(COUNT($K$9:P$9)+$R$4))),TREND($E31:$F31,$E$9:$F$9,P$9))</f>
-        <v>0.57092553245024391</v>
+        <v>7.8370212980097553E-2</v>
       </c>
       <c r="Q31">
         <f>IF($G31="s-curve",$E31+($F31-$E31)*$R$2/(1+EXP($R$3*(COUNT($K$9:Q$9)+$R$4))),TREND($E31:$F31,$E$9:$F$9,Q$9))</f>
-        <v>0.58399080743303777</v>
+        <v>8.3596322973215106E-2</v>
       </c>
       <c r="R31">
         <f>IF($G31="s-curve",$E31+($F31-$E31)*$R$2/(1+EXP($R$3*(COUNT($K$9:R$9)+$R$4))),TREND($E31:$F31,$E$9:$F$9,R$9))</f>
-        <v>0.59890805572070915</v>
+        <v>8.9563222288283645E-2</v>
       </c>
       <c r="S31">
         <f>IF($G31="s-curve",$E31+($F31-$E31)*$R$2/(1+EXP($R$3*(COUNT($K$9:S$9)+$R$4))),TREND($E31:$F31,$E$9:$F$9,S$9))</f>
-        <v>0.61573760825049118</v>
+        <v>9.6295043300196476E-2</v>
       </c>
       <c r="T31">
         <f>IF($G31="s-curve",$E31+($F31-$E31)*$R$2/(1+EXP($R$3*(COUNT($K$9:T$9)+$R$4))),TREND($E31:$F31,$E$9:$F$9,T$9))</f>
-        <v>0.63447071068499761</v>
+        <v>0.10378828427399903</v>
       </c>
       <c r="U31">
         <f>IF($G31="s-curve",$E31+($F31-$E31)*$R$2/(1+EXP($R$3*(COUNT($K$9:U$9)+$R$4))),TREND($E31:$F31,$E$9:$F$9,U$9))</f>
-        <v>0.65501275943619375</v>
+        <v>0.1120051037744775</v>
       </c>
       <c r="V31">
         <f>IF($G31="s-curve",$E31+($F31-$E31)*$R$2/(1+EXP($R$3*(COUNT($K$9:V$9)+$R$4))),TREND($E31:$F31,$E$9:$F$9,V$9))</f>
-        <v>0.6771718468871023</v>
+        <v>0.12086873875484092</v>
       </c>
       <c r="W31">
         <f>IF($G31="s-curve",$E31+($F31-$E31)*$R$2/(1+EXP($R$3*(COUNT($K$9:W$9)+$R$4))),TREND($E31:$F31,$E$9:$F$9,W$9))</f>
-        <v>0.700656169943774</v>
+        <v>0.13026246797750962</v>
       </c>
       <c r="X31">
         <f>IF($G31="s-curve",$E31+($F31-$E31)*$R$2/(1+EXP($R$3*(COUNT($K$9:X$9)+$R$4))),TREND($E31:$F31,$E$9:$F$9,X$9))</f>
-        <v>0.72508300134376102</v>
+        <v>0.14003320053750445</v>
       </c>
       <c r="Y31">
         <f>IF($G31="s-curve",$E31+($F31-$E31)*$R$2/(1+EXP($R$3*(COUNT($K$9:Y$9)+$R$4))),TREND($E31:$F31,$E$9:$F$9,Y$9))</f>
-        <v>0.75</v>
+        <v>0.15000000000000002</v>
       </c>
       <c r="Z31">
         <f>IF($G31="s-curve",$E31+($F31-$E31)*$R$2/(1+EXP($R$3*(COUNT($K$9:Z$9)+$R$4))),TREND($E31:$F31,$E$9:$F$9,Z$9))</f>
-        <v>0.77491699865623898</v>
+        <v>0.15996679946249559</v>
       </c>
       <c r="AA31">
         <f>IF($G31="s-curve",$E31+($F31-$E31)*$R$2/(1+EXP($R$3*(COUNT($K$9:AA$9)+$R$4))),TREND($E31:$F31,$E$9:$F$9,AA$9))</f>
-        <v>0.799343830056226</v>
+        <v>0.16973753202249042</v>
       </c>
       <c r="AB31">
         <f>IF($G31="s-curve",$E31+($F31-$E31)*$R$2/(1+EXP($R$3*(COUNT($K$9:AB$9)+$R$4))),TREND($E31:$F31,$E$9:$F$9,AB$9))</f>
-        <v>0.8228281531128977</v>
+        <v>0.1791312612451591</v>
       </c>
       <c r="AC31">
         <f>IF($G31="s-curve",$E31+($F31-$E31)*$R$2/(1+EXP($R$3*(COUNT($K$9:AC$9)+$R$4))),TREND($E31:$F31,$E$9:$F$9,AC$9))</f>
-        <v>0.84498724056380625</v>
+        <v>0.18799489622552251</v>
       </c>
       <c r="AD31">
         <f>IF($G31="s-curve",$E31+($F31-$E31)*$R$2/(1+EXP($R$3*(COUNT($K$9:AD$9)+$R$4))),TREND($E31:$F31,$E$9:$F$9,AD$9))</f>
-        <v>0.86552928931500239</v>
+        <v>0.19621171572600099</v>
       </c>
       <c r="AE31">
         <f>IF($G31="s-curve",$E31+($F31-$E31)*$R$2/(1+EXP($R$3*(COUNT($K$9:AE$9)+$R$4))),TREND($E31:$F31,$E$9:$F$9,AE$9))</f>
-        <v>0.88426239174950894</v>
+        <v>0.20370495669980354</v>
       </c>
       <c r="AF31">
         <f>IF($G31="s-curve",$E31+($F31-$E31)*$R$2/(1+EXP($R$3*(COUNT($K$9:AF$9)+$R$4))),TREND($E31:$F31,$E$9:$F$9,AF$9))</f>
-        <v>0.90109194427929085</v>
+        <v>0.21043677771171637</v>
       </c>
       <c r="AG31">
         <f>IF($G31="s-curve",$E31+($F31-$E31)*$R$2/(1+EXP($R$3*(COUNT($K$9:AG$9)+$R$4))),TREND($E31:$F31,$E$9:$F$9,AG$9))</f>
-        <v>0.91600919256696223</v>
+        <v>0.21640367702678492</v>
       </c>
       <c r="AH31">
         <f>IF($G31="s-curve",$E31+($F31-$E31)*$R$2/(1+EXP($R$3*(COUNT($K$9:AH$9)+$R$4))),TREND($E31:$F31,$E$9:$F$9,AH$9))</f>
-        <v>0.9290744675497562</v>
+        <v>0.22162978701990249</v>
       </c>
       <c r="AI31">
         <f>IF($G31="s-curve",$E31+($F31-$E31)*$R$2/(1+EXP($R$3*(COUNT($K$9:AI$9)+$R$4))),TREND($E31:$F31,$E$9:$F$9,AI$9))</f>
-        <v>0.9403985389889411</v>
+        <v>0.22615941559557651</v>
       </c>
       <c r="AJ31">
         <f>IF($G31="s-curve",$E31+($F31-$E31)*$R$2/(1+EXP($R$3*(COUNT($K$9:AJ$9)+$R$4))),TREND($E31:$F31,$E$9:$F$9,AJ$9))</f>
-        <v>0.9501247554401574</v>
+        <v>0.23004990217606297</v>
       </c>
       <c r="AK31">
         <f>IF($G31="s-curve",$E31+($F31-$E31)*$R$2/(1+EXP($R$3*(COUNT($K$9:AK$9)+$R$4))),TREND($E31:$F31,$E$9:$F$9,AK$9))</f>
-        <v>0.95841365175303883</v>
+        <v>0.23336546070121555</v>
       </c>
     </row>
     <row r="32" spans="1:37" x14ac:dyDescent="0.35">
@@ -66513,10 +66513,10 @@
         <v>4</v>
       </c>
       <c r="E34">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="F34">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="G34" s="7" t="str">
         <f>IF(E34=F34,"n/a",IF(OR(C34="battery electric vehicle",C34="natural gas vehicle",C34="plugin hybrid vehicle"),"s-curve","linear"))</f>
@@ -66524,119 +66524,119 @@
       </c>
       <c r="I34" s="22">
         <f t="shared" si="2"/>
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="J34">
         <f>IF($G34="s-curve",$E34+($F34-$E34)*$I$2/(1+EXP($I$3*(COUNT($I$9:J$9)+$I$4))),TREND($E34:$F34,$E$9:$F$9,J$9))</f>
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="K34">
         <f>IF($G34="s-curve",$E34+($F34-$E34)*$I$2/(1+EXP($I$3*(COUNT($I$9:K$9)+$I$4))),TREND($E34:$F34,$E$9:$F$9,K$9))</f>
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="L34">
         <f>IF($G34="s-curve",$E34+($F34-$E34)*$I$2/(1+EXP($I$3*(COUNT($I$9:L$9)+$I$4))),TREND($E34:$F34,$E$9:$F$9,L$9))</f>
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="M34">
         <f>IF($G34="s-curve",$E34+($F34-$E34)*$I$2/(1+EXP($I$3*(COUNT($I$9:M$9)+$I$4))),TREND($E34:$F34,$E$9:$F$9,M$9))</f>
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="N34">
         <f>IF($G34="s-curve",$E34+($F34-$E34)*$I$2/(1+EXP($I$3*(COUNT($I$9:N$9)+$I$4))),TREND($E34:$F34,$E$9:$F$9,N$9))</f>
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="O34">
         <f>IF($G34="s-curve",$E34+($F34-$E34)*$I$2/(1+EXP($I$3*(COUNT($I$9:O$9)+$I$4))),TREND($E34:$F34,$E$9:$F$9,O$9))</f>
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="P34">
         <f>IF($G34="s-curve",$E34+($F34-$E34)*$I$2/(1+EXP($I$3*(COUNT($I$9:P$9)+$I$4))),TREND($E34:$F34,$E$9:$F$9,P$9))</f>
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="Q34">
         <f>IF($G34="s-curve",$E34+($F34-$E34)*$I$2/(1+EXP($I$3*(COUNT($I$9:Q$9)+$I$4))),TREND($E34:$F34,$E$9:$F$9,Q$9))</f>
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="R34">
         <f>IF($G34="s-curve",$E34+($F34-$E34)*$I$2/(1+EXP($I$3*(COUNT($I$9:R$9)+$I$4))),TREND($E34:$F34,$E$9:$F$9,R$9))</f>
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="S34">
         <f>IF($G34="s-curve",$E34+($F34-$E34)*$I$2/(1+EXP($I$3*(COUNT($I$9:S$9)+$I$4))),TREND($E34:$F34,$E$9:$F$9,S$9))</f>
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="T34">
         <f>IF($G34="s-curve",$E34+($F34-$E34)*$I$2/(1+EXP($I$3*(COUNT($I$9:T$9)+$I$4))),TREND($E34:$F34,$E$9:$F$9,T$9))</f>
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="U34">
         <f>IF($G34="s-curve",$E34+($F34-$E34)*$I$2/(1+EXP($I$3*(COUNT($I$9:U$9)+$I$4))),TREND($E34:$F34,$E$9:$F$9,U$9))</f>
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="V34">
         <f>IF($G34="s-curve",$E34+($F34-$E34)*$I$2/(1+EXP($I$3*(COUNT($I$9:V$9)+$I$4))),TREND($E34:$F34,$E$9:$F$9,V$9))</f>
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="W34">
         <f>IF($G34="s-curve",$E34+($F34-$E34)*$I$2/(1+EXP($I$3*(COUNT($I$9:W$9)+$I$4))),TREND($E34:$F34,$E$9:$F$9,W$9))</f>
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="X34">
         <f>IF($G34="s-curve",$E34+($F34-$E34)*$I$2/(1+EXP($I$3*(COUNT($I$9:X$9)+$I$4))),TREND($E34:$F34,$E$9:$F$9,X$9))</f>
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="Y34">
         <f>IF($G34="s-curve",$E34+($F34-$E34)*$I$2/(1+EXP($I$3*(COUNT($I$9:Y$9)+$I$4))),TREND($E34:$F34,$E$9:$F$9,Y$9))</f>
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="Z34">
         <f>IF($G34="s-curve",$E34+($F34-$E34)*$I$2/(1+EXP($I$3*(COUNT($I$9:Z$9)+$I$4))),TREND($E34:$F34,$E$9:$F$9,Z$9))</f>
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="AA34">
         <f>IF($G34="s-curve",$E34+($F34-$E34)*$I$2/(1+EXP($I$3*(COUNT($I$9:AA$9)+$I$4))),TREND($E34:$F34,$E$9:$F$9,AA$9))</f>
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="AB34">
         <f>IF($G34="s-curve",$E34+($F34-$E34)*$I$2/(1+EXP($I$3*(COUNT($I$9:AB$9)+$I$4))),TREND($E34:$F34,$E$9:$F$9,AB$9))</f>
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="AC34">
         <f>IF($G34="s-curve",$E34+($F34-$E34)*$I$2/(1+EXP($I$3*(COUNT($I$9:AC$9)+$I$4))),TREND($E34:$F34,$E$9:$F$9,AC$9))</f>
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="AD34">
         <f>IF($G34="s-curve",$E34+($F34-$E34)*$I$2/(1+EXP($I$3*(COUNT($I$9:AD$9)+$I$4))),TREND($E34:$F34,$E$9:$F$9,AD$9))</f>
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="AE34">
         <f>IF($G34="s-curve",$E34+($F34-$E34)*$I$2/(1+EXP($I$3*(COUNT($I$9:AE$9)+$I$4))),TREND($E34:$F34,$E$9:$F$9,AE$9))</f>
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="AF34">
         <f>IF($G34="s-curve",$E34+($F34-$E34)*$I$2/(1+EXP($I$3*(COUNT($I$9:AF$9)+$I$4))),TREND($E34:$F34,$E$9:$F$9,AF$9))</f>
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="AG34">
         <f>IF($G34="s-curve",$E34+($F34-$E34)*$I$2/(1+EXP($I$3*(COUNT($I$9:AG$9)+$I$4))),TREND($E34:$F34,$E$9:$F$9,AG$9))</f>
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="AH34">
         <f>IF($G34="s-curve",$E34+($F34-$E34)*$I$2/(1+EXP($I$3*(COUNT($I$9:AH$9)+$I$4))),TREND($E34:$F34,$E$9:$F$9,AH$9))</f>
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="AI34">
         <f>IF($G34="s-curve",$E34+($F34-$E34)*$I$2/(1+EXP($I$3*(COUNT($I$9:AI$9)+$I$4))),TREND($E34:$F34,$E$9:$F$9,AI$9))</f>
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="AJ34">
         <f>IF($G34="s-curve",$E34+($F34-$E34)*$I$2/(1+EXP($I$3*(COUNT($I$9:AJ$9)+$I$4))),TREND($E34:$F34,$E$9:$F$9,AJ$9))</f>
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="AK34">
         <f>IF($G34="s-curve",$E34+($F34-$E34)*$I$2/(1+EXP($I$3*(COUNT($I$9:AK$9)+$I$4))),TREND($E34:$F34,$E$9:$F$9,AK$9))</f>
-        <v>2.5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="35" spans="1:37" x14ac:dyDescent="0.35">
@@ -66911,10 +66911,10 @@
       </c>
       <c r="D37" s="23"/>
       <c r="E37" s="26">
-        <v>7.4999999999999997E-2</v>
+        <v>0.01</v>
       </c>
       <c r="F37" s="26">
-        <v>0.15</v>
+        <v>0.03</v>
       </c>
       <c r="G37" s="8" t="str">
         <f>IF(E37=F37,"n/a",IF(OR(C37="battery electric vehicle",C37="natural gas vehicle",C37="plugin hybrid vehicle",C37="hydrogen vehicle"),"s-curve","linear"))</f>
@@ -66922,119 +66922,119 @@
       </c>
       <c r="I37" s="22">
         <f t="shared" si="2"/>
-        <v>7.4999999999999997E-2</v>
+        <v>0.01</v>
       </c>
       <c r="J37">
         <f>IF($G37="s-curve",$E37+($F37-$E37)*$I$2/(1+EXP($I$3*(COUNT($I$9:J$9)+$I$4))),TREND($E37:$F37,$E$9:$F$9,J$9))</f>
-        <v>7.6108052376995472E-2</v>
+        <v>1.0295480633865461E-2</v>
       </c>
       <c r="K37">
         <f>IF($G37="s-curve",$E37+($F37-$E37)*$I$2/(1+EXP($I$3*(COUNT($I$9:K$9)+$I$4))),TREND($E37:$F37,$E$9:$F$9,K$9))</f>
-        <v>7.6488022930055813E-2</v>
+        <v>1.039680611468155E-2</v>
       </c>
       <c r="L37">
         <f>IF($G37="s-curve",$E37+($F37-$E37)*$I$2/(1+EXP($I$3*(COUNT($I$9:L$9)+$I$4))),TREND($E37:$F37,$E$9:$F$9,L$9))</f>
-        <v>7.6994774518264933E-2</v>
+        <v>1.0531939871537317E-2</v>
       </c>
       <c r="M37">
         <f>IF($G37="s-curve",$E37+($F37-$E37)*$I$2/(1+EXP($I$3*(COUNT($I$9:M$9)+$I$4))),TREND($E37:$F37,$E$9:$F$9,M$9))</f>
-        <v>7.7667839195447716E-2</v>
+        <v>1.0711423785452723E-2</v>
       </c>
       <c r="N37">
         <f>IF($G37="s-curve",$E37+($F37-$E37)*$I$2/(1+EXP($I$3*(COUNT($I$9:N$9)+$I$4))),TREND($E37:$F37,$E$9:$F$9,N$9))</f>
-        <v>7.8556940488317503E-2</v>
+        <v>1.0948517463551336E-2</v>
       </c>
       <c r="O37">
         <f>IF($G37="s-curve",$E37+($F37-$E37)*$I$2/(1+EXP($I$3*(COUNT($I$9:O$9)+$I$4))),TREND($E37:$F37,$E$9:$F$9,O$9))</f>
-        <v>7.9723001704274737E-2</v>
+        <v>1.125946712113993E-2</v>
       </c>
       <c r="P37">
         <f>IF($G37="s-curve",$E37+($F37-$E37)*$I$2/(1+EXP($I$3*(COUNT($I$9:P$9)+$I$4))),TREND($E37:$F37,$E$9:$F$9,P$9))</f>
-        <v>8.1237952237044178E-2</v>
+        <v>1.1663453929878448E-2</v>
       </c>
       <c r="Q37">
         <f>IF($G37="s-curve",$E37+($F37-$E37)*$I$2/(1+EXP($I$3*(COUNT($I$9:Q$9)+$I$4))),TREND($E37:$F37,$E$9:$F$9,Q$9))</f>
-        <v>8.3182261589670958E-2</v>
+        <v>1.2181936423912259E-2</v>
       </c>
       <c r="R37">
         <f>IF($G37="s-curve",$E37+($F37-$E37)*$I$2/(1+EXP($I$3*(COUNT($I$9:R$9)+$I$4))),TREND($E37:$F37,$E$9:$F$9,R$9))</f>
-        <v>8.5638829867536584E-2</v>
+        <v>1.2837021298009756E-2</v>
       </c>
       <c r="S37">
         <f>IF($G37="s-curve",$E37+($F37-$E37)*$I$2/(1+EXP($I$3*(COUNT($I$9:S$9)+$I$4))),TREND($E37:$F37,$E$9:$F$9,S$9))</f>
-        <v>8.8681914285476726E-2</v>
+        <v>1.3648510476127126E-2</v>
       </c>
       <c r="T37">
         <f>IF($G37="s-curve",$E37+($F37-$E37)*$I$2/(1+EXP($I$3*(COUNT($I$9:T$9)+$I$4))),TREND($E37:$F37,$E$9:$F$9,T$9))</f>
-        <v>9.2360641237573676E-2</v>
+        <v>1.4629504330019647E-2</v>
       </c>
       <c r="U37">
         <f>IF($G37="s-curve",$E37+($F37-$E37)*$I$2/(1+EXP($I$3*(COUNT($I$9:U$9)+$I$4))),TREND($E37:$F37,$E$9:$F$9,U$9))</f>
-        <v>9.6678787303124708E-2</v>
+        <v>1.5781009947499921E-2</v>
       </c>
       <c r="V37">
         <f>IF($G37="s-curve",$E37+($F37-$E37)*$I$2/(1+EXP($I$3*(COUNT($I$9:V$9)+$I$4))),TREND($E37:$F37,$E$9:$F$9,V$9))</f>
-        <v>0.10157577703306533</v>
+        <v>1.708687387548409E-2</v>
       </c>
       <c r="W37">
         <f>IF($G37="s-curve",$E37+($F37-$E37)*$I$2/(1+EXP($I$3*(COUNT($I$9:W$9)+$I$4))),TREND($E37:$F37,$E$9:$F$9,W$9))</f>
-        <v>0.10691681123912558</v>
+        <v>1.8511149663766817E-2</v>
       </c>
       <c r="X37">
         <f>IF($G37="s-curve",$E37+($F37-$E37)*$I$2/(1+EXP($I$3*(COUNT($I$9:X$9)+$I$4))),TREND($E37:$F37,$E$9:$F$9,X$9))</f>
-        <v>0.11249999999999999</v>
+        <v>1.9999999999999997E-2</v>
       </c>
       <c r="Y37">
         <f>IF($G37="s-curve",$E37+($F37-$E37)*$I$2/(1+EXP($I$3*(COUNT($I$9:Y$9)+$I$4))),TREND($E37:$F37,$E$9:$F$9,Y$9))</f>
-        <v>0.11808318876087442</v>
+        <v>2.1488850336233177E-2</v>
       </c>
       <c r="Z37">
         <f>IF($G37="s-curve",$E37+($F37-$E37)*$I$2/(1+EXP($I$3*(COUNT($I$9:Z$9)+$I$4))),TREND($E37:$F37,$E$9:$F$9,Z$9))</f>
-        <v>0.12342422296693464</v>
+        <v>2.2913126124515907E-2</v>
       </c>
       <c r="AA37">
         <f>IF($G37="s-curve",$E37+($F37-$E37)*$I$2/(1+EXP($I$3*(COUNT($I$9:AA$9)+$I$4))),TREND($E37:$F37,$E$9:$F$9,AA$9))</f>
-        <v>0.1283212126968753</v>
+        <v>2.4218990052500076E-2</v>
       </c>
       <c r="AB37">
         <f>IF($G37="s-curve",$E37+($F37-$E37)*$I$2/(1+EXP($I$3*(COUNT($I$9:AB$9)+$I$4))),TREND($E37:$F37,$E$9:$F$9,AB$9))</f>
-        <v>0.13263935876242633</v>
+        <v>2.5370495669980349E-2</v>
       </c>
       <c r="AC37">
         <f>IF($G37="s-curve",$E37+($F37-$E37)*$I$2/(1+EXP($I$3*(COUNT($I$9:AC$9)+$I$4))),TREND($E37:$F37,$E$9:$F$9,AC$9))</f>
-        <v>0.13631808571452325</v>
+        <v>2.6351489523872867E-2</v>
       </c>
       <c r="AD37">
         <f>IF($G37="s-curve",$E37+($F37-$E37)*$I$2/(1+EXP($I$3*(COUNT($I$9:AD$9)+$I$4))),TREND($E37:$F37,$E$9:$F$9,AD$9))</f>
-        <v>0.13936117013246341</v>
+        <v>2.7162978701990241E-2</v>
       </c>
       <c r="AE37">
         <f>IF($G37="s-curve",$E37+($F37-$E37)*$I$2/(1+EXP($I$3*(COUNT($I$9:AE$9)+$I$4))),TREND($E37:$F37,$E$9:$F$9,AE$9))</f>
-        <v>0.14181773841032902</v>
+        <v>2.7818063576087737E-2</v>
       </c>
       <c r="AF37">
         <f>IF($G37="s-curve",$E37+($F37-$E37)*$I$2/(1+EXP($I$3*(COUNT($I$9:AF$9)+$I$4))),TREND($E37:$F37,$E$9:$F$9,AF$9))</f>
-        <v>0.14376204776295581</v>
+        <v>2.8336546070121552E-2</v>
       </c>
       <c r="AG37">
         <f>IF($G37="s-curve",$E37+($F37-$E37)*$I$2/(1+EXP($I$3*(COUNT($I$9:AG$9)+$I$4))),TREND($E37:$F37,$E$9:$F$9,AG$9))</f>
-        <v>0.14527699829572527</v>
+        <v>2.8740532878860067E-2</v>
       </c>
       <c r="AH37">
         <f>IF($G37="s-curve",$E37+($F37-$E37)*$I$2/(1+EXP($I$3*(COUNT($I$9:AH$9)+$I$4))),TREND($E37:$F37,$E$9:$F$9,AH$9))</f>
-        <v>0.14644305951168249</v>
+        <v>2.9051482536448667E-2</v>
       </c>
       <c r="AI37">
         <f>IF($G37="s-curve",$E37+($F37-$E37)*$I$2/(1+EXP($I$3*(COUNT($I$9:AI$9)+$I$4))),TREND($E37:$F37,$E$9:$F$9,AI$9))</f>
-        <v>0.1473321608045523</v>
+        <v>2.9288576214547273E-2</v>
       </c>
       <c r="AJ37">
         <f>IF($G37="s-curve",$E37+($F37-$E37)*$I$2/(1+EXP($I$3*(COUNT($I$9:AJ$9)+$I$4))),TREND($E37:$F37,$E$9:$F$9,AJ$9))</f>
-        <v>0.14800522548173506</v>
+        <v>2.9468060128462675E-2</v>
       </c>
       <c r="AK37">
         <f>IF($G37="s-curve",$E37+($F37-$E37)*$I$2/(1+EXP($I$3*(COUNT($I$9:AK$9)+$I$4))),TREND($E37:$F37,$E$9:$F$9,AK$9))</f>
-        <v>0.14851197706994418</v>
+        <v>2.960319388531845E-2</v>
       </c>
     </row>
     <row r="38" spans="1:37" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Removing #REF! errors in TTS
</commit_message>
<xml_diff>
--- a/InputData/trans/TTS/Transportation Technology Shareweights.xlsx
+++ b/InputData/trans/TTS/Transportation Technology Shareweights.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Modeling\EPS\EU\eps-eu\InputData\trans\TTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF42B77B-8B6A-4EA6-8929-0CFA3E600326}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8017AFA-7409-4617-B4D9-6A896298AC25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4890" yWindow="1320" windowWidth="22140" windowHeight="13245" firstSheet="7" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-100" yWindow="270" windowWidth="19180" windowHeight="11260" firstSheet="7" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -3852,7 +3852,7 @@
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3928,7 +3928,6 @@
     <xf numFmtId="167" fontId="0" fillId="3" borderId="0" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="10" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="88">
     <cellStyle name="20% - Accent1" xfId="28" builtinId="30" customBuiltin="1"/>
@@ -7954,10 +7953,10 @@
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
-  <dimension ref="A1:AE8"/>
+  <dimension ref="A1:AD8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="AE1" sqref="AE1:AE1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7966,7 +7965,7 @@
     <col min="2" max="2" width="13.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:30" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="25" t="s">
         <v>127</v>
       </c>
@@ -8085,12 +8084,8 @@
         <f>Data!AK9</f>
         <v>2050</v>
       </c>
-      <c r="AE1" t="e">
-        <f>Data!#REF!</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -8210,12 +8205,8 @@
         <f>Data!AK10</f>
         <v>0.99701824935068328</v>
       </c>
-      <c r="AE2" t="e">
-        <f>Data!#REF!</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -8335,12 +8326,8 @@
         <f>Data!AK11</f>
         <v>1.2181248751199165E-3</v>
       </c>
-      <c r="AE3" t="e">
-        <f>Data!#REF!</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -8460,12 +8447,8 @@
         <f>Data!AK12</f>
         <v>0.79999999999999893</v>
       </c>
-      <c r="AE4" t="e">
-        <f>Data!#REF!</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -8585,12 +8568,8 @@
         <f>Data!AK13</f>
         <v>0.20000000000000018</v>
       </c>
-      <c r="AE5" t="e">
-        <f>Data!#REF!</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -8710,12 +8689,8 @@
         <f>Data!AK14</f>
         <v>0.14981412463484778</v>
       </c>
-      <c r="AE6" t="e">
-        <f>Data!#REF!</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>124</v>
       </c>
@@ -8835,12 +8810,8 @@
         <f>Data!AK15</f>
         <v>8.6165104068936654E-4</v>
       </c>
-      <c r="AE7" t="e">
-        <f>Data!#REF!</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>125</v>
       </c>
@@ -8959,10 +8930,6 @@
       <c r="AD8">
         <f>Data!AK16</f>
         <v>3.091993773478644E-4</v>
-      </c>
-      <c r="AE8" t="e">
-        <f>Data!#REF!</f>
-        <v>#REF!</v>
       </c>
     </row>
   </sheetData>
@@ -8977,7 +8944,7 @@
   </sheetPr>
   <dimension ref="A1:AD8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="R1" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -9966,7 +9933,7 @@
   </sheetPr>
   <dimension ref="A1:AD8"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -62999,7 +62966,7 @@
   </sheetPr>
   <dimension ref="A1:AK95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
@@ -65194,7 +65161,7 @@
         <f>IF(E24=F24,"n/a",IF(OR(C24="battery electric vehicle",C24="natural gas vehicle",C24="plugin hybrid vehicle"),"s-curve","linear"))</f>
         <v>s-curve</v>
       </c>
-      <c r="I24" s="49">
+      <c r="I24" s="22">
         <f>D24</f>
         <v>0.6</v>
       </c>

</xml_diff>

<commit_message>
Recalibrated psgr-LDV sector following price adjustments
</commit_message>
<xml_diff>
--- a/InputData/trans/TTS/Transportation Technology Shareweights.xlsx
+++ b/InputData/trans/TTS/Transportation Technology Shareweights.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Modeling\EPS\EU\eps-eu\InputData\trans\TTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8017AFA-7409-4617-B4D9-6A896298AC25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B442D69-8641-4D6D-ADE1-DB9FEDC0D593}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-100" yWindow="270" windowWidth="19180" windowHeight="11260" firstSheet="7" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57795" yWindow="3525" windowWidth="15195" windowHeight="10920" firstSheet="7" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -5066,91 +5066,91 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="29"/>
                 <c:pt idx="0" formatCode="0.0000">
-                  <c:v>0.34799999999999998</c:v>
+                  <c:v>0.372</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.28576839372836865</c:v>
+                  <c:v>0.36646728950191665</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.30341908797231432</c:v>
+                  <c:v>0.3821236845260918</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.32590608580431069</c:v>
+                  <c:v>0.40206994364200543</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.35405389117397068</c:v>
+                  <c:v>0.42703741256080774</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.38852018628672946</c:v>
+                  <c:v>0.45760946394004709</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.4296033276297414</c:v>
+                  <c:v>0.49405074385858883</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.47703240163494742</c:v>
+                  <c:v>0.53612094846320657</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.52980778985909904</c:v>
+                  <c:v>0.58293340321268139</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.58617901908531289</c:v>
+                  <c:v>0.63293541563021916</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.6438209809146872</c:v>
+                  <c:v>0.68406458436978101</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.70019221014090094</c:v>
+                  <c:v>0.73406659678731867</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.75296759836505256</c:v>
+                  <c:v>0.78087905153679338</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.80039667237025858</c:v>
+                  <c:v>0.82294925614141134</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.84147981371327052</c:v>
+                  <c:v>0.85939053605995297</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.87594610882602941</c:v>
+                  <c:v>0.88996258743919232</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.9040939141956893</c:v>
+                  <c:v>0.91493005635799451</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.92658091202768578</c:v>
+                  <c:v>0.93487631547390837</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.94423160627163139</c:v>
+                  <c:v>0.95053271049808341</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.95789538574372557</c:v>
+                  <c:v>0.96265266034151242</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.96835971578564195</c:v>
+                  <c:v>0.97193465698908255</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.97630797829499605</c:v>
+                  <c:v>0.9789848690590679</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.98230742516928027</c:v>
+                  <c:v>0.98430645635145253</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.98681449434688973</c:v>
+                  <c:v>0.98830428524535807</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.99018839091263411</c:v>
+                  <c:v>0.99129697531601191</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.99270729644190148</c:v>
+                  <c:v>0.99353127723353074</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.9945841378906537</c:v>
+                  <c:v>0.99519605997313842</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.9959805032159601</c:v>
+                  <c:v>0.99643465415129961</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.99701824935068328</c:v>
+                  <c:v>0.99735514845002182</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7955,8 +7955,8 @@
   </sheetPr>
   <dimension ref="A1:AD8"/>
   <sheetViews>
-    <sheetView topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="AE1" sqref="AE1:AE1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8091,119 +8091,119 @@
       </c>
       <c r="B2">
         <f>Data!I10</f>
-        <v>0.34799999999999998</v>
+        <v>0.372</v>
       </c>
       <c r="C2">
         <f>Data!J10</f>
-        <v>0.28576839372836865</v>
+        <v>0.36646728950191665</v>
       </c>
       <c r="D2">
         <f>Data!K10</f>
-        <v>0.30341908797231432</v>
+        <v>0.3821236845260918</v>
       </c>
       <c r="E2">
         <f>Data!L10</f>
-        <v>0.32590608580431069</v>
+        <v>0.40206994364200543</v>
       </c>
       <c r="F2">
         <f>Data!M10</f>
-        <v>0.35405389117397068</v>
+        <v>0.42703741256080774</v>
       </c>
       <c r="G2">
         <f>Data!N10</f>
-        <v>0.38852018628672946</v>
+        <v>0.45760946394004709</v>
       </c>
       <c r="H2">
         <f>Data!O10</f>
-        <v>0.4296033276297414</v>
+        <v>0.49405074385858883</v>
       </c>
       <c r="I2">
         <f>Data!P10</f>
-        <v>0.47703240163494742</v>
+        <v>0.53612094846320657</v>
       </c>
       <c r="J2">
         <f>Data!Q10</f>
-        <v>0.52980778985909904</v>
+        <v>0.58293340321268139</v>
       </c>
       <c r="K2">
         <f>Data!R10</f>
-        <v>0.58617901908531289</v>
+        <v>0.63293541563021916</v>
       </c>
       <c r="L2">
         <f>Data!S10</f>
-        <v>0.6438209809146872</v>
+        <v>0.68406458436978101</v>
       </c>
       <c r="M2">
         <f>Data!T10</f>
-        <v>0.70019221014090094</v>
+        <v>0.73406659678731867</v>
       </c>
       <c r="N2">
         <f>Data!U10</f>
-        <v>0.75296759836505256</v>
+        <v>0.78087905153679338</v>
       </c>
       <c r="O2">
         <f>Data!V10</f>
-        <v>0.80039667237025858</v>
+        <v>0.82294925614141134</v>
       </c>
       <c r="P2">
         <f>Data!W10</f>
-        <v>0.84147981371327052</v>
+        <v>0.85939053605995297</v>
       </c>
       <c r="Q2">
         <f>Data!X10</f>
-        <v>0.87594610882602941</v>
+        <v>0.88996258743919232</v>
       </c>
       <c r="R2">
         <f>Data!Y10</f>
-        <v>0.9040939141956893</v>
+        <v>0.91493005635799451</v>
       </c>
       <c r="S2">
         <f>Data!Z10</f>
-        <v>0.92658091202768578</v>
+        <v>0.93487631547390837</v>
       </c>
       <c r="T2">
         <f>Data!AA10</f>
-        <v>0.94423160627163139</v>
+        <v>0.95053271049808341</v>
       </c>
       <c r="U2">
         <f>Data!AB10</f>
-        <v>0.95789538574372557</v>
+        <v>0.96265266034151242</v>
       </c>
       <c r="V2">
         <f>Data!AC10</f>
-        <v>0.96835971578564195</v>
+        <v>0.97193465698908255</v>
       </c>
       <c r="W2">
         <f>Data!AD10</f>
-        <v>0.97630797829499605</v>
+        <v>0.9789848690590679</v>
       </c>
       <c r="X2">
         <f>Data!AE10</f>
-        <v>0.98230742516928027</v>
+        <v>0.98430645635145253</v>
       </c>
       <c r="Y2">
         <f>Data!AF10</f>
-        <v>0.98681449434688973</v>
+        <v>0.98830428524535807</v>
       </c>
       <c r="Z2">
         <f>Data!AG10</f>
-        <v>0.99018839091263411</v>
+        <v>0.99129697531601191</v>
       </c>
       <c r="AA2">
         <f>Data!AH10</f>
-        <v>0.99270729644190148</v>
+        <v>0.99353127723353074</v>
       </c>
       <c r="AB2">
         <f>Data!AI10</f>
-        <v>0.9945841378906537</v>
+        <v>0.99519605997313842</v>
       </c>
       <c r="AC2">
         <f>Data!AJ10</f>
-        <v>0.9959805032159601</v>
+        <v>0.99643465415129961</v>
       </c>
       <c r="AD2">
         <f>Data!AK10</f>
-        <v>0.99701824935068328</v>
+        <v>0.99735514845002182</v>
       </c>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.35">
@@ -8575,119 +8575,119 @@
       </c>
       <c r="B6">
         <f>Data!I14</f>
-        <v>0.16400000000000001</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="C6">
         <f>Data!J14</f>
-        <v>0.10547647129735284</v>
+        <v>0.17681066213403793</v>
       </c>
       <c r="D6">
         <f>Data!K14</f>
-        <v>0.10657677431515725</v>
+        <v>0.17738373662247772</v>
       </c>
       <c r="E6">
         <f>Data!L14</f>
-        <v>0.10797856119299598</v>
+        <v>0.17811383395468541</v>
       </c>
       <c r="F6">
         <f>Data!M14</f>
-        <v>0.10973322957967609</v>
+        <v>0.17902772373941461</v>
       </c>
       <c r="G6">
         <f>Data!N14</f>
-        <v>0.11188177784644547</v>
+        <v>0.18014675929502369</v>
       </c>
       <c r="H6">
         <f>Data!O14</f>
-        <v>0.1144428048392566</v>
+        <v>0.18148062752044614</v>
       </c>
       <c r="I6">
         <f>Data!P14</f>
-        <v>0.11739942243958112</v>
+        <v>0.18302053252061518</v>
       </c>
       <c r="J6">
         <f>Data!Q14</f>
-        <v>0.12068931677043734</v>
+        <v>0.18473401915126944</v>
       </c>
       <c r="K6">
         <f>Data!R14</f>
-        <v>0.12420336742350002</v>
+        <v>0.18656425386640627</v>
       </c>
       <c r="L6">
         <f>Data!S14</f>
-        <v>0.12779663257649998</v>
+        <v>0.18843574613359373</v>
       </c>
       <c r="M6">
         <f>Data!T14</f>
-        <v>0.13131068322956266</v>
+        <v>0.19026598084873056</v>
       </c>
       <c r="N6">
         <f>Data!U14</f>
-        <v>0.13460057756041885</v>
+        <v>0.19197946747938482</v>
       </c>
       <c r="O6">
         <f>Data!V14</f>
-        <v>0.13755719516074338</v>
+        <v>0.19351937247955386</v>
       </c>
       <c r="P6">
         <f>Data!W14</f>
-        <v>0.14011822215355452</v>
+        <v>0.19485324070497631</v>
       </c>
       <c r="Q6">
         <f>Data!X14</f>
-        <v>0.1422667704203239</v>
+        <v>0.19597227626058539</v>
       </c>
       <c r="R6">
         <f>Data!Y14</f>
-        <v>0.14402143880700402</v>
+        <v>0.19688616604531459</v>
       </c>
       <c r="S6">
         <f>Data!Z14</f>
-        <v>0.14542322568484273</v>
+        <v>0.19761626337752228</v>
       </c>
       <c r="T6">
         <f>Data!AA14</f>
-        <v>0.14652352870264715</v>
+        <v>0.19818933786596207</v>
       </c>
       <c r="U6">
         <f>Data!AB14</f>
-        <v>0.14737529677363484</v>
+        <v>0.19863296706960148</v>
       </c>
       <c r="V6">
         <f>Data!AC14</f>
-        <v>0.14802761864637767</v>
+        <v>0.19897271804498839</v>
       </c>
       <c r="W6">
         <f>Data!AD14</f>
-        <v>0.1485230947508569</v>
+        <v>0.19923077851607132</v>
       </c>
       <c r="X6">
         <f>Data!AE14</f>
-        <v>0.14889708624431877</v>
+        <v>0.19942556575224937</v>
       </c>
       <c r="Y6">
         <f>Data!AF14</f>
-        <v>0.14917804640084506</v>
+        <v>0.19957189916710683</v>
       </c>
       <c r="Z6">
         <f>Data!AG14</f>
-        <v>0.14938836722572263</v>
+        <v>0.19968144126339721</v>
       </c>
       <c r="AA6">
         <f>Data!AH14</f>
-        <v>0.14954538990806659</v>
+        <v>0.19976322391045137</v>
       </c>
       <c r="AB6">
         <f>Data!AI14</f>
-        <v>0.14966238781656022</v>
+        <v>0.19982416032112513</v>
       </c>
       <c r="AC6">
         <f>Data!AJ14</f>
-        <v>0.1497494339667092</v>
+        <v>0.19986949685766106</v>
       </c>
       <c r="AD6">
         <f>Data!AK14</f>
-        <v>0.14981412463484778</v>
+        <v>0.19990318991398323</v>
       </c>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.35">
@@ -9568,115 +9568,115 @@
       </c>
       <c r="C6">
         <f>Data!J21</f>
-        <v>2.2161047539909582E-3</v>
+        <v>2.9548063386546112E-3</v>
       </c>
       <c r="D6">
         <f>Data!K21</f>
-        <v>2.9760458601116261E-3</v>
+        <v>3.9680611468155018E-3</v>
       </c>
       <c r="E6">
         <f>Data!L21</f>
-        <v>3.9895490365298792E-3</v>
+        <v>5.3193987153731734E-3</v>
       </c>
       <c r="F6">
         <f>Data!M21</f>
-        <v>5.3356783908954262E-3</v>
+        <v>7.1142378545272361E-3</v>
       </c>
       <c r="G6">
         <f>Data!N21</f>
-        <v>7.1138809766350172E-3</v>
+        <v>9.4851746355133562E-3</v>
       </c>
       <c r="H6">
         <f>Data!O21</f>
-        <v>9.4460034085494752E-3</v>
+        <v>1.2594671211399303E-2</v>
       </c>
       <c r="I6">
         <f>Data!P21</f>
-        <v>1.2475904474088355E-2</v>
+        <v>1.6634539298784477E-2</v>
       </c>
       <c r="J6">
         <f>Data!Q21</f>
-        <v>1.6364523179341936E-2</v>
+        <v>2.1819364239122584E-2</v>
       </c>
       <c r="K6">
         <f>Data!R21</f>
-        <v>2.1277659735073173E-2</v>
+        <v>2.8370212980097564E-2</v>
       </c>
       <c r="L6">
         <f>Data!S21</f>
-        <v>2.7363828570953451E-2</v>
+        <v>3.6485104761271273E-2</v>
       </c>
       <c r="M6">
         <f>Data!T21</f>
-        <v>3.4721282475147351E-2</v>
+        <v>4.629504330019648E-2</v>
       </c>
       <c r="N6">
         <f>Data!U21</f>
-        <v>4.3357574606249408E-2</v>
+        <v>5.7810099474999217E-2</v>
       </c>
       <c r="O6">
         <f>Data!V21</f>
-        <v>5.3151554066130681E-2</v>
+        <v>7.0868738754840913E-2</v>
       </c>
       <c r="P6">
         <f>Data!W21</f>
-        <v>6.3833622478251154E-2</v>
+        <v>8.5111496637668205E-2</v>
       </c>
       <c r="Q6">
         <f>Data!X21</f>
-        <v>7.4999999999999997E-2</v>
+        <v>0.1</v>
       </c>
       <c r="R6">
         <f>Data!Y21</f>
-        <v>8.6166377521748855E-2</v>
+        <v>0.11488850336233181</v>
       </c>
       <c r="S6">
         <f>Data!Z21</f>
-        <v>9.6848445933869307E-2</v>
+        <v>0.12913126124515908</v>
       </c>
       <c r="T6">
         <f>Data!AA21</f>
-        <v>0.10664242539375059</v>
+        <v>0.1421899005250008</v>
       </c>
       <c r="U6">
         <f>Data!AB21</f>
-        <v>0.11527871752485264</v>
+        <v>0.15370495669980352</v>
       </c>
       <c r="V6">
         <f>Data!AC21</f>
-        <v>0.12263617142904654</v>
+        <v>0.16351489523872872</v>
       </c>
       <c r="W6">
         <f>Data!AD21</f>
-        <v>0.12872234026492685</v>
+        <v>0.17162978701990247</v>
       </c>
       <c r="X6">
         <f>Data!AE21</f>
-        <v>0.13363547682065807</v>
+        <v>0.17818063576087742</v>
       </c>
       <c r="Y6">
         <f>Data!AF21</f>
-        <v>0.13752409552591163</v>
+        <v>0.18336546070121554</v>
       </c>
       <c r="Z6">
         <f>Data!AG21</f>
-        <v>0.14055399659145051</v>
+        <v>0.18740532878860072</v>
       </c>
       <c r="AA6">
         <f>Data!AH21</f>
-        <v>0.14288611902336498</v>
+        <v>0.19051482536448666</v>
       </c>
       <c r="AB6">
         <f>Data!AI21</f>
-        <v>0.14466432160910458</v>
+        <v>0.19288576214547279</v>
       </c>
       <c r="AC6">
         <f>Data!AJ21</f>
-        <v>0.1460104509634701</v>
+        <v>0.19468060128462683</v>
       </c>
       <c r="AD6">
         <f>Data!AK21</f>
-        <v>0.14702395413988836</v>
+        <v>0.19603193885318451</v>
       </c>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.35">
@@ -9933,7 +9933,7 @@
   </sheetPr>
   <dimension ref="A1:AD8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="Q1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -62966,8 +62966,8 @@
   </sheetPr>
   <dimension ref="A1:AK95"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -63275,10 +63275,10 @@
         <v>1</v>
       </c>
       <c r="D10">
-        <v>0.34799999999999998</v>
+        <v>0.372</v>
       </c>
       <c r="E10" s="22">
-        <v>0.23</v>
+        <v>0.317</v>
       </c>
       <c r="F10">
         <v>1</v>
@@ -63289,119 +63289,119 @@
       </c>
       <c r="I10" s="22">
         <f>D10</f>
-        <v>0.34799999999999998</v>
+        <v>0.372</v>
       </c>
       <c r="J10">
         <f>IF($G10="s-curve",$E10+($F10-$E10)*$O$2/(1+EXP($O$3*(COUNT($I$9:J$9)+$O$4))),TREND($E10:$F10,$E$9:$F$9,J$9))</f>
-        <v>0.28576839372836865</v>
+        <v>0.36646728950191665</v>
       </c>
       <c r="K10">
         <f>IF($G10="s-curve",$E10+($F10-$E10)*$O$2/(1+EXP($O$3*(COUNT($I$9:K$9)+$O$4))),TREND($E10:$F10,$E$9:$F$9,K$9))</f>
-        <v>0.30341908797231432</v>
+        <v>0.3821236845260918</v>
       </c>
       <c r="L10">
         <f>IF($G10="s-curve",$E10+($F10-$E10)*$O$2/(1+EXP($O$3*(COUNT($I$9:L$9)+$O$4))),TREND($E10:$F10,$E$9:$F$9,L$9))</f>
-        <v>0.32590608580431069</v>
+        <v>0.40206994364200543</v>
       </c>
       <c r="M10">
         <f>IF($G10="s-curve",$E10+($F10-$E10)*$O$2/(1+EXP($O$3*(COUNT($I$9:M$9)+$O$4))),TREND($E10:$F10,$E$9:$F$9,M$9))</f>
-        <v>0.35405389117397068</v>
+        <v>0.42703741256080774</v>
       </c>
       <c r="N10">
         <f>IF($G10="s-curve",$E10+($F10-$E10)*$O$2/(1+EXP($O$3*(COUNT($I$9:N$9)+$O$4))),TREND($E10:$F10,$E$9:$F$9,N$9))</f>
-        <v>0.38852018628672946</v>
+        <v>0.45760946394004709</v>
       </c>
       <c r="O10">
         <f>IF($G10="s-curve",$E10+($F10-$E10)*$O$2/(1+EXP($O$3*(COUNT($I$9:O$9)+$O$4))),TREND($E10:$F10,$E$9:$F$9,O$9))</f>
-        <v>0.4296033276297414</v>
+        <v>0.49405074385858883</v>
       </c>
       <c r="P10">
         <f>IF($G10="s-curve",$E10+($F10-$E10)*$O$2/(1+EXP($O$3*(COUNT($I$9:P$9)+$O$4))),TREND($E10:$F10,$E$9:$F$9,P$9))</f>
-        <v>0.47703240163494742</v>
+        <v>0.53612094846320657</v>
       </c>
       <c r="Q10">
         <f>IF($G10="s-curve",$E10+($F10-$E10)*$O$2/(1+EXP($O$3*(COUNT($I$9:Q$9)+$O$4))),TREND($E10:$F10,$E$9:$F$9,Q$9))</f>
-        <v>0.52980778985909904</v>
+        <v>0.58293340321268139</v>
       </c>
       <c r="R10">
         <f>IF($G10="s-curve",$E10+($F10-$E10)*$O$2/(1+EXP($O$3*(COUNT($I$9:R$9)+$O$4))),TREND($E10:$F10,$E$9:$F$9,R$9))</f>
-        <v>0.58617901908531289</v>
+        <v>0.63293541563021916</v>
       </c>
       <c r="S10">
         <f>IF($G10="s-curve",$E10+($F10-$E10)*$O$2/(1+EXP($O$3*(COUNT($I$9:S$9)+$O$4))),TREND($E10:$F10,$E$9:$F$9,S$9))</f>
-        <v>0.6438209809146872</v>
+        <v>0.68406458436978101</v>
       </c>
       <c r="T10">
         <f>IF($G10="s-curve",$E10+($F10-$E10)*$O$2/(1+EXP($O$3*(COUNT($I$9:T$9)+$O$4))),TREND($E10:$F10,$E$9:$F$9,T$9))</f>
-        <v>0.70019221014090094</v>
+        <v>0.73406659678731867</v>
       </c>
       <c r="U10">
         <f>IF($G10="s-curve",$E10+($F10-$E10)*$O$2/(1+EXP($O$3*(COUNT($I$9:U$9)+$O$4))),TREND($E10:$F10,$E$9:$F$9,U$9))</f>
-        <v>0.75296759836505256</v>
+        <v>0.78087905153679338</v>
       </c>
       <c r="V10">
         <f>IF($G10="s-curve",$E10+($F10-$E10)*$O$2/(1+EXP($O$3*(COUNT($I$9:V$9)+$O$4))),TREND($E10:$F10,$E$9:$F$9,V$9))</f>
-        <v>0.80039667237025858</v>
+        <v>0.82294925614141134</v>
       </c>
       <c r="W10">
         <f>IF($G10="s-curve",$E10+($F10-$E10)*$O$2/(1+EXP($O$3*(COUNT($I$9:W$9)+$O$4))),TREND($E10:$F10,$E$9:$F$9,W$9))</f>
-        <v>0.84147981371327052</v>
+        <v>0.85939053605995297</v>
       </c>
       <c r="X10">
         <f>IF($G10="s-curve",$E10+($F10-$E10)*$O$2/(1+EXP($O$3*(COUNT($I$9:X$9)+$O$4))),TREND($E10:$F10,$E$9:$F$9,X$9))</f>
-        <v>0.87594610882602941</v>
+        <v>0.88996258743919232</v>
       </c>
       <c r="Y10">
         <f>IF($G10="s-curve",$E10+($F10-$E10)*$O$2/(1+EXP($O$3*(COUNT($I$9:Y$9)+$O$4))),TREND($E10:$F10,$E$9:$F$9,Y$9))</f>
-        <v>0.9040939141956893</v>
+        <v>0.91493005635799451</v>
       </c>
       <c r="Z10">
         <f>IF($G10="s-curve",$E10+($F10-$E10)*$O$2/(1+EXP($O$3*(COUNT($I$9:Z$9)+$O$4))),TREND($E10:$F10,$E$9:$F$9,Z$9))</f>
-        <v>0.92658091202768578</v>
+        <v>0.93487631547390837</v>
       </c>
       <c r="AA10">
         <f>IF($G10="s-curve",$E10+($F10-$E10)*$O$2/(1+EXP($O$3*(COUNT($I$9:AA$9)+$O$4))),TREND($E10:$F10,$E$9:$F$9,AA$9))</f>
-        <v>0.94423160627163139</v>
+        <v>0.95053271049808341</v>
       </c>
       <c r="AB10">
         <f>IF($G10="s-curve",$E10+($F10-$E10)*$O$2/(1+EXP($O$3*(COUNT($I$9:AB$9)+$O$4))),TREND($E10:$F10,$E$9:$F$9,AB$9))</f>
-        <v>0.95789538574372557</v>
+        <v>0.96265266034151242</v>
       </c>
       <c r="AC10">
         <f>IF($G10="s-curve",$E10+($F10-$E10)*$O$2/(1+EXP($O$3*(COUNT($I$9:AC$9)+$O$4))),TREND($E10:$F10,$E$9:$F$9,AC$9))</f>
-        <v>0.96835971578564195</v>
+        <v>0.97193465698908255</v>
       </c>
       <c r="AD10">
         <f>IF($G10="s-curve",$E10+($F10-$E10)*$O$2/(1+EXP($O$3*(COUNT($I$9:AD$9)+$O$4))),TREND($E10:$F10,$E$9:$F$9,AD$9))</f>
-        <v>0.97630797829499605</v>
+        <v>0.9789848690590679</v>
       </c>
       <c r="AE10">
         <f>IF($G10="s-curve",$E10+($F10-$E10)*$O$2/(1+EXP($O$3*(COUNT($I$9:AE$9)+$O$4))),TREND($E10:$F10,$E$9:$F$9,AE$9))</f>
-        <v>0.98230742516928027</v>
+        <v>0.98430645635145253</v>
       </c>
       <c r="AF10">
         <f>IF($G10="s-curve",$E10+($F10-$E10)*$O$2/(1+EXP($O$3*(COUNT($I$9:AF$9)+$O$4))),TREND($E10:$F10,$E$9:$F$9,AF$9))</f>
-        <v>0.98681449434688973</v>
+        <v>0.98830428524535807</v>
       </c>
       <c r="AG10">
         <f>IF($G10="s-curve",$E10+($F10-$E10)*$O$2/(1+EXP($O$3*(COUNT($I$9:AG$9)+$O$4))),TREND($E10:$F10,$E$9:$F$9,AG$9))</f>
-        <v>0.99018839091263411</v>
+        <v>0.99129697531601191</v>
       </c>
       <c r="AH10">
         <f>IF($G10="s-curve",$E10+($F10-$E10)*$O$2/(1+EXP($O$3*(COUNT($I$9:AH$9)+$O$4))),TREND($E10:$F10,$E$9:$F$9,AH$9))</f>
-        <v>0.99270729644190148</v>
+        <v>0.99353127723353074</v>
       </c>
       <c r="AI10">
         <f>IF($G10="s-curve",$E10+($F10-$E10)*$O$2/(1+EXP($O$3*(COUNT($I$9:AI$9)+$O$4))),TREND($E10:$F10,$E$9:$F$9,AI$9))</f>
-        <v>0.9945841378906537</v>
+        <v>0.99519605997313842</v>
       </c>
       <c r="AJ10">
         <f>IF($G10="s-curve",$E10+($F10-$E10)*$O$2/(1+EXP($O$3*(COUNT($I$9:AJ$9)+$O$4))),TREND($E10:$F10,$E$9:$F$9,AJ$9))</f>
-        <v>0.9959805032159601</v>
+        <v>0.99643465415129961</v>
       </c>
       <c r="AK10">
         <f>IF($G10="s-curve",$E10+($F10-$E10)*$O$2/(1+EXP($O$3*(COUNT($I$9:AK$9)+$O$4))),TREND($E10:$F10,$E$9:$F$9,AK$9))</f>
-        <v>0.99701824935068328</v>
+        <v>0.99735514845002182</v>
       </c>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.35">
@@ -63804,13 +63804,13 @@
         <v>5</v>
       </c>
       <c r="D14" s="22">
-        <v>0.16400000000000001</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="E14" s="22">
-        <v>0.10199999999999999</v>
+        <v>0.17499999999999999</v>
       </c>
       <c r="F14" s="41">
-        <v>0.15</v>
+        <v>0.2</v>
       </c>
       <c r="G14" s="7" t="str">
         <f>IF(E14=F14,"n/a",IF(OR(C14="battery electric vehicle",C14="natural gas vehicle",C14="plugin hybrid vehicle",C14="hydrogen vehicle"),"s-curve","linear"))</f>
@@ -63818,119 +63818,119 @@
       </c>
       <c r="I14" s="22">
         <f>D14</f>
-        <v>0.16400000000000001</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="J14">
         <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:J$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,J$9))</f>
-        <v>0.10547647129735284</v>
+        <v>0.17681066213403793</v>
       </c>
       <c r="K14">
         <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:K$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,K$9))</f>
-        <v>0.10657677431515725</v>
+        <v>0.17738373662247772</v>
       </c>
       <c r="L14">
         <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:L$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,L$9))</f>
-        <v>0.10797856119299598</v>
+        <v>0.17811383395468541</v>
       </c>
       <c r="M14">
         <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:M$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,M$9))</f>
-        <v>0.10973322957967609</v>
+        <v>0.17902772373941461</v>
       </c>
       <c r="N14">
         <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:N$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,N$9))</f>
-        <v>0.11188177784644547</v>
+        <v>0.18014675929502369</v>
       </c>
       <c r="O14">
         <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:O$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,O$9))</f>
-        <v>0.1144428048392566</v>
+        <v>0.18148062752044614</v>
       </c>
       <c r="P14">
         <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:P$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,P$9))</f>
-        <v>0.11739942243958112</v>
+        <v>0.18302053252061518</v>
       </c>
       <c r="Q14">
         <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:Q$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,Q$9))</f>
-        <v>0.12068931677043734</v>
+        <v>0.18473401915126944</v>
       </c>
       <c r="R14">
         <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:R$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,R$9))</f>
-        <v>0.12420336742350002</v>
+        <v>0.18656425386640627</v>
       </c>
       <c r="S14">
         <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:S$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,S$9))</f>
-        <v>0.12779663257649998</v>
+        <v>0.18843574613359373</v>
       </c>
       <c r="T14">
         <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:T$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,T$9))</f>
-        <v>0.13131068322956266</v>
+        <v>0.19026598084873056</v>
       </c>
       <c r="U14">
         <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:U$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,U$9))</f>
-        <v>0.13460057756041885</v>
+        <v>0.19197946747938482</v>
       </c>
       <c r="V14">
         <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:V$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,V$9))</f>
-        <v>0.13755719516074338</v>
+        <v>0.19351937247955386</v>
       </c>
       <c r="W14">
         <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:W$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,W$9))</f>
-        <v>0.14011822215355452</v>
+        <v>0.19485324070497631</v>
       </c>
       <c r="X14">
         <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:X$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,X$9))</f>
-        <v>0.1422667704203239</v>
+        <v>0.19597227626058539</v>
       </c>
       <c r="Y14">
         <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:Y$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,Y$9))</f>
-        <v>0.14402143880700402</v>
+        <v>0.19688616604531459</v>
       </c>
       <c r="Z14">
         <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:Z$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,Z$9))</f>
-        <v>0.14542322568484273</v>
+        <v>0.19761626337752228</v>
       </c>
       <c r="AA14">
         <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:AA$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,AA$9))</f>
-        <v>0.14652352870264715</v>
+        <v>0.19818933786596207</v>
       </c>
       <c r="AB14">
         <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:AB$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,AB$9))</f>
-        <v>0.14737529677363484</v>
+        <v>0.19863296706960148</v>
       </c>
       <c r="AC14">
         <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:AC$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,AC$9))</f>
-        <v>0.14802761864637767</v>
+        <v>0.19897271804498839</v>
       </c>
       <c r="AD14">
         <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:AD$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,AD$9))</f>
-        <v>0.1485230947508569</v>
+        <v>0.19923077851607132</v>
       </c>
       <c r="AE14">
         <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:AE$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,AE$9))</f>
-        <v>0.14889708624431877</v>
+        <v>0.19942556575224937</v>
       </c>
       <c r="AF14">
         <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:AF$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,AF$9))</f>
-        <v>0.14917804640084506</v>
+        <v>0.19957189916710683</v>
       </c>
       <c r="AG14">
         <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:AG$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,AG$9))</f>
-        <v>0.14938836722572263</v>
+        <v>0.19968144126339721</v>
       </c>
       <c r="AH14">
         <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:AH$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,AH$9))</f>
-        <v>0.14954538990806659</v>
+        <v>0.19976322391045137</v>
       </c>
       <c r="AI14">
         <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:AI$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,AI$9))</f>
-        <v>0.14966238781656022</v>
+        <v>0.19982416032112513</v>
       </c>
       <c r="AJ14">
         <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:AJ$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,AJ$9))</f>
-        <v>0.1497494339667092</v>
+        <v>0.19986949685766106</v>
       </c>
       <c r="AK14">
         <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:AK$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,AK$9))</f>
-        <v>0.14981412463484778</v>
+        <v>0.19990318991398323</v>
       </c>
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.35">
@@ -64746,7 +64746,7 @@
       </c>
       <c r="F21" s="22">
         <f>F14</f>
-        <v>0.15</v>
+        <v>0.2</v>
       </c>
       <c r="G21" s="7" t="str">
         <f>IF(E21=F21,"n/a",IF(OR(C21="battery electric vehicle",C21="natural gas vehicle",C21="plugin hybrid vehicle"),"s-curve","linear"))</f>
@@ -64758,115 +64758,115 @@
       </c>
       <c r="J21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:J$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,J$9))</f>
-        <v>2.2161047539909582E-3</v>
+        <v>2.9548063386546112E-3</v>
       </c>
       <c r="K21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:K$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,K$9))</f>
-        <v>2.9760458601116261E-3</v>
+        <v>3.9680611468155018E-3</v>
       </c>
       <c r="L21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:L$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,L$9))</f>
-        <v>3.9895490365298792E-3</v>
+        <v>5.3193987153731734E-3</v>
       </c>
       <c r="M21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:M$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,M$9))</f>
-        <v>5.3356783908954262E-3</v>
+        <v>7.1142378545272361E-3</v>
       </c>
       <c r="N21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:N$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,N$9))</f>
-        <v>7.1138809766350172E-3</v>
+        <v>9.4851746355133562E-3</v>
       </c>
       <c r="O21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:O$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,O$9))</f>
-        <v>9.4460034085494752E-3</v>
+        <v>1.2594671211399303E-2</v>
       </c>
       <c r="P21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:P$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,P$9))</f>
-        <v>1.2475904474088355E-2</v>
+        <v>1.6634539298784477E-2</v>
       </c>
       <c r="Q21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:Q$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,Q$9))</f>
-        <v>1.6364523179341936E-2</v>
+        <v>2.1819364239122584E-2</v>
       </c>
       <c r="R21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:R$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,R$9))</f>
-        <v>2.1277659735073173E-2</v>
+        <v>2.8370212980097564E-2</v>
       </c>
       <c r="S21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:S$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,S$9))</f>
-        <v>2.7363828570953451E-2</v>
+        <v>3.6485104761271273E-2</v>
       </c>
       <c r="T21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:T$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,T$9))</f>
-        <v>3.4721282475147351E-2</v>
+        <v>4.629504330019648E-2</v>
       </c>
       <c r="U21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:U$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,U$9))</f>
-        <v>4.3357574606249408E-2</v>
+        <v>5.7810099474999217E-2</v>
       </c>
       <c r="V21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:V$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,V$9))</f>
-        <v>5.3151554066130681E-2</v>
+        <v>7.0868738754840913E-2</v>
       </c>
       <c r="W21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:W$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,W$9))</f>
-        <v>6.3833622478251154E-2</v>
+        <v>8.5111496637668205E-2</v>
       </c>
       <c r="X21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:X$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,X$9))</f>
-        <v>7.4999999999999997E-2</v>
+        <v>0.1</v>
       </c>
       <c r="Y21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:Y$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,Y$9))</f>
-        <v>8.6166377521748855E-2</v>
+        <v>0.11488850336233181</v>
       </c>
       <c r="Z21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:Z$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,Z$9))</f>
-        <v>9.6848445933869307E-2</v>
+        <v>0.12913126124515908</v>
       </c>
       <c r="AA21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:AA$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,AA$9))</f>
-        <v>0.10664242539375059</v>
+        <v>0.1421899005250008</v>
       </c>
       <c r="AB21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:AB$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,AB$9))</f>
-        <v>0.11527871752485264</v>
+        <v>0.15370495669980352</v>
       </c>
       <c r="AC21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:AC$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,AC$9))</f>
-        <v>0.12263617142904654</v>
+        <v>0.16351489523872872</v>
       </c>
       <c r="AD21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:AD$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,AD$9))</f>
-        <v>0.12872234026492685</v>
+        <v>0.17162978701990247</v>
       </c>
       <c r="AE21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:AE$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,AE$9))</f>
-        <v>0.13363547682065807</v>
+        <v>0.17818063576087742</v>
       </c>
       <c r="AF21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:AF$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,AF$9))</f>
-        <v>0.13752409552591163</v>
+        <v>0.18336546070121554</v>
       </c>
       <c r="AG21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:AG$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,AG$9))</f>
-        <v>0.14055399659145051</v>
+        <v>0.18740532878860072</v>
       </c>
       <c r="AH21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:AH$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,AH$9))</f>
-        <v>0.14288611902336498</v>
+        <v>0.19051482536448666</v>
       </c>
       <c r="AI21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:AI$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,AI$9))</f>
-        <v>0.14466432160910458</v>
+        <v>0.19288576214547279</v>
       </c>
       <c r="AJ21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:AJ$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,AJ$9))</f>
-        <v>0.1460104509634701</v>
+        <v>0.19468060128462683</v>
       </c>
       <c r="AK21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:AK$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,AK$9))</f>
-        <v>0.14702395413988836</v>
+        <v>0.19603193885318451</v>
       </c>
     </row>
     <row r="22" spans="1:37" x14ac:dyDescent="0.35">

</xml_diff>